<commit_message>
Rw Updates _ ShieldW Enabled
Boat Enabled - Wion
BirdW - [8] , FuelW - [10] , InCapacity = [2] , On Host - [1]

NodeW - [-3]
</commit_message>
<xml_diff>
--- a/System_2.1.9.xlsx
+++ b/System_2.1.9.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Work_For_\Work\Running AppS\System_Work_RW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F140FB7-BFF4-457B-BF99-59E2579F02CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53B6AA50-57FA-401D-B684-F57F7FA7D91D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1117" uniqueCount="625">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1115" uniqueCount="626">
   <si>
     <t>Zone</t>
   </si>
@@ -1910,10 +1910,13 @@
     <t>ndtv 24*7</t>
   </si>
   <si>
-    <t>6F Reserved</t>
-  </si>
-  <si>
-    <t>Wbt_X_7F</t>
+    <t>Wbt_X_8F</t>
+  </si>
+  <si>
+    <t>3F Reserved</t>
+  </si>
+  <si>
+    <t>France24 ES</t>
   </si>
 </sst>
 </file>
@@ -5883,8 +5886,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:X28"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView topLeftCell="B9" workbookViewId="0">
+      <selection activeCell="X18" sqref="X18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6614,7 +6617,7 @@
       <c r="P22" s="313"/>
       <c r="T22" s="609"/>
       <c r="X22" s="19" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
     </row>
     <row r="23" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6646,7 +6649,7 @@
       <c r="P23" s="313"/>
       <c r="T23" s="609"/>
       <c r="U23" s="2" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="V23" s="100" t="s">
         <v>44</v>
@@ -8971,8 +8974,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB54FD83-008D-4F8B-87AC-83E7F70047CB}">
   <dimension ref="A1:AL31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N8" workbookViewId="0">
-      <selection activeCell="AA17" sqref="AA17"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="AO7" sqref="AO7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9142,7 +9145,7 @@
       </c>
       <c r="S2" s="21">
         <f>S7+S20</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T2" s="172">
         <f>SUM(T4:T16)</f>
@@ -9193,7 +9196,7 @@
       </c>
       <c r="Q3" s="471">
         <f>SUM(X23:X31)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="U3" s="6"/>
       <c r="V3" s="470"/>
@@ -9367,7 +9370,7 @@
       </c>
       <c r="AF6" s="64">
         <f>AF7-SUM(AI2:AI10)+AF11</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AH6" s="6"/>
       <c r="AI6" s="525"/>
@@ -9435,7 +9438,7 @@
       </c>
       <c r="AF7" s="295">
         <f>8-AF11</f>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="AH7" s="6"/>
       <c r="AI7" s="469"/>
@@ -9507,12 +9510,8 @@
       <c r="AC9" s="515"/>
       <c r="AE9" s="20"/>
       <c r="AF9" s="20"/>
-      <c r="AH9" s="6" t="s">
-        <v>233</v>
-      </c>
-      <c r="AI9" s="470">
-        <v>1</v>
-      </c>
+      <c r="AH9" s="6"/>
+      <c r="AI9" s="470"/>
       <c r="AJ9" s="553"/>
       <c r="AK9" s="6" t="s">
         <v>598</v>
@@ -9625,7 +9624,7 @@
         <v>0</v>
       </c>
       <c r="AF11" s="24">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AG11" s="414"/>
       <c r="AH11" s="713" t="s">
@@ -9733,7 +9732,7 @@
       <c r="X14"/>
       <c r="Z14" s="68">
         <f>SUM(X23:X31)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -9828,11 +9827,9 @@
         <v>424</v>
       </c>
       <c r="U17" s="19" t="s">
-        <v>471</v>
-      </c>
-      <c r="V17" s="24">
-        <v>1</v>
-      </c>
+        <v>625</v>
+      </c>
+      <c r="V17" s="24"/>
       <c r="W17" s="6"/>
       <c r="X17" s="24"/>
     </row>
@@ -9854,14 +9851,10 @@
       </c>
       <c r="S18" s="24">
         <f>5-S26</f>
-        <v>5</v>
-      </c>
-      <c r="U18" s="19" t="s">
-        <v>472</v>
-      </c>
-      <c r="V18" s="24">
-        <v>1</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="U18" s="19"/>
+      <c r="V18" s="24"/>
       <c r="W18" s="19"/>
       <c r="X18" s="24"/>
     </row>
@@ -9874,7 +9867,7 @@
         <v>233</v>
       </c>
       <c r="V19" s="24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="W19" s="19" t="s">
         <v>345</v>
@@ -9921,7 +9914,7 @@
       </c>
       <c r="S20" s="24">
         <f>S18-SUM(V16:V21)+S26</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U20" s="220" t="s">
         <v>83</v>
@@ -9985,7 +9978,7 @@
       <c r="I23" s="708"/>
       <c r="Q23" s="24">
         <f>SUM(V23:V31)</f>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="U23" s="342"/>
       <c r="V23" s="183">
@@ -10002,13 +9995,13 @@
       <c r="I24" s="708"/>
       <c r="U24" s="35"/>
       <c r="V24" s="509">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="W24" s="54" t="s">
         <v>73</v>
       </c>
       <c r="X24" s="24">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -10090,7 +10083,7 @@
         <v>2</v>
       </c>
       <c r="S26" s="24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T26" s="61" t="s">
         <v>557</v>
@@ -10171,13 +10164,13 @@
         <v>558</v>
       </c>
       <c r="V29" s="509">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W29" s="54" t="s">
         <v>498</v>
       </c>
       <c r="X29" s="472">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -10242,8 +10235,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2029A93E-B53C-4201-9F17-439C144F3CF1}">
   <dimension ref="A1:AT37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10399,7 +10392,7 @@
       </c>
       <c r="J2" s="318">
         <f>K2+L2</f>
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="K2" s="723">
         <f>SUM(K4:K37)</f>
@@ -10407,7 +10400,7 @@
       </c>
       <c r="L2" s="721">
         <f>SUM(L4:L37)</f>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="M2" s="736">
         <f>SUM(M5:M30)</f>
@@ -10419,7 +10412,7 @@
       </c>
       <c r="O2" s="740">
         <f>SUM(O4:O29)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="P2" s="668">
         <f>SUM(N30:N37)* (-1)</f>
@@ -10548,15 +10541,15 @@
       </c>
       <c r="AA3" s="66">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="AB3" s="66">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="AC3" s="66">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="AD3" s="66">
         <f t="shared" ref="AD3:AO3" si="1">SUM(AD4:AD29)</f>
@@ -10564,7 +10557,7 @@
       </c>
       <c r="AE3" s="66">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="AF3" s="66">
         <f t="shared" si="1"/>
@@ -10576,7 +10569,7 @@
       </c>
       <c r="AH3" s="66">
         <f>SUM(AH4:AH29)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="AI3" s="374">
         <f t="shared" si="1"/>
@@ -10588,23 +10581,23 @@
       </c>
       <c r="AK3" s="404">
         <f>SUM(AK4:AK37)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL3" s="404">
         <f>SUM(AL4:AL37)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AM3" s="100">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="AN3" s="310">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="AO3" s="311">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="AR3" s="142"/>
     </row>
@@ -11230,7 +11223,7 @@
       </c>
       <c r="K10" s="575"/>
       <c r="L10" s="581">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M10" s="328"/>
       <c r="N10" s="107">
@@ -11238,7 +11231,7 @@
       </c>
       <c r="O10" s="293">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P10" s="719"/>
       <c r="Q10" s="20"/>
@@ -11268,27 +11261,27 @@
       <c r="Z10" s="296"/>
       <c r="AA10" s="117">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB10" s="290">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC10" s="290">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD10" s="290">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AE10" s="294">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF10" s="300"/>
       <c r="AG10" s="296"/>
       <c r="AH10" s="296">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI10" s="375"/>
       <c r="AJ10" s="509"/>
@@ -11296,15 +11289,15 @@
       <c r="AL10" s="317"/>
       <c r="AM10" s="336">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN10" s="308">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO10" s="309">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AP10" s="6" t="s">
         <v>73</v>
@@ -11605,7 +11598,7 @@
       <c r="J14" s="571"/>
       <c r="K14" s="575"/>
       <c r="L14" s="581">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M14" s="328"/>
       <c r="N14" s="291">
@@ -11667,10 +11660,10 @@
       <c r="AJ14" s="509">
         <v>1</v>
       </c>
-      <c r="AK14" s="559"/>
-      <c r="AL14" s="317">
-        <v>1</v>
-      </c>
+      <c r="AK14" s="559">
+        <v>1</v>
+      </c>
+      <c r="AL14" s="317"/>
       <c r="AM14" s="336">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -11684,13 +11677,13 @@
         <v>0</v>
       </c>
       <c r="AP14" s="6" t="s">
-        <v>560</v>
+        <v>625</v>
       </c>
       <c r="AQ14" s="564" t="s">
         <v>563</v>
       </c>
       <c r="AR14" s="508" t="s">
-        <v>471</v>
+        <v>498</v>
       </c>
     </row>
     <row r="15" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -13357,9 +13350,7 @@
     </row>
     <row r="33" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="80"/>
-      <c r="B33" s="24">
-        <v>1</v>
-      </c>
+      <c r="B33" s="24"/>
       <c r="G33" s="382">
         <v>-1</v>
       </c>
@@ -13737,7 +13728,7 @@
     </row>
     <row r="37" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B37" s="24">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D37" s="382">
         <v>1</v>

</xml_diff>

<commit_message>
Boat Enabled - Zee N
Boat Enabled - Zee N

Failover Corrected , Require Action for Deployment
</commit_message>
<xml_diff>
--- a/System_2.1.9.xlsx
+++ b/System_2.1.9.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Work_For_\Work\Running AppS\System_Work_RW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53B6AA50-57FA-401D-B684-F57F7FA7D91D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5607769B-F2FB-4BFD-9F63-15CBCCA3A4D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BoardRW" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1115" uniqueCount="626">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1112" uniqueCount="625">
   <si>
     <t>Zone</t>
   </si>
@@ -1911,9 +1911,6 @@
   </si>
   <si>
     <t>Wbt_X_8F</t>
-  </si>
-  <si>
-    <t>3F Reserved</t>
   </si>
   <si>
     <t>France24 ES</t>
@@ -5887,7 +5884,7 @@
   <dimension ref="B1:X28"/>
   <sheetViews>
     <sheetView topLeftCell="B9" workbookViewId="0">
-      <selection activeCell="X18" sqref="X18"/>
+      <selection activeCell="X20" sqref="X20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6072,7 +6069,7 @@
         <v>226</v>
       </c>
       <c r="V5" s="24">
-        <v>6900</v>
+        <v>7020</v>
       </c>
     </row>
     <row r="6" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6289,7 +6286,7 @@
         <v>225</v>
       </c>
       <c r="V11" s="64">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="12" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6616,9 +6613,7 @@
       </c>
       <c r="P22" s="313"/>
       <c r="T22" s="609"/>
-      <c r="X22" s="19" t="s">
-        <v>624</v>
-      </c>
+      <c r="X22" s="19"/>
     </row>
     <row r="23" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="2" t="s">
@@ -7541,7 +7536,7 @@
       <c r="D10" s="142"/>
       <c r="E10" s="237">
         <f>Boat!W8</f>
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F10" s="643"/>
       <c r="N10" s="418" t="s">
@@ -8974,8 +8969,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB54FD83-008D-4F8B-87AC-83E7F70047CB}">
   <dimension ref="A1:AL31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="AO7" sqref="AO7"/>
+    <sheetView topLeftCell="N12" workbookViewId="0">
+      <selection activeCell="AC26" sqref="AC26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9141,11 +9136,11 @@
       <c r="Q2" s="717"/>
       <c r="R2" s="21">
         <f>R7+R20</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="S2" s="21">
         <f>S7+S20</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T2" s="172">
         <f>SUM(T4:T16)</f>
@@ -9196,7 +9191,7 @@
       </c>
       <c r="Q3" s="471">
         <f>SUM(X23:X31)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="U3" s="6"/>
       <c r="V3" s="470"/>
@@ -9212,12 +9207,8 @@
         <f>IF((AE7-SUM(AL2:AL10)&lt;0),AE7-SUM(AI2:AI10),0)</f>
         <v>0</v>
       </c>
-      <c r="AH3" s="6" t="s">
-        <v>250</v>
-      </c>
-      <c r="AI3" s="470">
-        <v>1</v>
-      </c>
+      <c r="AH3" s="6"/>
+      <c r="AI3" s="470"/>
       <c r="AJ3" s="553"/>
       <c r="AK3" s="6" t="s">
         <v>250</v>
@@ -9360,7 +9351,7 @@
       </c>
       <c r="S6" s="64">
         <f>S7+S11-SUM(V2:V10)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AB6" s="711"/>
       <c r="AC6" s="35"/>
@@ -9370,7 +9361,7 @@
       </c>
       <c r="AF6" s="64">
         <f>AF7-SUM(AI2:AI10)+AF11</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AH6" s="6"/>
       <c r="AI6" s="525"/>
@@ -9407,20 +9398,16 @@
       </c>
       <c r="R7" s="24">
         <f>3-R11</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S7" s="24">
         <f>3-S11</f>
-        <v>1</v>
-      </c>
-      <c r="U7" s="6" t="s">
-        <v>345</v>
-      </c>
-      <c r="V7" s="469">
-        <v>1</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="U7" s="6"/>
+      <c r="V7" s="469"/>
       <c r="W7" s="6" t="s">
-        <v>345</v>
+        <v>250</v>
       </c>
       <c r="X7" s="469">
         <v>1</v>
@@ -9438,7 +9425,7 @@
       </c>
       <c r="AF7" s="295">
         <f>8-AF11</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AH7" s="6"/>
       <c r="AI7" s="469"/>
@@ -9531,7 +9518,7 @@
       <c r="D10" s="108"/>
       <c r="E10" s="68">
         <f>Boat!W8</f>
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G10" s="601"/>
       <c r="I10" s="708"/>
@@ -9602,10 +9589,10 @@
         <v>44</v>
       </c>
       <c r="R11" s="24">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="S11" s="24">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="U11" s="713" t="s">
         <v>559</v>
@@ -9624,7 +9611,7 @@
         <v>0</v>
       </c>
       <c r="AF11" s="24">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AG11" s="414"/>
       <c r="AH11" s="713" t="s">
@@ -9732,7 +9719,7 @@
       <c r="X14"/>
       <c r="Z14" s="68">
         <f>SUM(X23:X31)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -9827,7 +9814,7 @@
         <v>424</v>
       </c>
       <c r="U17" s="19" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="V17" s="24"/>
       <c r="W17" s="6"/>
@@ -9873,7 +9860,7 @@
         <v>345</v>
       </c>
       <c r="X19" s="24">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -9910,7 +9897,7 @@
       </c>
       <c r="R20" s="24">
         <f>R18-SUM(X16:X21)+R26</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="S20" s="24">
         <f>S18-SUM(V16:V21)+S26</f>
@@ -9978,17 +9965,17 @@
       <c r="I23" s="708"/>
       <c r="Q23" s="24">
         <f>SUM(V23:V31)</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="U23" s="342"/>
       <c r="V23" s="183">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W23" s="54" t="s">
         <v>495</v>
       </c>
       <c r="X23" s="24">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -10235,8 +10222,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2029A93E-B53C-4201-9F17-439C144F3CF1}">
   <dimension ref="A1:AT37"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
+      <selection activeCell="V33" sqref="V33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10392,7 +10379,7 @@
       </c>
       <c r="J2" s="318">
         <f>K2+L2</f>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="K2" s="723">
         <f>SUM(K4:K37)</f>
@@ -10400,7 +10387,7 @@
       </c>
       <c r="L2" s="721">
         <f>SUM(L4:L37)</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M2" s="736">
         <f>SUM(M5:M30)</f>
@@ -10408,7 +10395,7 @@
       </c>
       <c r="N2" s="738">
         <f>SUM(N4:N29)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O2" s="740">
         <f>SUM(O4:O29)</f>
@@ -10524,7 +10511,7 @@
       </c>
       <c r="V3" s="484">
         <f>SUM(V4:V29)</f>
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="W3" s="743"/>
       <c r="X3" s="485">
@@ -10533,7 +10520,7 @@
       </c>
       <c r="Y3" s="485">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z3" s="59">
         <f t="shared" si="0"/>
@@ -10545,7 +10532,7 @@
       </c>
       <c r="AB3" s="66">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="AC3" s="66">
         <f t="shared" si="0"/>
@@ -10577,11 +10564,11 @@
       </c>
       <c r="AJ3" s="404">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AK3" s="404">
         <f>SUM(AK4:AK37)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AL3" s="404">
         <f>SUM(AL4:AL37)</f>
@@ -11058,7 +11045,7 @@
       </c>
       <c r="W8" s="24">
         <f>V3</f>
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="X8" s="497">
         <v>0</v>
@@ -11285,7 +11272,9 @@
       </c>
       <c r="AI10" s="375"/>
       <c r="AJ10" s="509"/>
-      <c r="AK10" s="559"/>
+      <c r="AK10" s="559">
+        <v>1</v>
+      </c>
       <c r="AL10" s="317"/>
       <c r="AM10" s="336">
         <f t="shared" si="6"/>
@@ -11677,7 +11666,7 @@
         <v>0</v>
       </c>
       <c r="AP14" s="6" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="AQ14" s="564" t="s">
         <v>563</v>
@@ -12587,13 +12576,13 @@
         <v>1</v>
       </c>
       <c r="L24" s="581">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M24" s="326">
         <v>0</v>
       </c>
       <c r="N24" s="107">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O24" s="293">
         <f t="shared" si="10"/>
@@ -12613,7 +12602,7 @@
         <v>2</v>
       </c>
       <c r="V24" s="492">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="W24" s="526">
         <v>-2</v>
@@ -12621,7 +12610,7 @@
       <c r="X24" s="26"/>
       <c r="Y24" s="548">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z24" s="296"/>
       <c r="AA24" s="117">
@@ -12630,7 +12619,7 @@
       </c>
       <c r="AB24" s="290">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AC24" s="290">
         <v>1</v>
@@ -12653,9 +12642,7 @@
         <v>1</v>
       </c>
       <c r="AI24" s="375"/>
-      <c r="AJ24" s="509">
-        <v>1</v>
-      </c>
+      <c r="AJ24" s="509"/>
       <c r="AK24" s="559"/>
       <c r="AL24" s="317"/>
       <c r="AM24" s="336">
@@ -13419,9 +13406,7 @@
         <v>1</v>
       </c>
       <c r="AI33" s="375"/>
-      <c r="AJ33" s="155">
-        <v>2</v>
-      </c>
+      <c r="AJ33" s="155"/>
       <c r="AK33" s="155">
         <v>0</v>
       </c>
@@ -13728,7 +13713,7 @@
     </row>
     <row r="37" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B37" s="24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D37" s="382">
         <v>1</v>

</xml_diff>

<commit_message>
Boat Enabled - Polimer , RBharat
Boat Enabled - Polimer , RBharat

BirdW - [6] , FuelW - [11] , InCapacity = [10] , On Host - [4 +1]

NodeW - [-3]
</commit_message>
<xml_diff>
--- a/System_2.1.9.xlsx
+++ b/System_2.1.9.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Work_For_\Work\Running AppS\System_Work_RW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34E80814-C835-44E9-92D9-BE3A93A388B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65BCC380-909B-4483-B401-3E83965E8B46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BoardRW" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1103" uniqueCount="624">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1104" uniqueCount="624">
   <si>
     <t>Zone</t>
   </si>
@@ -1904,13 +1904,13 @@
     <t>Nippon TV</t>
   </si>
   <si>
-    <t>7F</t>
-  </si>
-  <si>
-    <t>5F INCapacity</t>
-  </si>
-  <si>
     <t>Wbt_X_6F</t>
+  </si>
+  <si>
+    <t>Rbangla</t>
+  </si>
+  <si>
+    <t>10 F INCapacity</t>
   </si>
 </sst>
 </file>
@@ -5033,6 +5033,159 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="49" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="49" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="49" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -5051,12 +5204,6 @@
     <xf numFmtId="0" fontId="18" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="13" fillId="27" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -5111,169 +5258,61 @@
     <xf numFmtId="0" fontId="3" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="49" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="49" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="49" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="32" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5315,43 +5354,70 @@
     <xf numFmtId="0" fontId="3" fillId="36" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    <xf numFmtId="0" fontId="3" fillId="43" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="43" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="43" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="40" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="40" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="40" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="52" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="52" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="14" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="14" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="35" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5375,112 +5441,25 @@
     <xf numFmtId="0" fontId="29" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="43" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="43" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="43" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="40" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="40" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="40" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="32" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="32" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="52" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="52" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="14" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="14" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5558,25 +5537,46 @@
     <xf numFmtId="0" fontId="3" fillId="21" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -5874,8 +5874,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:X28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="X15" sqref="X15"/>
+    <sheetView topLeftCell="C9" workbookViewId="0">
+      <selection activeCell="Y19" sqref="Y19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6599,7 +6599,7 @@
       <c r="P22" s="313"/>
       <c r="T22" s="607"/>
       <c r="X22" s="19" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
     </row>
     <row r="23" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6631,7 +6631,7 @@
       <c r="P23" s="313"/>
       <c r="T23" s="607"/>
       <c r="U23" s="2" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="V23" s="100" t="s">
         <v>44</v>
@@ -6745,9 +6745,7 @@
       </c>
       <c r="P26" s="313"/>
       <c r="T26" s="607"/>
-      <c r="V26" s="24" t="s">
-        <v>621</v>
-      </c>
+      <c r="V26" s="24"/>
     </row>
     <row r="27" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="256" t="s">
@@ -6911,7 +6909,7 @@
       <c r="H1" s="97" t="s">
         <v>344</v>
       </c>
-      <c r="I1" s="659" t="s">
+      <c r="I1" s="613" t="s">
         <v>370</v>
       </c>
       <c r="J1" s="2" t="s">
@@ -6947,7 +6945,7 @@
       <c r="X1" s="430" t="s">
         <v>155</v>
       </c>
-      <c r="Y1" s="653" t="s">
+      <c r="Y1" s="657" t="s">
         <v>530</v>
       </c>
       <c r="Z1" s="406">
@@ -6972,7 +6970,7 @@
         <v>499</v>
       </c>
       <c r="AM1" s="402"/>
-      <c r="AN1" s="635"/>
+      <c r="AN1" s="640"/>
       <c r="AO1" s="338" t="s">
         <v>470</v>
       </c>
@@ -6981,23 +6979,23 @@
       </c>
     </row>
     <row r="2" spans="1:43" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="617">
+      <c r="A2" s="666">
         <f ca="1">TODAY()</f>
         <v>45285</v>
       </c>
-      <c r="B2" s="619" t="s">
+      <c r="B2" s="668" t="s">
         <v>371</v>
       </c>
-      <c r="C2" s="615" t="s">
+      <c r="C2" s="645" t="s">
         <v>358</v>
       </c>
-      <c r="D2" s="621" t="s">
+      <c r="D2" s="670" t="s">
         <v>356</v>
       </c>
-      <c r="E2" s="669" t="s">
+      <c r="E2" s="609" t="s">
         <v>64</v>
       </c>
-      <c r="F2" s="640" t="s">
+      <c r="F2" s="619" t="s">
         <v>102</v>
       </c>
       <c r="G2" s="393" t="s">
@@ -7006,31 +7004,31 @@
       <c r="H2" s="80" t="s">
         <v>33</v>
       </c>
-      <c r="I2" s="660"/>
+      <c r="I2" s="614"/>
       <c r="J2" s="81" t="s">
         <v>76</v>
       </c>
-      <c r="K2" s="671" t="s">
+      <c r="K2" s="611" t="s">
         <v>343</v>
       </c>
-      <c r="L2" s="672"/>
-      <c r="M2" s="640" t="s">
+      <c r="L2" s="612"/>
+      <c r="M2" s="619" t="s">
         <v>102</v>
       </c>
       <c r="N2" s="69" t="s">
         <v>28</v>
       </c>
-      <c r="O2" s="644" t="s">
+      <c r="O2" s="649" t="s">
         <v>102</v>
       </c>
       <c r="P2" s="85" t="s">
         <v>147</v>
       </c>
-      <c r="Q2" s="615" t="s">
+      <c r="Q2" s="645" t="s">
         <v>143</v>
       </c>
       <c r="R2" s="598"/>
-      <c r="S2" s="657" t="s">
+      <c r="S2" s="634" t="s">
         <v>148</v>
       </c>
       <c r="T2" s="89"/>
@@ -7040,7 +7038,7 @@
       <c r="X2" s="431" t="s">
         <v>156</v>
       </c>
-      <c r="Y2" s="654"/>
+      <c r="Y2" s="658"/>
       <c r="Z2" s="407">
         <v>1</v>
       </c>
@@ -7063,15 +7061,15 @@
         <v>464</v>
       </c>
       <c r="AM2" s="428"/>
-      <c r="AN2" s="636"/>
+      <c r="AN2" s="641"/>
     </row>
     <row r="3" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="618"/>
-      <c r="B3" s="620"/>
-      <c r="C3" s="616"/>
-      <c r="D3" s="622"/>
-      <c r="E3" s="670"/>
-      <c r="F3" s="641"/>
+      <c r="A3" s="667"/>
+      <c r="B3" s="669"/>
+      <c r="C3" s="646"/>
+      <c r="D3" s="671"/>
+      <c r="E3" s="610"/>
+      <c r="F3" s="620"/>
       <c r="G3" s="394" t="s">
         <v>28</v>
       </c>
@@ -7090,17 +7088,17 @@
       <c r="L3" s="201" t="s">
         <v>107</v>
       </c>
-      <c r="M3" s="641"/>
+      <c r="M3" s="620"/>
       <c r="N3" s="69" t="s">
         <v>146</v>
       </c>
-      <c r="O3" s="645"/>
+      <c r="O3" s="650"/>
       <c r="P3" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="Q3" s="616"/>
+      <c r="Q3" s="646"/>
       <c r="R3" s="600"/>
-      <c r="S3" s="658"/>
+      <c r="S3" s="636"/>
       <c r="T3" s="89"/>
       <c r="U3" s="124"/>
       <c r="V3" s="120"/>
@@ -7108,7 +7106,7 @@
       <c r="X3" s="431" t="s">
         <v>157</v>
       </c>
-      <c r="Y3" s="654"/>
+      <c r="Y3" s="658"/>
       <c r="Z3" s="408">
         <v>1</v>
       </c>
@@ -7117,7 +7115,7 @@
       <c r="AC3" s="100" t="s">
         <v>481</v>
       </c>
-      <c r="AD3" s="656" t="s">
+      <c r="AD3" s="631" t="s">
         <v>456</v>
       </c>
       <c r="AE3" s="257"/>
@@ -7129,16 +7127,16 @@
       <c r="AK3" s="257"/>
       <c r="AL3" s="16"/>
       <c r="AM3" s="428"/>
-      <c r="AN3" s="636"/>
+      <c r="AN3" s="641"/>
     </row>
     <row r="4" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="238" t="s">
         <v>183</v>
       </c>
-      <c r="B4" s="633" t="s">
+      <c r="B4" s="682" t="s">
         <v>374</v>
       </c>
-      <c r="C4" s="615" t="s">
+      <c r="C4" s="645" t="s">
         <v>154</v>
       </c>
       <c r="D4" s="347" t="s">
@@ -7147,7 +7145,7 @@
       <c r="E4" s="378">
         <v>2</v>
       </c>
-      <c r="F4" s="641"/>
+      <c r="F4" s="620"/>
       <c r="G4" s="381" t="s">
         <v>202</v>
       </c>
@@ -7164,11 +7162,11 @@
         <v>150</v>
       </c>
       <c r="L4" s="204"/>
-      <c r="M4" s="641"/>
+      <c r="M4" s="620"/>
       <c r="N4" s="174" t="s">
         <v>69</v>
       </c>
-      <c r="O4" s="645"/>
+      <c r="O4" s="650"/>
       <c r="P4" s="2" t="s">
         <v>191</v>
       </c>
@@ -7190,12 +7188,12 @@
       <c r="X4" s="431" t="s">
         <v>158</v>
       </c>
-      <c r="Y4" s="654"/>
+      <c r="Y4" s="658"/>
       <c r="Z4" s="409"/>
       <c r="AA4" s="307"/>
       <c r="AB4" s="209"/>
       <c r="AC4" s="16"/>
-      <c r="AD4" s="656"/>
+      <c r="AD4" s="631"/>
       <c r="AE4" s="257"/>
       <c r="AF4" s="257"/>
       <c r="AG4" s="16"/>
@@ -7205,37 +7203,37 @@
       <c r="AK4" s="257"/>
       <c r="AL4" s="16"/>
       <c r="AM4" s="428"/>
-      <c r="AN4" s="636"/>
+      <c r="AN4" s="641"/>
       <c r="AO4" s="338" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="659" t="s">
+      <c r="A5" s="613" t="s">
         <v>419</v>
       </c>
-      <c r="B5" s="634"/>
-      <c r="C5" s="616"/>
+      <c r="B5" s="683"/>
+      <c r="C5" s="646"/>
       <c r="D5" s="61" t="s">
         <v>153</v>
       </c>
       <c r="E5" s="379">
         <v>1</v>
       </c>
-      <c r="F5" s="641"/>
-      <c r="G5" s="625" t="s">
+      <c r="F5" s="620"/>
+      <c r="G5" s="674" t="s">
         <v>192</v>
       </c>
-      <c r="H5" s="625"/>
-      <c r="I5" s="625"/>
-      <c r="J5" s="625"/>
-      <c r="K5" s="625"/>
-      <c r="L5" s="626"/>
-      <c r="M5" s="641"/>
+      <c r="H5" s="674"/>
+      <c r="I5" s="674"/>
+      <c r="J5" s="674"/>
+      <c r="K5" s="674"/>
+      <c r="L5" s="675"/>
+      <c r="M5" s="620"/>
       <c r="N5" s="21">
         <v>8</v>
       </c>
-      <c r="O5" s="645"/>
+      <c r="O5" s="650"/>
       <c r="T5" s="89"/>
       <c r="U5" s="124"/>
       <c r="V5" s="120"/>
@@ -7243,7 +7241,7 @@
       <c r="X5" s="431" t="s">
         <v>159</v>
       </c>
-      <c r="Y5" s="654"/>
+      <c r="Y5" s="658"/>
       <c r="Z5" s="409">
         <v>1</v>
       </c>
@@ -7266,24 +7264,24 @@
       <c r="AK5" s="257"/>
       <c r="AL5" s="80"/>
       <c r="AM5" s="428"/>
-      <c r="AN5" s="636"/>
+      <c r="AN5" s="641"/>
     </row>
     <row r="6" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="660"/>
-      <c r="B6" s="631" t="s">
+      <c r="A6" s="614"/>
+      <c r="B6" s="680" t="s">
         <v>177</v>
       </c>
-      <c r="C6" s="661"/>
-      <c r="D6" s="662"/>
-      <c r="F6" s="641"/>
-      <c r="G6" s="627"/>
-      <c r="H6" s="627"/>
-      <c r="I6" s="627"/>
-      <c r="J6" s="627"/>
-      <c r="K6" s="627"/>
-      <c r="L6" s="628"/>
-      <c r="M6" s="641"/>
-      <c r="O6" s="645"/>
+      <c r="C6" s="628"/>
+      <c r="D6" s="629"/>
+      <c r="F6" s="620"/>
+      <c r="G6" s="676"/>
+      <c r="H6" s="676"/>
+      <c r="I6" s="676"/>
+      <c r="J6" s="676"/>
+      <c r="K6" s="676"/>
+      <c r="L6" s="677"/>
+      <c r="M6" s="620"/>
+      <c r="O6" s="650"/>
       <c r="T6" s="89"/>
       <c r="U6" s="124"/>
       <c r="V6" s="98" t="s">
@@ -7293,7 +7291,7 @@
       <c r="X6" s="431" t="s">
         <v>160</v>
       </c>
-      <c r="Y6" s="654"/>
+      <c r="Y6" s="658"/>
       <c r="Z6" s="407">
         <v>1</v>
       </c>
@@ -7307,16 +7305,16 @@
       <c r="AF6" s="257"/>
       <c r="AG6" s="257"/>
       <c r="AH6" s="257"/>
-      <c r="AI6" s="650"/>
+      <c r="AI6" s="630"/>
       <c r="AJ6" s="441" t="s">
         <v>459</v>
       </c>
-      <c r="AK6" s="650" t="s">
+      <c r="AK6" s="630" t="s">
         <v>252</v>
       </c>
       <c r="AL6" s="257"/>
       <c r="AM6" s="428"/>
-      <c r="AN6" s="636"/>
+      <c r="AN6" s="641"/>
       <c r="AO6" s="338" t="s">
         <v>471</v>
       </c>
@@ -7325,7 +7323,7 @@
       <c r="A7" s="232" t="s">
         <v>573</v>
       </c>
-      <c r="B7" s="632"/>
+      <c r="B7" s="681"/>
       <c r="C7" s="202" t="s">
         <v>375</v>
       </c>
@@ -7335,7 +7333,7 @@
       <c r="E7" s="265">
         <v>3</v>
       </c>
-      <c r="F7" s="641"/>
+      <c r="F7" s="620"/>
       <c r="G7" s="395">
         <v>0</v>
       </c>
@@ -7354,8 +7352,8 @@
       <c r="L7" s="212">
         <v>0</v>
       </c>
-      <c r="M7" s="641"/>
-      <c r="O7" s="645"/>
+      <c r="M7" s="620"/>
+      <c r="O7" s="650"/>
       <c r="R7" s="99" t="s">
         <v>44</v>
       </c>
@@ -7369,7 +7367,7 @@
       <c r="X7" s="431" t="s">
         <v>161</v>
       </c>
-      <c r="Y7" s="654"/>
+      <c r="Y7" s="658"/>
       <c r="Z7" s="407">
         <v>1</v>
       </c>
@@ -7379,18 +7377,18 @@
       <c r="AD7" s="16"/>
       <c r="AE7" s="257"/>
       <c r="AF7" s="257"/>
-      <c r="AG7" s="656" t="s">
+      <c r="AG7" s="631" t="s">
         <v>455</v>
       </c>
       <c r="AH7" s="257"/>
-      <c r="AI7" s="650"/>
+      <c r="AI7" s="630"/>
       <c r="AJ7" s="257"/>
-      <c r="AK7" s="650"/>
+      <c r="AK7" s="630"/>
       <c r="AL7" s="80" t="s">
         <v>497</v>
       </c>
       <c r="AM7" s="428"/>
-      <c r="AN7" s="636"/>
+      <c r="AN7" s="641"/>
       <c r="AP7" s="76" t="s">
         <v>472</v>
       </c>
@@ -7407,27 +7405,27 @@
         <f>SUM(G7:N9)</f>
         <v>15</v>
       </c>
-      <c r="F8" s="641"/>
-      <c r="G8" s="626">
-        <v>0</v>
-      </c>
-      <c r="H8" s="623" t="s">
+      <c r="F8" s="620"/>
+      <c r="G8" s="675">
+        <v>0</v>
+      </c>
+      <c r="H8" s="672" t="s">
         <v>104</v>
       </c>
       <c r="I8" s="598">
         <v>0</v>
       </c>
-      <c r="J8" s="623" t="s">
+      <c r="J8" s="672" t="s">
         <v>104</v>
       </c>
-      <c r="K8" s="629"/>
-      <c r="L8" s="663"/>
-      <c r="M8" s="642"/>
-      <c r="N8" s="666">
+      <c r="K8" s="678"/>
+      <c r="L8" s="632"/>
+      <c r="M8" s="647"/>
+      <c r="N8" s="637">
         <f>N5+N11</f>
         <v>15</v>
       </c>
-      <c r="O8" s="645"/>
+      <c r="O8" s="650"/>
       <c r="T8" s="103" t="s">
         <v>44</v>
       </c>
@@ -7437,7 +7435,7 @@
       <c r="X8" s="431" t="s">
         <v>162</v>
       </c>
-      <c r="Y8" s="654"/>
+      <c r="Y8" s="658"/>
       <c r="Z8" s="409"/>
       <c r="AA8" s="307"/>
       <c r="AB8" s="209"/>
@@ -7445,14 +7443,14 @@
       <c r="AD8" s="16"/>
       <c r="AE8" s="257"/>
       <c r="AF8" s="257"/>
-      <c r="AG8" s="656"/>
+      <c r="AG8" s="631"/>
       <c r="AH8" s="257"/>
-      <c r="AI8" s="650"/>
+      <c r="AI8" s="630"/>
       <c r="AJ8" s="257"/>
       <c r="AK8" s="257"/>
       <c r="AL8" s="257"/>
       <c r="AM8" s="428"/>
-      <c r="AN8" s="636"/>
+      <c r="AN8" s="641"/>
     </row>
     <row r="9" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="232" t="s">
@@ -7467,17 +7465,17 @@
       <c r="D9" s="348" t="s">
         <v>282</v>
       </c>
-      <c r="F9" s="641"/>
-      <c r="G9" s="628"/>
-      <c r="H9" s="624"/>
+      <c r="F9" s="620"/>
+      <c r="G9" s="677"/>
+      <c r="H9" s="673"/>
       <c r="I9" s="600"/>
-      <c r="J9" s="624"/>
-      <c r="K9" s="630"/>
-      <c r="L9" s="664"/>
-      <c r="M9" s="643"/>
-      <c r="N9" s="667"/>
-      <c r="O9" s="646"/>
-      <c r="S9" s="657" t="s">
+      <c r="J9" s="673"/>
+      <c r="K9" s="679"/>
+      <c r="L9" s="633"/>
+      <c r="M9" s="648"/>
+      <c r="N9" s="638"/>
+      <c r="O9" s="651"/>
+      <c r="S9" s="634" t="s">
         <v>61</v>
       </c>
       <c r="T9" s="89"/>
@@ -7489,7 +7487,7 @@
       <c r="X9" s="431" t="s">
         <v>163</v>
       </c>
-      <c r="Y9" s="654"/>
+      <c r="Y9" s="658"/>
       <c r="Z9" s="410"/>
       <c r="AA9" s="307"/>
       <c r="AB9" s="209"/>
@@ -7499,16 +7497,16 @@
       </c>
       <c r="AE9" s="257"/>
       <c r="AF9" s="257"/>
-      <c r="AG9" s="656"/>
+      <c r="AG9" s="631"/>
       <c r="AH9" s="257"/>
-      <c r="AI9" s="650"/>
+      <c r="AI9" s="630"/>
       <c r="AJ9" s="80"/>
-      <c r="AK9" s="650" t="s">
+      <c r="AK9" s="630" t="s">
         <v>252</v>
       </c>
       <c r="AL9" s="257"/>
       <c r="AM9" s="428"/>
-      <c r="AN9" s="636"/>
+      <c r="AN9" s="641"/>
       <c r="AP9" s="2" t="s">
         <v>509</v>
       </c>
@@ -7523,22 +7521,22 @@
       <c r="D10" s="142"/>
       <c r="E10" s="237">
         <f>Boat!W8</f>
-        <v>43</v>
-      </c>
-      <c r="F10" s="641"/>
+        <v>41</v>
+      </c>
+      <c r="F10" s="620"/>
       <c r="N10" s="418" t="s">
         <v>397</v>
       </c>
-      <c r="O10" s="678" t="s">
+      <c r="O10" s="622" t="s">
         <v>102</v>
       </c>
-      <c r="P10" s="647" t="s">
+      <c r="P10" s="652" t="s">
         <v>401</v>
       </c>
       <c r="R10" s="74" t="s">
         <v>44</v>
       </c>
-      <c r="S10" s="665"/>
+      <c r="S10" s="635"/>
       <c r="T10" s="89"/>
       <c r="U10" s="123" t="s">
         <v>176</v>
@@ -7550,7 +7548,7 @@
       <c r="X10" s="431" t="s">
         <v>164</v>
       </c>
-      <c r="Y10" s="654"/>
+      <c r="Y10" s="658"/>
       <c r="Z10" s="409">
         <v>0</v>
       </c>
@@ -7568,16 +7566,16 @@
       <c r="AF10" s="238" t="s">
         <v>312</v>
       </c>
-      <c r="AG10" s="656"/>
+      <c r="AG10" s="631"/>
       <c r="AH10" s="80"/>
-      <c r="AI10" s="650"/>
+      <c r="AI10" s="630"/>
       <c r="AJ10" s="257"/>
-      <c r="AK10" s="650"/>
+      <c r="AK10" s="630"/>
       <c r="AL10" s="257"/>
       <c r="AM10" s="442" t="s">
         <v>319</v>
       </c>
-      <c r="AN10" s="636"/>
+      <c r="AN10" s="641"/>
       <c r="AO10" s="204" t="s">
         <v>94</v>
       </c>
@@ -7595,18 +7593,18 @@
       <c r="D11" s="170" t="s">
         <v>356</v>
       </c>
-      <c r="F11" s="641"/>
+      <c r="F11" s="620"/>
       <c r="M11" s="6"/>
       <c r="N11" s="117">
         <v>7</v>
       </c>
-      <c r="O11" s="679"/>
-      <c r="P11" s="648"/>
+      <c r="O11" s="623"/>
+      <c r="P11" s="653"/>
       <c r="Q11" s="65"/>
       <c r="R11" s="120" t="s">
         <v>221</v>
       </c>
-      <c r="S11" s="665"/>
+      <c r="S11" s="635"/>
       <c r="T11" s="102" t="s">
         <v>44</v>
       </c>
@@ -7616,7 +7614,7 @@
       <c r="X11" s="431" t="s">
         <v>165</v>
       </c>
-      <c r="Y11" s="654"/>
+      <c r="Y11" s="658"/>
       <c r="Z11" s="409"/>
       <c r="AA11" s="307">
         <v>1</v>
@@ -7630,14 +7628,14 @@
       <c r="AF11" s="257" t="s">
         <v>477</v>
       </c>
-      <c r="AG11" s="656"/>
+      <c r="AG11" s="631"/>
       <c r="AH11" s="257"/>
       <c r="AI11" s="70"/>
       <c r="AJ11" s="257"/>
       <c r="AK11" s="257"/>
       <c r="AL11" s="257"/>
       <c r="AM11" s="428"/>
-      <c r="AN11" s="636"/>
+      <c r="AN11" s="641"/>
       <c r="AP11" s="76" t="s">
         <v>485</v>
       </c>
@@ -7656,7 +7654,7 @@
       <c r="E12" s="224">
         <v>3</v>
       </c>
-      <c r="F12" s="641"/>
+      <c r="F12" s="620"/>
       <c r="G12" s="337" t="s">
         <v>401</v>
       </c>
@@ -7665,16 +7663,16 @@
       </c>
       <c r="I12" s="605"/>
       <c r="J12" s="605"/>
-      <c r="K12" s="683"/>
+      <c r="K12" s="627"/>
       <c r="L12" s="203"/>
       <c r="M12" s="203"/>
       <c r="N12" s="203"/>
-      <c r="O12" s="679"/>
-      <c r="P12" s="648"/>
+      <c r="O12" s="623"/>
+      <c r="P12" s="653"/>
       <c r="R12" s="122" t="s">
         <v>180</v>
       </c>
-      <c r="S12" s="658"/>
+      <c r="S12" s="636"/>
       <c r="T12" s="101" t="s">
         <v>44</v>
       </c>
@@ -7684,7 +7682,7 @@
       <c r="X12" s="431" t="s">
         <v>166</v>
       </c>
-      <c r="Y12" s="654"/>
+      <c r="Y12" s="658"/>
       <c r="Z12" s="407">
         <v>1</v>
       </c>
@@ -7695,16 +7693,16 @@
       <c r="AC12" s="100" t="s">
         <v>482</v>
       </c>
-      <c r="AD12" s="668" t="s">
+      <c r="AD12" s="639" t="s">
         <v>241</v>
       </c>
       <c r="AE12" s="441" t="s">
         <v>240</v>
       </c>
-      <c r="AF12" s="656" t="s">
+      <c r="AF12" s="631" t="s">
         <v>229</v>
       </c>
-      <c r="AG12" s="656"/>
+      <c r="AG12" s="631"/>
       <c r="AH12" s="238" t="s">
         <v>260</v>
       </c>
@@ -7714,10 +7712,10 @@
       <c r="AJ12" s="257"/>
       <c r="AK12" s="257"/>
       <c r="AL12" s="257"/>
-      <c r="AM12" s="651" t="s">
+      <c r="AM12" s="655" t="s">
         <v>250</v>
       </c>
-      <c r="AN12" s="636"/>
+      <c r="AN12" s="641"/>
       <c r="AO12" s="338" t="s">
         <v>96</v>
       </c>
@@ -7729,17 +7727,17 @@
       <c r="E13" s="448">
         <v>-3</v>
       </c>
-      <c r="F13" s="641"/>
+      <c r="F13" s="620"/>
       <c r="G13" s="605" t="s">
         <v>431</v>
       </c>
       <c r="H13" s="605"/>
       <c r="I13" s="605"/>
-      <c r="J13" s="683"/>
+      <c r="J13" s="627"/>
       <c r="M13" s="6"/>
       <c r="N13" s="6"/>
-      <c r="O13" s="679"/>
-      <c r="P13" s="649"/>
+      <c r="O13" s="623"/>
+      <c r="P13" s="654"/>
       <c r="T13" s="105" t="s">
         <v>44</v>
       </c>
@@ -7749,7 +7747,7 @@
       <c r="X13" s="431" t="s">
         <v>167</v>
       </c>
-      <c r="Y13" s="654"/>
+      <c r="Y13" s="658"/>
       <c r="Z13" s="407">
         <v>1</v>
       </c>
@@ -7760,8 +7758,8 @@
         <v>501</v>
       </c>
       <c r="AC13" s="16"/>
-      <c r="AD13" s="668"/>
-      <c r="AF13" s="656"/>
+      <c r="AD13" s="639"/>
+      <c r="AF13" s="631"/>
       <c r="AG13" s="80"/>
       <c r="AH13" s="238" t="s">
         <v>309</v>
@@ -7772,8 +7770,8 @@
       <c r="AJ13" s="80"/>
       <c r="AK13" s="257"/>
       <c r="AL13" s="257"/>
-      <c r="AM13" s="651"/>
-      <c r="AN13" s="636"/>
+      <c r="AM13" s="655"/>
+      <c r="AN13" s="641"/>
     </row>
     <row r="14" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="450"/>
@@ -7781,18 +7779,18 @@
       <c r="C14" s="459"/>
       <c r="D14" s="452"/>
       <c r="E14" s="453"/>
-      <c r="F14" s="641"/>
+      <c r="F14" s="620"/>
       <c r="G14" s="605" t="s">
         <v>430</v>
       </c>
       <c r="H14" s="605"/>
       <c r="I14" s="605"/>
-      <c r="J14" s="683"/>
+      <c r="J14" s="627"/>
       <c r="K14" s="2">
         <v>12</v>
       </c>
       <c r="N14" s="6"/>
-      <c r="O14" s="679"/>
+      <c r="O14" s="623"/>
       <c r="Q14" s="61" t="s">
         <v>534</v>
       </c>
@@ -7806,24 +7804,24 @@
       <c r="X14" s="431" t="s">
         <v>168</v>
       </c>
-      <c r="Y14" s="654"/>
+      <c r="Y14" s="658"/>
       <c r="Z14" s="407">
         <v>1</v>
       </c>
       <c r="AA14" s="307"/>
       <c r="AB14" s="209"/>
       <c r="AC14" s="16"/>
-      <c r="AD14" s="668"/>
+      <c r="AD14" s="639"/>
       <c r="AE14" s="257"/>
-      <c r="AF14" s="656"/>
+      <c r="AF14" s="631"/>
       <c r="AG14" s="257"/>
       <c r="AH14" s="257"/>
       <c r="AI14" s="70"/>
       <c r="AJ14" s="257"/>
       <c r="AK14" s="257"/>
       <c r="AL14" s="257"/>
-      <c r="AM14" s="651"/>
-      <c r="AN14" s="636"/>
+      <c r="AM14" s="655"/>
+      <c r="AN14" s="641"/>
     </row>
     <row r="15" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="449" t="s">
@@ -7832,8 +7830,8 @@
       <c r="C15" s="598" t="s">
         <v>374</v>
       </c>
-      <c r="F15" s="641"/>
-      <c r="O15" s="679"/>
+      <c r="F15" s="620"/>
+      <c r="O15" s="623"/>
       <c r="R15" s="99" t="s">
         <v>44</v>
       </c>
@@ -7846,7 +7844,7 @@
       <c r="X15" s="431" t="s">
         <v>169</v>
       </c>
-      <c r="Y15" s="654"/>
+      <c r="Y15" s="658"/>
       <c r="Z15" s="409">
         <v>1</v>
       </c>
@@ -7855,8 +7853,8 @@
       <c r="AC15" s="76" t="s">
         <v>480</v>
       </c>
-      <c r="AD15" s="668"/>
-      <c r="AF15" s="656"/>
+      <c r="AD15" s="639"/>
+      <c r="AF15" s="631"/>
       <c r="AG15" s="80"/>
       <c r="AH15" s="238" t="s">
         <v>449</v>
@@ -7869,8 +7867,8 @@
       </c>
       <c r="AK15" s="257"/>
       <c r="AL15" s="257"/>
-      <c r="AM15" s="651"/>
-      <c r="AN15" s="636"/>
+      <c r="AM15" s="655"/>
+      <c r="AN15" s="641"/>
       <c r="AP15" s="76" t="s">
         <v>73</v>
       </c>
@@ -7892,13 +7890,13 @@
       <c r="E16" s="224">
         <v>1</v>
       </c>
-      <c r="F16" s="641"/>
+      <c r="F16" s="620"/>
       <c r="G16" s="337" t="s">
         <v>489</v>
       </c>
       <c r="I16" s="469"/>
       <c r="J16" s="20"/>
-      <c r="O16" s="679"/>
+      <c r="O16" s="623"/>
       <c r="R16" s="435" t="s">
         <v>184</v>
       </c>
@@ -7909,7 +7907,7 @@
       <c r="X16" s="431" t="s">
         <v>170</v>
       </c>
-      <c r="Y16" s="654"/>
+      <c r="Y16" s="658"/>
       <c r="Z16" s="407">
         <v>1</v>
       </c>
@@ -7930,18 +7928,18 @@
       <c r="AM16" s="428" t="s">
         <v>318</v>
       </c>
-      <c r="AN16" s="636"/>
+      <c r="AN16" s="641"/>
       <c r="AP16" s="76" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="17" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="80"/>
-      <c r="F17" s="641"/>
+      <c r="F17" s="620"/>
       <c r="I17" s="470"/>
       <c r="J17" s="20"/>
       <c r="N17" s="6"/>
-      <c r="O17" s="679"/>
+      <c r="O17" s="623"/>
       <c r="Q17" s="21" t="s">
         <v>532</v>
       </c>
@@ -7961,7 +7959,7 @@
       <c r="X17" s="431" t="s">
         <v>171</v>
       </c>
-      <c r="Y17" s="654"/>
+      <c r="Y17" s="658"/>
       <c r="Z17" s="409"/>
       <c r="AA17" s="307"/>
       <c r="AB17" s="209"/>
@@ -7986,7 +7984,7 @@
       <c r="AK17" s="257"/>
       <c r="AL17" s="80"/>
       <c r="AM17" s="428"/>
-      <c r="AN17" s="636"/>
+      <c r="AN17" s="641"/>
       <c r="AO17" s="204" t="s">
         <v>498</v>
       </c>
@@ -8010,21 +8008,21 @@
       <c r="E18" s="99" t="s">
         <v>44</v>
       </c>
-      <c r="F18" s="641"/>
+      <c r="F18" s="620"/>
       <c r="G18" s="337" t="s">
         <v>529</v>
       </c>
       <c r="I18" s="24"/>
       <c r="J18" s="20"/>
-      <c r="O18" s="679"/>
+      <c r="O18" s="623"/>
       <c r="Q18" s="112"/>
-      <c r="R18" s="673" t="s">
+      <c r="R18" s="615" t="s">
         <v>537</v>
       </c>
       <c r="T18" s="100" t="s">
         <v>44</v>
       </c>
-      <c r="U18" s="612" t="s">
+      <c r="U18" s="663" t="s">
         <v>44</v>
       </c>
       <c r="V18" s="120"/>
@@ -8034,7 +8032,7 @@
       <c r="X18" s="431" t="s">
         <v>172</v>
       </c>
-      <c r="Y18" s="654"/>
+      <c r="Y18" s="658"/>
       <c r="Z18" s="409">
         <v>1</v>
       </c>
@@ -8045,38 +8043,38 @@
       <c r="AC18" s="16"/>
       <c r="AD18" s="16"/>
       <c r="AE18" s="257"/>
-      <c r="AF18" s="650" t="s">
+      <c r="AF18" s="630" t="s">
         <v>476</v>
       </c>
       <c r="AG18" s="257"/>
       <c r="AH18" s="70"/>
       <c r="AI18" s="70"/>
-      <c r="AJ18" s="652" t="s">
+      <c r="AJ18" s="656" t="s">
         <v>316</v>
       </c>
       <c r="AK18" s="257"/>
       <c r="AL18" s="80"/>
       <c r="AM18" s="428"/>
-      <c r="AN18" s="636"/>
+      <c r="AN18" s="641"/>
       <c r="AP18" s="76" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="19" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F19" s="641"/>
+      <c r="F19" s="620"/>
       <c r="I19" s="219"/>
-      <c r="O19" s="679"/>
-      <c r="R19" s="674"/>
+      <c r="O19" s="623"/>
+      <c r="R19" s="616"/>
       <c r="S19" s="30" t="s">
         <v>535</v>
       </c>
-      <c r="U19" s="613"/>
+      <c r="U19" s="664"/>
       <c r="V19" s="146"/>
       <c r="W19" s="146"/>
       <c r="X19" s="431" t="s">
         <v>173</v>
       </c>
-      <c r="Y19" s="654"/>
+      <c r="Y19" s="658"/>
       <c r="Z19" s="407">
         <v>1</v>
       </c>
@@ -8085,17 +8083,17 @@
       <c r="AC19" s="16"/>
       <c r="AD19" s="16"/>
       <c r="AE19" s="257"/>
-      <c r="AF19" s="650"/>
+      <c r="AF19" s="630"/>
       <c r="AG19" s="257"/>
       <c r="AH19" s="257"/>
       <c r="AI19" s="70"/>
-      <c r="AJ19" s="652"/>
+      <c r="AJ19" s="656"/>
       <c r="AK19" s="460" t="s">
         <v>252</v>
       </c>
       <c r="AL19" s="80"/>
       <c r="AM19" s="428"/>
-      <c r="AN19" s="636"/>
+      <c r="AN19" s="641"/>
       <c r="AP19" s="76" t="s">
         <v>469</v>
       </c>
@@ -8116,24 +8114,24 @@
       <c r="E20" s="437">
         <v>-1</v>
       </c>
-      <c r="F20" s="641"/>
+      <c r="F20" s="620"/>
       <c r="G20" s="337" t="s">
         <v>492</v>
       </c>
       <c r="I20" s="219"/>
-      <c r="O20" s="679"/>
-      <c r="Q20" s="681" t="s">
+      <c r="O20" s="623"/>
+      <c r="Q20" s="625" t="s">
         <v>48</v>
       </c>
       <c r="T20" s="404" t="s">
         <v>44</v>
       </c>
-      <c r="U20" s="614"/>
+      <c r="U20" s="665"/>
       <c r="W20" s="405"/>
       <c r="X20" s="432" t="s">
         <v>174</v>
       </c>
-      <c r="Y20" s="654"/>
+      <c r="Y20" s="658"/>
       <c r="Z20" s="411">
         <v>1</v>
       </c>
@@ -8158,7 +8156,7 @@
       <c r="AM20" s="381" t="s">
         <v>250</v>
       </c>
-      <c r="AN20" s="636"/>
+      <c r="AN20" s="641"/>
       <c r="AO20" s="338" t="s">
         <v>461</v>
       </c>
@@ -8179,20 +8177,20 @@
       <c r="E21" s="265">
         <v>0</v>
       </c>
-      <c r="F21" s="641"/>
+      <c r="F21" s="620"/>
       <c r="I21" s="219"/>
-      <c r="O21" s="679"/>
-      <c r="Q21" s="682"/>
+      <c r="O21" s="623"/>
+      <c r="Q21" s="626"/>
       <c r="T21" s="422"/>
       <c r="U21" s="14"/>
-      <c r="V21" s="609"/>
+      <c r="V21" s="660"/>
       <c r="W21" s="426" t="s">
         <v>175</v>
       </c>
       <c r="X21" s="429" t="s">
         <v>186</v>
       </c>
-      <c r="Y21" s="654"/>
+      <c r="Y21" s="658"/>
       <c r="Z21" s="445">
         <v>3</v>
       </c>
@@ -8223,15 +8221,15 @@
       <c r="AM21" s="428" t="s">
         <v>546</v>
       </c>
-      <c r="AN21" s="636"/>
+      <c r="AN21" s="641"/>
     </row>
     <row r="22" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F22" s="641"/>
+      <c r="F22" s="620"/>
       <c r="G22" s="337" t="s">
         <v>490</v>
       </c>
       <c r="I22" s="219"/>
-      <c r="O22" s="679"/>
+      <c r="O22" s="623"/>
       <c r="R22" s="434" t="s">
         <v>44</v>
       </c>
@@ -8239,14 +8237,14 @@
         <v>44</v>
       </c>
       <c r="U22" s="15"/>
-      <c r="V22" s="610"/>
+      <c r="V22" s="661"/>
       <c r="W22" s="426" t="s">
         <v>175</v>
       </c>
       <c r="X22" s="429" t="s">
         <v>187</v>
       </c>
-      <c r="Y22" s="654"/>
+      <c r="Y22" s="658"/>
       <c r="Z22" s="415"/>
       <c r="AA22" s="10"/>
       <c r="AB22" s="415"/>
@@ -8257,7 +8255,7 @@
       <c r="AG22" s="6"/>
       <c r="AH22" s="6"/>
       <c r="AI22" s="6"/>
-      <c r="AJ22" s="650" t="s">
+      <c r="AJ22" s="630" t="s">
         <v>473</v>
       </c>
       <c r="AK22" s="257"/>
@@ -8265,7 +8263,7 @@
         <v>479</v>
       </c>
       <c r="AM22" s="300"/>
-      <c r="AN22" s="636"/>
+      <c r="AN22" s="641"/>
     </row>
     <row r="23" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="231" t="s">
@@ -8283,22 +8281,22 @@
       <c r="E23" s="225">
         <v>1</v>
       </c>
-      <c r="F23" s="641"/>
+      <c r="F23" s="620"/>
       <c r="I23" s="219"/>
-      <c r="O23" s="679"/>
-      <c r="Q23" s="681" t="s">
+      <c r="O23" s="623"/>
+      <c r="Q23" s="625" t="s">
         <v>144</v>
       </c>
       <c r="T23" s="17"/>
       <c r="U23" s="420" t="s">
         <v>44</v>
       </c>
-      <c r="V23" s="610"/>
+      <c r="V23" s="661"/>
       <c r="W23" s="148"/>
       <c r="X23" s="429" t="s">
         <v>188</v>
       </c>
-      <c r="Y23" s="654"/>
+      <c r="Y23" s="658"/>
       <c r="Z23" s="17"/>
       <c r="AA23" s="10"/>
       <c r="AB23" s="415"/>
@@ -8309,13 +8307,13 @@
       <c r="AG23" s="6"/>
       <c r="AH23" s="6"/>
       <c r="AI23" s="6"/>
-      <c r="AJ23" s="650"/>
+      <c r="AJ23" s="630"/>
       <c r="AK23" s="257"/>
       <c r="AL23" s="80" t="s">
         <v>508</v>
       </c>
       <c r="AM23" s="300"/>
-      <c r="AN23" s="636"/>
+      <c r="AN23" s="641"/>
     </row>
     <row r="24" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="440" t="s">
@@ -8333,23 +8331,23 @@
       <c r="E24" s="436">
         <v>1</v>
       </c>
-      <c r="F24" s="641"/>
+      <c r="F24" s="620"/>
       <c r="G24" s="61" t="s">
         <v>491</v>
       </c>
       <c r="I24" s="219"/>
-      <c r="O24" s="679"/>
-      <c r="Q24" s="682"/>
+      <c r="O24" s="623"/>
+      <c r="Q24" s="626"/>
       <c r="T24" s="17"/>
       <c r="U24" s="227" t="s">
         <v>44</v>
       </c>
-      <c r="V24" s="610"/>
+      <c r="V24" s="661"/>
       <c r="W24" s="148"/>
       <c r="X24" s="429" t="s">
         <v>185</v>
       </c>
-      <c r="Y24" s="654"/>
+      <c r="Y24" s="658"/>
       <c r="Z24" s="17"/>
       <c r="AA24" s="10"/>
       <c r="AB24" s="415"/>
@@ -8368,12 +8366,12 @@
         <v>464</v>
       </c>
       <c r="AM24" s="300"/>
-      <c r="AN24" s="636"/>
+      <c r="AN24" s="641"/>
     </row>
     <row r="25" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F25" s="641"/>
+      <c r="F25" s="620"/>
       <c r="I25" s="219"/>
-      <c r="O25" s="679"/>
+      <c r="O25" s="623"/>
       <c r="P25" s="204" t="s">
         <v>281</v>
       </c>
@@ -8386,12 +8384,12 @@
       <c r="U25" s="400" t="s">
         <v>44</v>
       </c>
-      <c r="V25" s="611"/>
+      <c r="V25" s="662"/>
       <c r="W25" s="148"/>
       <c r="X25" s="429" t="s">
         <v>189</v>
       </c>
-      <c r="Y25" s="654"/>
+      <c r="Y25" s="658"/>
       <c r="Z25" s="17"/>
       <c r="AA25" s="10"/>
       <c r="AB25" s="415"/>
@@ -8408,7 +8406,7 @@
       <c r="AK25" s="142"/>
       <c r="AL25" s="6"/>
       <c r="AM25" s="300"/>
-      <c r="AN25" s="636"/>
+      <c r="AN25" s="641"/>
     </row>
     <row r="26" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="231" t="s">
@@ -8426,17 +8424,17 @@
       <c r="E26" s="380">
         <v>1</v>
       </c>
-      <c r="F26" s="641"/>
+      <c r="F26" s="620"/>
       <c r="G26" s="337" t="s">
         <v>488</v>
       </c>
       <c r="I26" s="219"/>
-      <c r="O26" s="679"/>
-      <c r="P26" s="638" t="s">
+      <c r="O26" s="623"/>
+      <c r="P26" s="643" t="s">
         <v>527</v>
       </c>
-      <c r="Q26" s="639"/>
-      <c r="R26" s="675" t="s">
+      <c r="Q26" s="644"/>
+      <c r="R26" s="617" t="s">
         <v>536</v>
       </c>
       <c r="T26" s="178"/>
@@ -8448,7 +8446,7 @@
       <c r="X26" s="429" t="s">
         <v>181</v>
       </c>
-      <c r="Y26" s="654"/>
+      <c r="Y26" s="658"/>
       <c r="Z26" s="17"/>
       <c r="AA26" s="10"/>
       <c r="AB26" s="415"/>
@@ -8475,7 +8473,7 @@
       <c r="AM26" s="442" t="s">
         <v>457</v>
       </c>
-      <c r="AN26" s="636"/>
+      <c r="AN26" s="641"/>
     </row>
     <row r="27" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="21" t="s">
@@ -8487,13 +8485,13 @@
       <c r="E27" s="265" t="s">
         <v>44</v>
       </c>
-      <c r="F27" s="677"/>
+      <c r="F27" s="621"/>
       <c r="G27" s="61" t="s">
         <v>545</v>
       </c>
       <c r="I27" s="220"/>
-      <c r="O27" s="680"/>
-      <c r="R27" s="676"/>
+      <c r="O27" s="624"/>
+      <c r="R27" s="618"/>
       <c r="S27" s="421" t="s">
         <v>54</v>
       </c>
@@ -8506,7 +8504,7 @@
       <c r="X27" s="429" t="s">
         <v>531</v>
       </c>
-      <c r="Y27" s="655"/>
+      <c r="Y27" s="659"/>
       <c r="Z27" s="161"/>
       <c r="AA27" s="13"/>
       <c r="AB27" s="416"/>
@@ -8523,32 +8521,26 @@
       <c r="AM27" s="381" t="s">
         <v>320</v>
       </c>
-      <c r="AN27" s="637"/>
+      <c r="AN27" s="642"/>
     </row>
   </sheetData>
   <mergeCells count="54">
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="R18:R19"/>
-    <mergeCell ref="R26:R27"/>
-    <mergeCell ref="F2:F27"/>
-    <mergeCell ref="O10:O27"/>
-    <mergeCell ref="Q20:Q21"/>
-    <mergeCell ref="Q23:Q24"/>
-    <mergeCell ref="G14:J14"/>
-    <mergeCell ref="G13:J13"/>
-    <mergeCell ref="H12:K12"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="AI6:AI10"/>
-    <mergeCell ref="AF12:AF15"/>
-    <mergeCell ref="AG7:AG12"/>
-    <mergeCell ref="L8:L9"/>
-    <mergeCell ref="S9:S12"/>
-    <mergeCell ref="N8:N9"/>
-    <mergeCell ref="AD12:AD15"/>
-    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="V21:V25"/>
+    <mergeCell ref="U18:U20"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="J8:J9"/>
+    <mergeCell ref="G5:L6"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="K7:K9"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B4:B5"/>
     <mergeCell ref="AN1:AN27"/>
     <mergeCell ref="P26:Q26"/>
     <mergeCell ref="Q2:Q3"/>
@@ -8565,22 +8557,28 @@
     <mergeCell ref="AD3:AD4"/>
     <mergeCell ref="S2:S3"/>
     <mergeCell ref="R2:R3"/>
-    <mergeCell ref="V21:V25"/>
-    <mergeCell ref="U18:U20"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="J8:J9"/>
-    <mergeCell ref="G5:L6"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="K7:K9"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="AI6:AI10"/>
+    <mergeCell ref="AF12:AF15"/>
+    <mergeCell ref="AG7:AG12"/>
+    <mergeCell ref="L8:L9"/>
+    <mergeCell ref="S9:S12"/>
+    <mergeCell ref="N8:N9"/>
+    <mergeCell ref="AD12:AD15"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="R18:R19"/>
+    <mergeCell ref="R26:R27"/>
+    <mergeCell ref="F2:F27"/>
+    <mergeCell ref="O10:O27"/>
+    <mergeCell ref="Q20:Q21"/>
+    <mergeCell ref="Q23:Q24"/>
+    <mergeCell ref="G14:J14"/>
+    <mergeCell ref="G13:J13"/>
+    <mergeCell ref="H12:K12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8617,12 +8615,12 @@
       <c r="B1" s="603" t="s">
         <v>311</v>
       </c>
-      <c r="C1" s="683"/>
+      <c r="C1" s="627"/>
       <c r="D1" s="204"/>
       <c r="J1" s="603" t="s">
         <v>69</v>
       </c>
-      <c r="K1" s="683"/>
+      <c r="K1" s="627"/>
       <c r="L1" s="195" t="s">
         <v>331</v>
       </c>
@@ -8956,8 +8954,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB54FD83-008D-4F8B-87AC-83E7F70047CB}">
   <dimension ref="A1:AL31"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="AF27" sqref="AF27"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="AG14" sqref="AG14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9025,7 +9023,7 @@
       <c r="P1" s="398" t="s">
         <v>398</v>
       </c>
-      <c r="Q1" s="714" t="s">
+      <c r="Q1" s="701" t="s">
         <v>180</v>
       </c>
       <c r="R1" s="100" t="s">
@@ -9049,7 +9047,7 @@
       <c r="AA1" s="517" t="s">
         <v>438</v>
       </c>
-      <c r="AB1" s="708" t="s">
+      <c r="AB1" s="695" t="s">
         <v>595</v>
       </c>
       <c r="AC1" s="99" t="s">
@@ -9071,32 +9069,32 @@
       </c>
     </row>
     <row r="2" spans="1:38" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="693">
+      <c r="A2" s="706">
         <f ca="1">TODAY()</f>
         <v>45285</v>
       </c>
-      <c r="B2" s="695" t="s">
+      <c r="B2" s="708" t="s">
         <v>380</v>
       </c>
-      <c r="C2" s="615" t="s">
+      <c r="C2" s="645" t="s">
         <v>358</v>
       </c>
-      <c r="D2" s="697" t="s">
+      <c r="D2" s="710" t="s">
         <v>102</v>
       </c>
-      <c r="E2" s="699" t="s">
+      <c r="E2" s="712" t="s">
         <v>64</v>
       </c>
       <c r="F2" s="191" t="s">
         <v>219</v>
       </c>
-      <c r="G2" s="659" t="s">
+      <c r="G2" s="613" t="s">
         <v>373</v>
       </c>
       <c r="H2" s="206" t="s">
         <v>219</v>
       </c>
-      <c r="I2" s="705" t="s">
+      <c r="I2" s="692" t="s">
         <v>102</v>
       </c>
       <c r="J2" s="396" t="s">
@@ -9120,7 +9118,7 @@
       <c r="P2" s="399">
         <v>40</v>
       </c>
-      <c r="Q2" s="715"/>
+      <c r="Q2" s="702"/>
       <c r="R2" s="21">
         <f>R7+R20</f>
         <v>2</v>
@@ -9145,7 +9143,7 @@
         <f>IF((Z2+T2)&gt;0,0,-1)</f>
         <v>0</v>
       </c>
-      <c r="AB2" s="709"/>
+      <c r="AB2" s="696"/>
       <c r="AC2" s="35"/>
       <c r="AH2" s="6" t="s">
         <v>345</v>
@@ -9158,14 +9156,14 @@
       <c r="AL2" s="469"/>
     </row>
     <row r="3" spans="1:38" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="694"/>
-      <c r="B3" s="696"/>
-      <c r="C3" s="616"/>
-      <c r="D3" s="698"/>
-      <c r="E3" s="700"/>
-      <c r="G3" s="660"/>
+      <c r="A3" s="707"/>
+      <c r="B3" s="709"/>
+      <c r="C3" s="646"/>
+      <c r="D3" s="711"/>
+      <c r="E3" s="713"/>
+      <c r="G3" s="614"/>
       <c r="H3" s="6"/>
-      <c r="I3" s="706"/>
+      <c r="I3" s="693"/>
       <c r="K3" s="24">
         <v>2</v>
       </c>
@@ -9180,7 +9178,7 @@
       <c r="V3" s="470"/>
       <c r="W3" s="6"/>
       <c r="X3" s="470"/>
-      <c r="AB3" s="709"/>
+      <c r="AB3" s="696"/>
       <c r="AC3" s="35"/>
       <c r="AE3" s="100" t="s">
         <v>590</v>
@@ -9205,10 +9203,10 @@
         <v>381</v>
       </c>
       <c r="B4" s="243"/>
-      <c r="C4" s="701" t="s">
+      <c r="C4" s="714" t="s">
         <v>177</v>
       </c>
-      <c r="I4" s="706"/>
+      <c r="I4" s="693"/>
       <c r="R4" s="471" t="s">
         <v>590</v>
       </c>
@@ -9220,7 +9218,7 @@
       <c r="V4" s="470"/>
       <c r="W4" s="6"/>
       <c r="X4" s="470"/>
-      <c r="AB4" s="709"/>
+      <c r="AB4" s="696"/>
       <c r="AC4" s="35"/>
       <c r="AE4" s="20"/>
       <c r="AF4" s="100" t="s">
@@ -9247,7 +9245,7 @@
       <c r="B5" s="100" t="s">
         <v>358</v>
       </c>
-      <c r="C5" s="702"/>
+      <c r="C5" s="715"/>
       <c r="D5" s="222" t="s">
         <v>102</v>
       </c>
@@ -9263,7 +9261,7 @@
       <c r="H5" s="206" t="s">
         <v>219</v>
       </c>
-      <c r="I5" s="706"/>
+      <c r="I5" s="693"/>
       <c r="J5" s="397" t="s">
         <v>269</v>
       </c>
@@ -9290,7 +9288,7 @@
       <c r="V5" s="468"/>
       <c r="W5" s="6"/>
       <c r="X5" s="468"/>
-      <c r="AB5" s="709"/>
+      <c r="AB5" s="696"/>
       <c r="AC5" s="2" t="s">
         <v>593</v>
       </c>
@@ -9308,19 +9306,19 @@
       </c>
     </row>
     <row r="6" spans="1:38" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="690" t="s">
+      <c r="A6" s="703" t="s">
         <v>286</v>
       </c>
       <c r="B6" s="105" t="s">
         <v>198</v>
       </c>
-      <c r="C6" s="661"/>
-      <c r="D6" s="662"/>
+      <c r="C6" s="628"/>
+      <c r="D6" s="629"/>
       <c r="E6" s="96">
         <v>1</v>
       </c>
       <c r="G6" s="599"/>
-      <c r="I6" s="706"/>
+      <c r="I6" s="693"/>
       <c r="P6" s="61" t="s">
         <v>593</v>
       </c>
@@ -9332,11 +9330,11 @@
         <f>S7+S11-SUM(V2:V10)</f>
         <v>3</v>
       </c>
-      <c r="AB6" s="709"/>
+      <c r="AB6" s="696"/>
       <c r="AC6" s="35"/>
       <c r="AE6" s="64">
         <f>AE7-SUM(AL2:AL10)+AE11</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AF6" s="64">
         <f>AF7-SUM(AI2:AI10)+AF11</f>
@@ -9348,7 +9346,7 @@
       <c r="AL6" s="112"/>
     </row>
     <row r="7" spans="1:38" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="691"/>
+      <c r="A7" s="704"/>
       <c r="B7" s="100" t="s">
         <v>154</v>
       </c>
@@ -9359,7 +9357,7 @@
         <v>135</v>
       </c>
       <c r="G7" s="599"/>
-      <c r="I7" s="706"/>
+      <c r="I7" s="693"/>
       <c r="M7" s="16" t="s">
         <v>348</v>
       </c>
@@ -9391,7 +9389,7 @@
       <c r="X7" s="469">
         <v>1</v>
       </c>
-      <c r="AB7" s="709"/>
+      <c r="AB7" s="696"/>
       <c r="AC7" s="99" t="s">
         <v>594</v>
       </c>
@@ -9413,11 +9411,11 @@
         <v>614</v>
       </c>
       <c r="AL7" s="24">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="692"/>
+      <c r="A8" s="705"/>
       <c r="B8" s="212" t="s">
         <v>28</v>
       </c>
@@ -9426,13 +9424,13 @@
         <v>3</v>
       </c>
       <c r="G8" s="599"/>
-      <c r="I8" s="706"/>
+      <c r="I8" s="693"/>
       <c r="N8" s="80"/>
       <c r="U8" s="6"/>
       <c r="V8" s="24"/>
       <c r="W8" s="6"/>
       <c r="X8" s="470"/>
-      <c r="AB8" s="709"/>
+      <c r="AB8" s="696"/>
       <c r="AC8" s="515"/>
       <c r="AH8" s="6" t="s">
         <v>613</v>
@@ -9441,8 +9439,12 @@
         <v>1</v>
       </c>
       <c r="AJ8" s="553"/>
-      <c r="AK8" s="6"/>
-      <c r="AL8" s="469"/>
+      <c r="AK8" s="6" t="s">
+        <v>622</v>
+      </c>
+      <c r="AL8" s="469">
+        <v>1</v>
+      </c>
     </row>
     <row r="9" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="231" t="s">
@@ -9459,7 +9461,7 @@
       </c>
       <c r="G9" s="599"/>
       <c r="H9" s="6"/>
-      <c r="I9" s="706"/>
+      <c r="I9" s="693"/>
       <c r="M9" s="19" t="s">
         <v>526</v>
       </c>
@@ -9468,7 +9470,7 @@
       <c r="V9" s="24"/>
       <c r="W9" s="6"/>
       <c r="X9" s="470"/>
-      <c r="AB9" s="709"/>
+      <c r="AB9" s="696"/>
       <c r="AC9" s="515"/>
       <c r="AE9" s="20"/>
       <c r="AF9" s="20"/>
@@ -9489,10 +9491,10 @@
       <c r="D10" s="108"/>
       <c r="E10" s="68">
         <f>Boat!W8</f>
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G10" s="599"/>
-      <c r="I10" s="706"/>
+      <c r="I10" s="693"/>
       <c r="J10" s="24" t="s">
         <v>373</v>
       </c>
@@ -9507,7 +9509,7 @@
       <c r="V10" s="470"/>
       <c r="W10" s="6"/>
       <c r="X10" s="470"/>
-      <c r="AB10" s="709"/>
+      <c r="AB10" s="696"/>
       <c r="AC10" s="515"/>
       <c r="AE10" s="20"/>
       <c r="AF10" s="20"/>
@@ -9539,7 +9541,7 @@
         <v>266</v>
       </c>
       <c r="G11" s="599"/>
-      <c r="I11" s="706"/>
+      <c r="I11" s="693"/>
       <c r="J11" s="24" t="s">
         <v>194</v>
       </c>
@@ -9565,13 +9567,13 @@
       <c r="S11" s="24">
         <v>3</v>
       </c>
-      <c r="U11" s="711" t="s">
+      <c r="U11" s="698" t="s">
         <v>559</v>
       </c>
-      <c r="V11" s="712"/>
-      <c r="W11" s="712"/>
-      <c r="X11" s="713"/>
-      <c r="AB11" s="710"/>
+      <c r="V11" s="699"/>
+      <c r="W11" s="699"/>
+      <c r="X11" s="700"/>
+      <c r="AB11" s="697"/>
       <c r="AC11" s="99" t="s">
         <v>596</v>
       </c>
@@ -9585,13 +9587,13 @@
         <v>5</v>
       </c>
       <c r="AG11" s="414"/>
-      <c r="AH11" s="711" t="s">
+      <c r="AH11" s="698" t="s">
         <v>604</v>
       </c>
-      <c r="AI11" s="712"/>
-      <c r="AJ11" s="712"/>
-      <c r="AK11" s="712"/>
-      <c r="AL11" s="713"/>
+      <c r="AI11" s="699"/>
+      <c r="AJ11" s="699"/>
+      <c r="AK11" s="699"/>
+      <c r="AL11" s="700"/>
     </row>
     <row r="12" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="227" t="s">
@@ -9602,7 +9604,7 @@
         <v>3</v>
       </c>
       <c r="G12" s="599"/>
-      <c r="I12" s="706"/>
+      <c r="I12" s="693"/>
       <c r="J12" s="24" t="s">
         <v>517</v>
       </c>
@@ -9635,7 +9637,7 @@
       </c>
       <c r="D13" s="20"/>
       <c r="G13" s="599"/>
-      <c r="I13" s="706"/>
+      <c r="I13" s="693"/>
       <c r="J13" s="108" t="s">
         <v>549</v>
       </c>
@@ -9679,7 +9681,7 @@
       <c r="H14" s="206" t="s">
         <v>219</v>
       </c>
-      <c r="I14" s="706"/>
+      <c r="I14" s="693"/>
       <c r="U14" s="67" t="s">
         <v>80</v>
       </c>
@@ -9706,7 +9708,7 @@
       <c r="H15" s="271">
         <v>0</v>
       </c>
-      <c r="I15" s="706"/>
+      <c r="I15" s="693"/>
       <c r="J15" s="108" t="s">
         <v>153</v>
       </c>
@@ -9737,7 +9739,7 @@
       <c r="D16" s="2" t="s">
         <v>493</v>
       </c>
-      <c r="I16" s="706"/>
+      <c r="I16" s="693"/>
       <c r="K16" s="100" t="s">
         <v>44</v>
       </c>
@@ -9773,7 +9775,7 @@
       <c r="G17" s="2" t="s">
         <v>424</v>
       </c>
-      <c r="I17" s="706"/>
+      <c r="I17" s="693"/>
       <c r="L17" s="2" t="s">
         <v>427</v>
       </c>
@@ -9787,13 +9789,13 @@
     </row>
     <row r="18" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G18" s="16"/>
-      <c r="I18" s="706"/>
+      <c r="I18" s="693"/>
       <c r="L18" s="16"/>
       <c r="M18" s="21"/>
-      <c r="O18" s="703" t="s">
+      <c r="O18" s="690" t="s">
         <v>518</v>
       </c>
-      <c r="P18" s="704"/>
+      <c r="P18" s="691"/>
       <c r="Q18" s="127" t="s">
         <v>44</v>
       </c>
@@ -9811,7 +9813,7 @@
       <c r="X18" s="24"/>
     </row>
     <row r="19" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I19" s="706"/>
+      <c r="I19" s="693"/>
       <c r="M19" s="21" t="s">
         <v>426</v>
       </c>
@@ -9843,7 +9845,7 @@
       <c r="G20" s="2" t="s">
         <v>424</v>
       </c>
-      <c r="I20" s="706"/>
+      <c r="I20" s="693"/>
       <c r="K20" s="19" t="s">
         <v>423</v>
       </c>
@@ -9870,7 +9872,7 @@
       <c r="X20" s="468"/>
     </row>
     <row r="21" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I21" s="706"/>
+      <c r="I21" s="693"/>
       <c r="M21" s="216" t="s">
         <v>412</v>
       </c>
@@ -9904,7 +9906,7 @@
       <c r="G22" s="2" t="s">
         <v>424</v>
       </c>
-      <c r="I22" s="706"/>
+      <c r="I22" s="693"/>
       <c r="P22" s="99" t="s">
         <v>592</v>
       </c>
@@ -9919,7 +9921,7 @@
       <c r="E23" s="283" t="s">
         <v>44</v>
       </c>
-      <c r="I23" s="706"/>
+      <c r="I23" s="693"/>
       <c r="Q23" s="24">
         <f>SUM(V23:V31)</f>
         <v>10</v>
@@ -9936,7 +9938,7 @@
       </c>
     </row>
     <row r="24" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I24" s="706"/>
+      <c r="I24" s="693"/>
       <c r="U24" s="35"/>
       <c r="V24" s="509">
         <v>2</v>
@@ -9964,7 +9966,7 @@
       <c r="H25" s="191" t="s">
         <v>267</v>
       </c>
-      <c r="I25" s="706"/>
+      <c r="I25" s="693"/>
       <c r="J25" s="397" t="s">
         <v>270</v>
       </c>
@@ -10009,7 +10011,7 @@
       <c r="H26" s="19" t="s">
         <v>219</v>
       </c>
-      <c r="I26" s="706"/>
+      <c r="I26" s="693"/>
       <c r="K26" s="24">
         <v>15</v>
       </c>
@@ -10044,7 +10046,7 @@
       </c>
     </row>
     <row r="27" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I27" s="706"/>
+      <c r="I27" s="693"/>
       <c r="O27" s="2" t="s">
         <v>98</v>
       </c>
@@ -10071,7 +10073,7 @@
       <c r="E28" s="215">
         <v>2</v>
       </c>
-      <c r="I28" s="706"/>
+      <c r="I28" s="693"/>
       <c r="Q28" s="6"/>
       <c r="R28" s="112"/>
       <c r="T28" s="142"/>
@@ -10093,7 +10095,7 @@
       <c r="H29" s="191" t="s">
         <v>268</v>
       </c>
-      <c r="I29" s="707"/>
+      <c r="I29" s="694"/>
       <c r="J29" s="324"/>
       <c r="L29" s="96" t="s">
         <v>274</v>
@@ -10151,13 +10153,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="I2:I29"/>
-    <mergeCell ref="AB1:AB11"/>
-    <mergeCell ref="AH11:AL11"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="Q1:Q2"/>
-    <mergeCell ref="U11:X11"/>
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="G5:G14"/>
     <mergeCell ref="A2:A3"/>
@@ -10169,6 +10164,13 @@
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="G2:G3"/>
     <mergeCell ref="C2:C3"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="I2:I29"/>
+    <mergeCell ref="AB1:AB11"/>
+    <mergeCell ref="AH11:AL11"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="Q1:Q2"/>
+    <mergeCell ref="U11:X11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -10180,7 +10182,7 @@
   <dimension ref="A1:AT37"/>
   <sheetViews>
     <sheetView topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10280,14 +10282,14 @@
         <f ca="1">TODAY()</f>
         <v>45285</v>
       </c>
-      <c r="T1" s="742"/>
+      <c r="T1" s="735"/>
       <c r="U1" s="142"/>
       <c r="V1" s="6"/>
       <c r="W1" s="6"/>
-      <c r="X1" s="726" t="s">
+      <c r="X1" s="719" t="s">
         <v>442</v>
       </c>
-      <c r="Y1" s="727"/>
+      <c r="Y1" s="720"/>
       <c r="Z1" s="306">
         <f>68-(W8+Y3+X3+U3)</f>
         <v>0</v>
@@ -10303,27 +10305,27 @@
       <c r="AD1" s="302" t="s">
         <v>44</v>
       </c>
-      <c r="AE1" s="728" t="s">
+      <c r="AE1" s="721" t="s">
         <v>190</v>
       </c>
-      <c r="AF1" s="729"/>
-      <c r="AG1" s="730"/>
-      <c r="AH1" s="731" t="s">
+      <c r="AF1" s="722"/>
+      <c r="AG1" s="723"/>
+      <c r="AH1" s="724" t="s">
         <v>294</v>
       </c>
-      <c r="AI1" s="732"/>
-      <c r="AJ1" s="733"/>
-      <c r="AK1" s="659" t="s">
+      <c r="AI1" s="725"/>
+      <c r="AJ1" s="726"/>
+      <c r="AK1" s="613" t="s">
         <v>617</v>
       </c>
       <c r="AL1" s="551" t="s">
         <v>618</v>
       </c>
-      <c r="AM1" s="723" t="s">
+      <c r="AM1" s="716" t="s">
         <v>445</v>
       </c>
-      <c r="AN1" s="724"/>
-      <c r="AO1" s="725"/>
+      <c r="AN1" s="717"/>
+      <c r="AO1" s="718"/>
       <c r="AR1" s="142"/>
     </row>
     <row r="2" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -10336,29 +10338,29 @@
       </c>
       <c r="J2" s="318">
         <f>K2+L2</f>
-        <v>15</v>
-      </c>
-      <c r="K2" s="721">
+        <v>17</v>
+      </c>
+      <c r="K2" s="743">
         <f>SUM(K4:K37)</f>
         <v>6</v>
       </c>
-      <c r="L2" s="719">
+      <c r="L2" s="741">
         <f>SUM(L4:L37)</f>
-        <v>9</v>
-      </c>
-      <c r="M2" s="734">
+        <v>11</v>
+      </c>
+      <c r="M2" s="727">
         <f>SUM(M5:M30)</f>
         <v>0</v>
       </c>
-      <c r="N2" s="736">
+      <c r="N2" s="729">
         <f>SUM(N4:N29)</f>
-        <v>2</v>
-      </c>
-      <c r="O2" s="738">
+        <v>4</v>
+      </c>
+      <c r="O2" s="731">
         <f>SUM(O4:O29)</f>
         <v>6</v>
       </c>
-      <c r="P2" s="666">
+      <c r="P2" s="637">
         <f>SUM(N30:N37)* (-1)</f>
         <v>-1</v>
       </c>
@@ -10371,14 +10373,14 @@
       <c r="S2" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="T2" s="743"/>
+      <c r="T2" s="736"/>
       <c r="U2" s="537" t="s">
         <v>263</v>
       </c>
       <c r="V2" s="482" t="s">
         <v>220</v>
       </c>
-      <c r="W2" s="740" t="s">
+      <c r="W2" s="733" t="s">
         <v>235</v>
       </c>
       <c r="X2" s="483" t="s">
@@ -10420,7 +10422,7 @@
       <c r="AJ2" s="150" t="s">
         <v>289</v>
       </c>
-      <c r="AK2" s="660"/>
+      <c r="AK2" s="614"/>
       <c r="AL2" s="592" t="s">
         <v>289</v>
       </c>
@@ -10448,12 +10450,12 @@
         <f>V3+X3+Y3+U3</f>
         <v>68</v>
       </c>
-      <c r="K3" s="722"/>
-      <c r="L3" s="720"/>
-      <c r="M3" s="735"/>
-      <c r="N3" s="737"/>
-      <c r="O3" s="739"/>
-      <c r="P3" s="667"/>
+      <c r="K3" s="744"/>
+      <c r="L3" s="742"/>
+      <c r="M3" s="728"/>
+      <c r="N3" s="730"/>
+      <c r="O3" s="732"/>
+      <c r="P3" s="638"/>
       <c r="Q3" s="172">
         <f>(M2+N2)-Y3</f>
         <v>0</v>
@@ -10461,23 +10463,23 @@
       <c r="S3" s="159" t="s">
         <v>245</v>
       </c>
-      <c r="T3" s="744"/>
+      <c r="T3" s="737"/>
       <c r="U3" s="538">
         <f>SUM(U4:U29)</f>
         <v>13</v>
       </c>
       <c r="V3" s="484">
         <f>SUM(V4:V29)</f>
-        <v>43</v>
-      </c>
-      <c r="W3" s="741"/>
+        <v>41</v>
+      </c>
+      <c r="W3" s="734"/>
       <c r="X3" s="485">
         <f t="shared" ref="X3:AC3" si="0">SUM(X4:X29)</f>
         <v>10</v>
       </c>
       <c r="Y3" s="485">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="Z3" s="59">
         <f t="shared" si="0"/>
@@ -10489,7 +10491,7 @@
       </c>
       <c r="AB3" s="66">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="AC3" s="66">
         <f t="shared" si="0"/>
@@ -10576,7 +10578,7 @@
         <f>AC4</f>
         <v>0</v>
       </c>
-      <c r="P4" s="716" t="s">
+      <c r="P4" s="738" t="s">
         <v>199</v>
       </c>
       <c r="Q4" s="20"/>
@@ -10662,7 +10664,7 @@
         <f>AC5</f>
         <v>0</v>
       </c>
-      <c r="P5" s="717"/>
+      <c r="P5" s="739"/>
       <c r="Q5" s="20"/>
       <c r="R5" s="2" t="s">
         <v>341</v>
@@ -10756,7 +10758,7 @@
         <f>AC6</f>
         <v>0</v>
       </c>
-      <c r="P6" s="717"/>
+      <c r="P6" s="739"/>
       <c r="Q6" s="19" t="s">
         <v>336</v>
       </c>
@@ -10857,7 +10859,7 @@
         <f>AC7</f>
         <v>1</v>
       </c>
-      <c r="P7" s="717"/>
+      <c r="P7" s="739"/>
       <c r="Q7" s="20"/>
       <c r="R7" s="2" t="s">
         <v>336</v>
@@ -10973,7 +10975,7 @@
         <f t="shared" ref="O8:O37" si="10">AC8</f>
         <v>0</v>
       </c>
-      <c r="P8" s="717"/>
+      <c r="P8" s="739"/>
       <c r="Q8" s="21" t="s">
         <v>234</v>
       </c>
@@ -10994,7 +10996,7 @@
       </c>
       <c r="W8" s="24">
         <f>V3</f>
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="X8" s="497">
         <v>0</v>
@@ -11064,7 +11066,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="P9" s="717"/>
+      <c r="P9" s="739"/>
       <c r="Q9" s="21" t="s">
         <v>336</v>
       </c>
@@ -11169,7 +11171,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="P10" s="717"/>
+      <c r="P10" s="739"/>
       <c r="Q10" s="20"/>
       <c r="R10" s="2" t="s">
         <v>341</v>
@@ -11261,7 +11263,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="P11" s="717"/>
+      <c r="P11" s="739"/>
       <c r="Q11" s="21" t="s">
         <v>336</v>
       </c>
@@ -11326,14 +11328,14 @@
       <c r="AR11" s="508"/>
     </row>
     <row r="12" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="626" t="s">
+      <c r="A12" s="675" t="s">
         <v>55</v>
       </c>
       <c r="B12" s="30">
         <v>13</v>
       </c>
       <c r="C12" s="2"/>
-      <c r="E12" s="681" t="s">
+      <c r="E12" s="625" t="s">
         <v>56</v>
       </c>
       <c r="G12" s="262"/>
@@ -11348,17 +11350,17 @@
       </c>
       <c r="K12" s="575"/>
       <c r="L12" s="581">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M12" s="328"/>
       <c r="N12" s="107">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O12" s="293">
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="P12" s="717"/>
+      <c r="P12" s="739"/>
       <c r="Q12" s="21" t="s">
         <v>336</v>
       </c>
@@ -11371,7 +11373,7 @@
       </c>
       <c r="U12" s="503"/>
       <c r="V12" s="492">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="W12" s="493">
         <v>-2</v>
@@ -11379,7 +11381,7 @@
       <c r="X12" s="496"/>
       <c r="Y12" s="183">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z12" s="296"/>
       <c r="AA12" s="117">
@@ -11388,7 +11390,7 @@
       </c>
       <c r="AB12" s="290">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AC12" s="290">
         <v>1</v>
@@ -11430,17 +11432,19 @@
       <c r="AQ12" s="562" t="s">
         <v>511</v>
       </c>
-      <c r="AR12" s="509"/>
+      <c r="AR12" s="509" t="s">
+        <v>622</v>
+      </c>
     </row>
     <row r="13" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="628"/>
+      <c r="A13" s="677"/>
       <c r="B13" s="584">
         <v>12</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E13" s="682"/>
+      <c r="E13" s="626"/>
       <c r="F13" s="172">
         <v>0</v>
       </c>
@@ -11464,7 +11468,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="P13" s="717"/>
+      <c r="P13" s="739"/>
       <c r="Q13" s="21" t="s">
         <v>336</v>
       </c>
@@ -11546,7 +11550,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="P14" s="717"/>
+      <c r="P14" s="739"/>
       <c r="Q14" s="20"/>
       <c r="R14" s="200" t="s">
         <v>340</v>
@@ -11647,7 +11651,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="P15" s="717"/>
+      <c r="P15" s="739"/>
       <c r="Q15" s="20"/>
       <c r="R15" s="200" t="s">
         <v>340</v>
@@ -11739,7 +11743,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="P16" s="717"/>
+      <c r="P16" s="739"/>
       <c r="Q16" s="21" t="s">
         <v>336</v>
       </c>
@@ -11840,7 +11844,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="P17" s="717"/>
+      <c r="P17" s="739"/>
       <c r="Q17" s="20"/>
       <c r="R17" s="2" t="s">
         <v>342</v>
@@ -11940,7 +11944,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="P18" s="717"/>
+      <c r="P18" s="739"/>
       <c r="Q18" s="21" t="s">
         <v>336</v>
       </c>
@@ -12020,17 +12024,17 @@
         <v>2</v>
       </c>
       <c r="L19" s="582">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M19" s="118"/>
       <c r="N19" s="107">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O19" s="293">
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="P19" s="717"/>
+      <c r="P19" s="739"/>
       <c r="Q19" s="20"/>
       <c r="R19" s="2" t="s">
         <v>335</v>
@@ -12043,7 +12047,7 @@
       </c>
       <c r="U19" s="503"/>
       <c r="V19" s="492">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W19" s="493">
         <v>-1</v>
@@ -12053,7 +12057,7 @@
       </c>
       <c r="Y19" s="183">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z19" s="296"/>
       <c r="AA19" s="117">
@@ -12062,7 +12066,7 @@
       </c>
       <c r="AB19" s="290">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AC19" s="290">
         <v>1</v>
@@ -12138,11 +12142,11 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="P20" s="718"/>
+      <c r="P20" s="740"/>
       <c r="Q20" s="603" t="s">
         <v>336</v>
       </c>
-      <c r="R20" s="683"/>
+      <c r="R20" s="627"/>
       <c r="S20" s="534" t="s">
         <v>85</v>
       </c>
@@ -12402,7 +12406,7 @@
     </row>
     <row r="23" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="24"/>
-      <c r="E23" s="633" t="s">
+      <c r="E23" s="682" t="s">
         <v>290</v>
       </c>
       <c r="F23" s="180"/>
@@ -12505,7 +12509,7 @@
       <c r="C24" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="E24" s="634"/>
+      <c r="E24" s="683"/>
       <c r="F24" s="172"/>
       <c r="H24" s="42"/>
       <c r="J24" s="571" t="s">
@@ -12530,7 +12534,7 @@
       <c r="Q24" s="603" t="s">
         <v>336</v>
       </c>
-      <c r="R24" s="683"/>
+      <c r="R24" s="627"/>
       <c r="S24" s="534" t="s">
         <v>250</v>
       </c>
@@ -13181,8 +13185,8 @@
       <c r="AR31" s="508"/>
     </row>
     <row r="32" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="650"/>
-      <c r="B32" s="650"/>
+      <c r="A32" s="630"/>
+      <c r="B32" s="630"/>
       <c r="J32" s="572"/>
       <c r="K32" s="587"/>
       <c r="L32" s="581"/>
@@ -13652,7 +13656,7 @@
     </row>
     <row r="37" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B37" s="21">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D37" s="382">
         <v>1</v>
@@ -13757,6 +13761,15 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="Q24:R24"/>
+    <mergeCell ref="P4:P20"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="L2:L3"/>
+    <mergeCell ref="K2:K3"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="Q20:R20"/>
     <mergeCell ref="AM1:AO1"/>
     <mergeCell ref="X1:Y1"/>
     <mergeCell ref="AE1:AG1"/>
@@ -13768,15 +13781,6 @@
     <mergeCell ref="W2:W3"/>
     <mergeCell ref="T1:T3"/>
     <mergeCell ref="AK1:AK2"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="Q24:R24"/>
-    <mergeCell ref="P4:P20"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="L2:L3"/>
-    <mergeCell ref="K2:K3"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="Q20:R20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -13844,7 +13848,7 @@
       <c r="V1" s="603" t="s">
         <v>70</v>
       </c>
-      <c r="W1" s="683"/>
+      <c r="W1" s="627"/>
       <c r="X1" s="62" t="s">
         <v>101</v>
       </c>
@@ -13863,7 +13867,7 @@
       <c r="AC1" s="116" t="s">
         <v>190</v>
       </c>
-      <c r="AD1" s="759" t="s">
+      <c r="AD1" s="752" t="s">
         <v>212</v>
       </c>
       <c r="AE1" s="116" t="s">
@@ -13880,10 +13884,10 @@
       <c r="E2" s="39" t="s">
         <v>73</v>
       </c>
-      <c r="F2" s="790" t="s">
+      <c r="F2" s="751" t="s">
         <v>74</v>
       </c>
-      <c r="G2" s="747" t="s">
+      <c r="G2" s="779" t="s">
         <v>44</v>
       </c>
       <c r="H2" s="40" t="s">
@@ -13911,10 +13915,10 @@
       <c r="U2" s="60" t="s">
         <v>105</v>
       </c>
-      <c r="V2" s="726" t="s">
+      <c r="V2" s="719" t="s">
         <v>120</v>
       </c>
-      <c r="W2" s="727"/>
+      <c r="W2" s="720"/>
       <c r="X2" s="64" t="s">
         <v>109</v>
       </c>
@@ -13933,7 +13937,7 @@
       <c r="AC2" s="117" t="s">
         <v>98</v>
       </c>
-      <c r="AD2" s="760"/>
+      <c r="AD2" s="753"/>
       <c r="AE2" s="64" t="s">
         <v>98</v>
       </c>
@@ -13952,8 +13956,8 @@
       <c r="E3" s="39" t="s">
         <v>79</v>
       </c>
-      <c r="F3" s="630"/>
-      <c r="G3" s="748"/>
+      <c r="F3" s="679"/>
+      <c r="G3" s="780"/>
       <c r="H3" s="40" t="s">
         <v>80</v>
       </c>
@@ -13964,13 +13968,13 @@
         <v>81</v>
       </c>
       <c r="N3" s="44"/>
-      <c r="O3" s="757" t="s">
+      <c r="O3" s="789" t="s">
         <v>44</v>
       </c>
-      <c r="P3" s="778" t="s">
+      <c r="P3" s="771" t="s">
         <v>218</v>
       </c>
-      <c r="Q3" s="779"/>
+      <c r="Q3" s="772"/>
       <c r="S3" s="57" t="s">
         <v>219</v>
       </c>
@@ -13980,15 +13984,15 @@
       <c r="W3" s="59" t="s">
         <v>104</v>
       </c>
-      <c r="AD3" s="760"/>
+      <c r="AD3" s="753"/>
     </row>
     <row r="4" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G4" s="748"/>
+      <c r="G4" s="780"/>
       <c r="H4" s="6"/>
       <c r="L4" s="687" t="s">
         <v>82</v>
       </c>
-      <c r="O4" s="758"/>
+      <c r="O4" s="790"/>
       <c r="T4" s="55" t="s">
         <v>97</v>
       </c>
@@ -14002,8 +14006,8 @@
         <v>194</v>
       </c>
       <c r="Z4" s="605"/>
-      <c r="AA4" s="683"/>
-      <c r="AD4" s="760"/>
+      <c r="AA4" s="627"/>
+      <c r="AD4" s="753"/>
     </row>
     <row r="5" spans="1:31" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" s="52" t="s">
@@ -14018,21 +14022,21 @@
       <c r="F5" s="66" t="s">
         <v>84</v>
       </c>
-      <c r="G5" s="748"/>
+      <c r="G5" s="780"/>
       <c r="H5" s="46" t="s">
         <v>75</v>
       </c>
-      <c r="K5" s="765" t="s">
+      <c r="K5" s="758" t="s">
         <v>216</v>
       </c>
-      <c r="L5" s="780"/>
+      <c r="L5" s="773"/>
       <c r="M5" s="2" t="s">
         <v>214</v>
       </c>
       <c r="N5" s="61" t="s">
         <v>213</v>
       </c>
-      <c r="O5" s="758"/>
+      <c r="O5" s="790"/>
       <c r="P5" s="108" t="s">
         <v>215</v>
       </c>
@@ -14048,11 +14052,11 @@
       <c r="U5" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="Y5" s="768" t="s">
+      <c r="Y5" s="761" t="s">
         <v>283</v>
       </c>
-      <c r="Z5" s="769"/>
-      <c r="AD5" s="760"/>
+      <c r="Z5" s="762"/>
+      <c r="AD5" s="753"/>
     </row>
     <row r="6" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C6" s="109"/>
@@ -14062,16 +14066,16 @@
       <c r="E6" s="45" t="s">
         <v>85</v>
       </c>
-      <c r="G6" s="748"/>
+      <c r="G6" s="780"/>
       <c r="H6" s="46" t="s">
         <v>80</v>
       </c>
       <c r="I6" s="23">
         <v>15</v>
       </c>
-      <c r="K6" s="766"/>
-      <c r="L6" s="780"/>
-      <c r="O6" s="758"/>
+      <c r="K6" s="759"/>
+      <c r="L6" s="773"/>
+      <c r="O6" s="790"/>
       <c r="T6" s="2" t="s">
         <v>100</v>
       </c>
@@ -14081,23 +14085,23 @@
       <c r="V6" s="21">
         <v>-1</v>
       </c>
-      <c r="AD6" s="760"/>
+      <c r="AD6" s="753"/>
     </row>
     <row r="7" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C7" s="110"/>
-      <c r="G7" s="748"/>
+      <c r="G7" s="780"/>
       <c r="H7" s="6"/>
-      <c r="K7" s="766"/>
-      <c r="L7" s="780"/>
+      <c r="K7" s="759"/>
+      <c r="L7" s="773"/>
       <c r="N7" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="O7" s="758"/>
+      <c r="O7" s="790"/>
       <c r="P7" s="73"/>
       <c r="U7" s="104" t="s">
         <v>20</v>
       </c>
-      <c r="AD7" s="760"/>
+      <c r="AD7" s="753"/>
     </row>
     <row r="8" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C8" s="130"/>
@@ -14110,7 +14114,7 @@
       <c r="F8" s="66" t="s">
         <v>86</v>
       </c>
-      <c r="G8" s="748"/>
+      <c r="G8" s="780"/>
       <c r="H8" s="50" t="s">
         <v>75</v>
       </c>
@@ -14120,41 +14124,41 @@
       <c r="J8" s="111">
         <v>115</v>
       </c>
-      <c r="K8" s="766"/>
-      <c r="L8" s="780"/>
-      <c r="O8" s="758"/>
+      <c r="K8" s="759"/>
+      <c r="L8" s="773"/>
+      <c r="O8" s="790"/>
       <c r="P8" s="49"/>
-      <c r="S8" s="762" t="s">
+      <c r="S8" s="755" t="s">
         <v>211</v>
       </c>
-      <c r="T8" s="763"/>
-      <c r="U8" s="763"/>
-      <c r="V8" s="763"/>
-      <c r="W8" s="763"/>
-      <c r="X8" s="763"/>
-      <c r="Y8" s="763"/>
-      <c r="Z8" s="763"/>
-      <c r="AA8" s="763"/>
-      <c r="AB8" s="763"/>
-      <c r="AC8" s="764"/>
-      <c r="AD8" s="760"/>
+      <c r="T8" s="756"/>
+      <c r="U8" s="756"/>
+      <c r="V8" s="756"/>
+      <c r="W8" s="756"/>
+      <c r="X8" s="756"/>
+      <c r="Y8" s="756"/>
+      <c r="Z8" s="756"/>
+      <c r="AA8" s="756"/>
+      <c r="AB8" s="756"/>
+      <c r="AC8" s="757"/>
+      <c r="AD8" s="753"/>
     </row>
     <row r="9" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="784"/>
-      <c r="G9" s="748"/>
+      <c r="C9" s="745"/>
+      <c r="G9" s="780"/>
       <c r="H9" s="6"/>
-      <c r="K9" s="766"/>
-      <c r="L9" s="751" t="s">
+      <c r="K9" s="759"/>
+      <c r="L9" s="783" t="s">
         <v>217</v>
       </c>
-      <c r="M9" s="752"/>
-      <c r="N9" s="753"/>
-      <c r="O9" s="758"/>
+      <c r="M9" s="784"/>
+      <c r="N9" s="785"/>
+      <c r="O9" s="790"/>
       <c r="P9" s="75"/>
-      <c r="AD9" s="760"/>
+      <c r="AD9" s="753"/>
     </row>
     <row r="10" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="785"/>
+      <c r="C10" s="746"/>
       <c r="D10" s="23"/>
       <c r="E10" s="45" t="s">
         <v>87</v>
@@ -14162,7 +14166,7 @@
       <c r="F10" s="66" t="s">
         <v>88</v>
       </c>
-      <c r="G10" s="748"/>
+      <c r="G10" s="780"/>
       <c r="H10" s="51"/>
       <c r="I10" s="21" t="s">
         <v>80</v>
@@ -14170,33 +14174,33 @@
       <c r="J10" s="3">
         <v>15</v>
       </c>
-      <c r="K10" s="766"/>
-      <c r="M10" s="787" t="s">
+      <c r="K10" s="759"/>
+      <c r="M10" s="748" t="s">
         <v>89</v>
       </c>
-      <c r="N10" s="788"/>
-      <c r="O10" s="788"/>
-      <c r="P10" s="788"/>
-      <c r="Q10" s="788"/>
-      <c r="R10" s="788"/>
-      <c r="S10" s="788"/>
-      <c r="T10" s="788"/>
-      <c r="U10" s="788"/>
-      <c r="V10" s="788"/>
-      <c r="W10" s="788"/>
-      <c r="X10" s="788"/>
-      <c r="Y10" s="788"/>
-      <c r="Z10" s="788"/>
-      <c r="AA10" s="788"/>
-      <c r="AB10" s="788"/>
-      <c r="AC10" s="789"/>
-      <c r="AD10" s="760"/>
+      <c r="N10" s="749"/>
+      <c r="O10" s="749"/>
+      <c r="P10" s="749"/>
+      <c r="Q10" s="749"/>
+      <c r="R10" s="749"/>
+      <c r="S10" s="749"/>
+      <c r="T10" s="749"/>
+      <c r="U10" s="749"/>
+      <c r="V10" s="749"/>
+      <c r="W10" s="749"/>
+      <c r="X10" s="749"/>
+      <c r="Y10" s="749"/>
+      <c r="Z10" s="749"/>
+      <c r="AA10" s="749"/>
+      <c r="AB10" s="749"/>
+      <c r="AC10" s="750"/>
+      <c r="AD10" s="753"/>
     </row>
     <row r="11" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="786"/>
-      <c r="G11" s="748"/>
+      <c r="C11" s="747"/>
+      <c r="G11" s="780"/>
       <c r="H11" s="6"/>
-      <c r="K11" s="766"/>
+      <c r="K11" s="759"/>
       <c r="R11" s="52" t="s">
         <v>44</v>
       </c>
@@ -14204,17 +14208,17 @@
       <c r="Y11" s="68" t="s">
         <v>120</v>
       </c>
-      <c r="Z11" s="776" t="s">
+      <c r="Z11" s="769" t="s">
         <v>120</v>
       </c>
-      <c r="AA11" s="777"/>
+      <c r="AA11" s="770"/>
       <c r="AB11" s="52" t="s">
         <v>44</v>
       </c>
       <c r="AC11" s="118" t="s">
         <v>120</v>
       </c>
-      <c r="AD11" s="760"/>
+      <c r="AD11" s="753"/>
     </row>
     <row r="12" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C12" s="129"/>
@@ -14227,7 +14231,7 @@
       <c r="F12" s="66" t="s">
         <v>91</v>
       </c>
-      <c r="G12" s="748"/>
+      <c r="G12" s="780"/>
       <c r="H12" s="128"/>
       <c r="I12" s="19" t="s">
         <v>80</v>
@@ -14235,8 +14239,8 @@
       <c r="J12" s="3">
         <v>15</v>
       </c>
-      <c r="K12" s="766"/>
-      <c r="L12" s="781" t="s">
+      <c r="K12" s="759"/>
+      <c r="L12" s="774" t="s">
         <v>92</v>
       </c>
       <c r="M12" s="21" t="s">
@@ -14267,25 +14271,25 @@
         <v>115</v>
       </c>
       <c r="Y12" s="6"/>
-      <c r="AA12" s="770" t="s">
+      <c r="AA12" s="763" t="s">
         <v>125</v>
       </c>
-      <c r="AB12" s="771"/>
+      <c r="AB12" s="764"/>
       <c r="AC12" s="21" t="s">
         <v>231</v>
       </c>
-      <c r="AD12" s="760"/>
+      <c r="AD12" s="753"/>
     </row>
     <row r="13" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="784"/>
-      <c r="G13" s="748"/>
-      <c r="K13" s="766"/>
-      <c r="L13" s="782"/>
+      <c r="C13" s="745"/>
+      <c r="G13" s="780"/>
+      <c r="K13" s="759"/>
+      <c r="L13" s="775"/>
       <c r="M13" s="47"/>
-      <c r="Q13" s="750" t="s">
+      <c r="Q13" s="782" t="s">
         <v>209</v>
       </c>
-      <c r="R13" s="639"/>
+      <c r="R13" s="644"/>
       <c r="S13" s="599"/>
       <c r="T13" s="6"/>
       <c r="U13" s="96" t="s">
@@ -14294,17 +14298,17 @@
       <c r="X13" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="AA13" s="772"/>
-      <c r="AB13" s="773"/>
-      <c r="AD13" s="760"/>
+      <c r="AA13" s="765"/>
+      <c r="AB13" s="766"/>
+      <c r="AD13" s="753"/>
     </row>
     <row r="14" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
         <v>333</v>
       </c>
-      <c r="C14" s="786"/>
+      <c r="C14" s="747"/>
       <c r="D14" s="23"/>
-      <c r="G14" s="748"/>
+      <c r="G14" s="780"/>
       <c r="H14" s="125"/>
       <c r="I14" s="99" t="s">
         <v>44</v>
@@ -14312,8 +14316,8 @@
       <c r="J14" s="111">
         <v>115</v>
       </c>
-      <c r="K14" s="766"/>
-      <c r="L14" s="782"/>
+      <c r="K14" s="759"/>
+      <c r="L14" s="775"/>
       <c r="M14" s="21" t="s">
         <v>110</v>
       </c>
@@ -14334,9 +14338,9 @@
       <c r="Y14" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="AA14" s="772"/>
-      <c r="AB14" s="773"/>
-      <c r="AD14" s="760"/>
+      <c r="AA14" s="765"/>
+      <c r="AB14" s="766"/>
+      <c r="AD14" s="753"/>
     </row>
     <row r="15" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C15" s="130" t="s">
@@ -14351,19 +14355,19 @@
       <c r="F15" s="66" t="s">
         <v>93</v>
       </c>
-      <c r="G15" s="748"/>
+      <c r="G15" s="780"/>
       <c r="H15" s="2" t="s">
         <v>80</v>
       </c>
       <c r="I15" s="53" t="s">
         <v>80</v>
       </c>
-      <c r="K15" s="766"/>
-      <c r="L15" s="783"/>
-      <c r="Q15" s="750" t="s">
+      <c r="K15" s="759"/>
+      <c r="L15" s="776"/>
+      <c r="Q15" s="782" t="s">
         <v>210</v>
       </c>
-      <c r="R15" s="639"/>
+      <c r="R15" s="644"/>
       <c r="S15" s="599"/>
       <c r="T15" s="6"/>
       <c r="V15" s="68" t="s">
@@ -14372,14 +14376,14 @@
       <c r="X15" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="AA15" s="772"/>
-      <c r="AB15" s="773"/>
-      <c r="AD15" s="760"/>
+      <c r="AA15" s="765"/>
+      <c r="AB15" s="766"/>
+      <c r="AD15" s="753"/>
     </row>
     <row r="16" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C16" s="132"/>
-      <c r="G16" s="748"/>
-      <c r="K16" s="766"/>
+      <c r="G16" s="780"/>
+      <c r="K16" s="759"/>
       <c r="N16" s="47"/>
       <c r="O16" s="61" t="s">
         <v>108</v>
@@ -14398,24 +14402,24 @@
       <c r="Z16" s="76" t="s">
         <v>126</v>
       </c>
-      <c r="AA16" s="772"/>
-      <c r="AB16" s="773"/>
-      <c r="AD16" s="760"/>
+      <c r="AA16" s="765"/>
+      <c r="AB16" s="766"/>
+      <c r="AD16" s="753"/>
     </row>
     <row r="17" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C17" s="109"/>
       <c r="E17" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="F17" s="745" t="s">
+      <c r="F17" s="777" t="s">
         <v>95</v>
       </c>
-      <c r="G17" s="748"/>
+      <c r="G17" s="780"/>
       <c r="H17" s="54"/>
       <c r="I17" s="133" t="s">
         <v>80</v>
       </c>
-      <c r="K17" s="766"/>
+      <c r="K17" s="759"/>
       <c r="S17" s="599"/>
       <c r="V17" s="68" t="s">
         <v>44</v>
@@ -14423,9 +14427,9 @@
       <c r="X17" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="AA17" s="772"/>
-      <c r="AB17" s="773"/>
-      <c r="AD17" s="760"/>
+      <c r="AA17" s="765"/>
+      <c r="AB17" s="766"/>
+      <c r="AD17" s="753"/>
     </row>
     <row r="18" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C18" s="130"/>
@@ -14435,15 +14439,15 @@
       <c r="E18" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="F18" s="746"/>
-      <c r="G18" s="748"/>
+      <c r="F18" s="778"/>
+      <c r="G18" s="780"/>
       <c r="H18" s="108" t="s">
         <v>75</v>
       </c>
       <c r="I18" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="K18" s="766"/>
+      <c r="K18" s="759"/>
       <c r="O18" s="64" t="s">
         <v>114</v>
       </c>
@@ -14454,39 +14458,42 @@
       <c r="X18" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="AA18" s="774"/>
-      <c r="AB18" s="775"/>
-      <c r="AD18" s="760"/>
+      <c r="AA18" s="767"/>
+      <c r="AB18" s="768"/>
+      <c r="AD18" s="753"/>
     </row>
     <row r="19" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F19" s="64" t="s">
         <v>208</v>
       </c>
-      <c r="G19" s="749"/>
-      <c r="K19" s="767"/>
+      <c r="G19" s="781"/>
+      <c r="K19" s="760"/>
       <c r="Q19" s="68" t="s">
         <v>44</v>
       </c>
-      <c r="R19" s="754" t="s">
+      <c r="R19" s="786" t="s">
         <v>123</v>
       </c>
-      <c r="S19" s="755"/>
-      <c r="T19" s="756"/>
+      <c r="S19" s="787"/>
+      <c r="T19" s="788"/>
       <c r="V19" s="77" t="s">
         <v>114</v>
       </c>
       <c r="Y19" s="19" t="s">
         <v>124</v>
       </c>
-      <c r="AD19" s="761"/>
+      <c r="AD19" s="754"/>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="V2:W2"/>
-    <mergeCell ref="M10:AC10"/>
-    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="G2:G19"/>
+    <mergeCell ref="Q13:R13"/>
+    <mergeCell ref="Q15:R15"/>
+    <mergeCell ref="L9:N9"/>
+    <mergeCell ref="R19:T19"/>
+    <mergeCell ref="S12:S18"/>
+    <mergeCell ref="O3:O9"/>
     <mergeCell ref="AD1:AD19"/>
     <mergeCell ref="S8:AC8"/>
     <mergeCell ref="K5:K19"/>
@@ -14498,14 +14505,11 @@
     <mergeCell ref="P3:Q3"/>
     <mergeCell ref="L4:L8"/>
     <mergeCell ref="L12:L15"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="G2:G19"/>
-    <mergeCell ref="Q13:R13"/>
-    <mergeCell ref="Q15:R15"/>
-    <mergeCell ref="L9:N9"/>
-    <mergeCell ref="R19:T19"/>
-    <mergeCell ref="S12:S18"/>
-    <mergeCell ref="O3:O9"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="V2:W2"/>
+    <mergeCell ref="M10:AC10"/>
+    <mergeCell ref="F2:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Rw Usage Updates_15:40 PM
Rw Usage Updates_15:40 PM
</commit_message>
<xml_diff>
--- a/System_2.1.9.xlsx
+++ b/System_2.1.9.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Work_For_\Work\Running AppS\System_Work_RW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67C73566-3590-4916-9A82-E7CEBAA6AFF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE3A7134-B7BB-4CEE-A7A8-0E6F0C59FBD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BoardRW" sheetId="1" r:id="rId1"/>
@@ -1907,7 +1907,7 @@
     <t>Rbangla</t>
   </si>
   <si>
-    <t>10 F INCapacity</t>
+    <t>2 F INCapacity</t>
   </si>
 </sst>
 </file>
@@ -5871,8 +5871,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:X28"/>
   <sheetViews>
-    <sheetView topLeftCell="C9" workbookViewId="0">
-      <selection activeCell="Y19" sqref="Y19"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="Y20" sqref="Y20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6055,7 +6055,7 @@
         <v>225</v>
       </c>
       <c r="V5" s="24">
-        <v>7140</v>
+        <v>7200</v>
       </c>
     </row>
     <row r="6" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6268,7 +6268,7 @@
         <v>224</v>
       </c>
       <c r="V11" s="64">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="12" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8951,7 +8951,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB54FD83-008D-4F8B-87AC-83E7F70047CB}">
   <dimension ref="A1:AL31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+    <sheetView topLeftCell="N12" workbookViewId="0">
       <selection activeCell="AH21" sqref="AH21"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Rw Updates _ 22ErrorFix_Usage_20:30PM
Rw Updates _ 22ErrorFix_Usage_20:30PM

Boat Updates:-
InCapacity - [2+15+3] , NodeW - [-3] , BirdW - [6] , FuelW - [19]

Host - [9 + 1] ,
</commit_message>
<xml_diff>
--- a/System_2.1.9.xlsx
+++ b/System_2.1.9.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Work_For_\Work\Running AppS\System_Work_RW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56C49918-BCBD-4F56-90F6-65A49BD885DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD6A46D6-CD2E-4A8A-880E-EB45FADC4C3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BoardRW" sheetId="1" r:id="rId1"/>
@@ -1913,7 +1913,7 @@
     <t>15F</t>
   </si>
   <si>
-    <t>3F</t>
+    <t>3M 3F</t>
   </si>
 </sst>
 </file>
@@ -5036,6 +5036,186 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="73" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="27" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="27" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="49" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="49" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="49" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="19" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -5048,12 +5228,6 @@
     <xf numFmtId="0" fontId="17" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -5065,12 +5239,6 @@
     </xf>
     <xf numFmtId="0" fontId="38" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
@@ -5093,190 +5261,61 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="27" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="27" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="27" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="13" fillId="27" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="49" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="49" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="49" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="73" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="13" fillId="27" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="13" fillId="27" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="36" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5318,43 +5357,25 @@
     <xf numFmtId="0" fontId="39" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="27" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="27" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="13" fillId="27" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="13" fillId="27" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="35" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="35" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="35" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="43" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5423,46 +5444,46 @@
     <xf numFmtId="14" fontId="5" fillId="14" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="35" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="35" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="35" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5540,46 +5561,25 @@
     <xf numFmtId="0" fontId="3" fillId="21" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -5878,7 +5878,7 @@
   <dimension ref="B1:X28"/>
   <sheetViews>
     <sheetView topLeftCell="C9" workbookViewId="0">
-      <selection activeCell="X26" sqref="X26"/>
+      <selection activeCell="X13" sqref="X13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6916,7 +6916,7 @@
       <c r="H1" s="97" t="s">
         <v>343</v>
       </c>
-      <c r="I1" s="613" t="s">
+      <c r="I1" s="659" t="s">
         <v>369</v>
       </c>
       <c r="J1" s="2" t="s">
@@ -6952,7 +6952,7 @@
       <c r="X1" s="430" t="s">
         <v>155</v>
       </c>
-      <c r="Y1" s="657" t="s">
+      <c r="Y1" s="653" t="s">
         <v>529</v>
       </c>
       <c r="Z1" s="406">
@@ -6977,7 +6977,7 @@
         <v>498</v>
       </c>
       <c r="AM1" s="402"/>
-      <c r="AN1" s="640"/>
+      <c r="AN1" s="635"/>
       <c r="AO1" s="338" t="s">
         <v>469</v>
       </c>
@@ -6986,23 +6986,23 @@
       </c>
     </row>
     <row r="2" spans="1:43" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="666">
+      <c r="A2" s="617">
         <f ca="1">TODAY()</f>
         <v>45285</v>
       </c>
-      <c r="B2" s="668" t="s">
+      <c r="B2" s="619" t="s">
         <v>370</v>
       </c>
-      <c r="C2" s="645" t="s">
+      <c r="C2" s="615" t="s">
         <v>357</v>
       </c>
-      <c r="D2" s="670" t="s">
+      <c r="D2" s="621" t="s">
         <v>355</v>
       </c>
-      <c r="E2" s="609" t="s">
+      <c r="E2" s="669" t="s">
         <v>64</v>
       </c>
-      <c r="F2" s="619" t="s">
+      <c r="F2" s="640" t="s">
         <v>102</v>
       </c>
       <c r="G2" s="393" t="s">
@@ -7011,31 +7011,31 @@
       <c r="H2" s="80" t="s">
         <v>33</v>
       </c>
-      <c r="I2" s="614"/>
+      <c r="I2" s="660"/>
       <c r="J2" s="81" t="s">
         <v>76</v>
       </c>
-      <c r="K2" s="611" t="s">
+      <c r="K2" s="671" t="s">
         <v>342</v>
       </c>
-      <c r="L2" s="612"/>
-      <c r="M2" s="619" t="s">
+      <c r="L2" s="672"/>
+      <c r="M2" s="640" t="s">
         <v>102</v>
       </c>
       <c r="N2" s="69" t="s">
         <v>28</v>
       </c>
-      <c r="O2" s="649" t="s">
+      <c r="O2" s="644" t="s">
         <v>102</v>
       </c>
       <c r="P2" s="85" t="s">
         <v>147</v>
       </c>
-      <c r="Q2" s="645" t="s">
+      <c r="Q2" s="615" t="s">
         <v>143</v>
       </c>
       <c r="R2" s="598"/>
-      <c r="S2" s="634" t="s">
+      <c r="S2" s="657" t="s">
         <v>148</v>
       </c>
       <c r="T2" s="89"/>
@@ -7045,7 +7045,7 @@
       <c r="X2" s="431" t="s">
         <v>156</v>
       </c>
-      <c r="Y2" s="658"/>
+      <c r="Y2" s="654"/>
       <c r="Z2" s="407">
         <v>1</v>
       </c>
@@ -7068,15 +7068,15 @@
         <v>463</v>
       </c>
       <c r="AM2" s="428"/>
-      <c r="AN2" s="641"/>
+      <c r="AN2" s="636"/>
     </row>
     <row r="3" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="667"/>
-      <c r="B3" s="669"/>
-      <c r="C3" s="646"/>
-      <c r="D3" s="671"/>
-      <c r="E3" s="610"/>
-      <c r="F3" s="620"/>
+      <c r="A3" s="618"/>
+      <c r="B3" s="620"/>
+      <c r="C3" s="616"/>
+      <c r="D3" s="622"/>
+      <c r="E3" s="670"/>
+      <c r="F3" s="641"/>
       <c r="G3" s="394" t="s">
         <v>28</v>
       </c>
@@ -7095,17 +7095,17 @@
       <c r="L3" s="201" t="s">
         <v>107</v>
       </c>
-      <c r="M3" s="620"/>
+      <c r="M3" s="641"/>
       <c r="N3" s="69" t="s">
         <v>146</v>
       </c>
-      <c r="O3" s="650"/>
+      <c r="O3" s="645"/>
       <c r="P3" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="Q3" s="646"/>
+      <c r="Q3" s="616"/>
       <c r="R3" s="600"/>
-      <c r="S3" s="636"/>
+      <c r="S3" s="658"/>
       <c r="T3" s="89"/>
       <c r="U3" s="124"/>
       <c r="V3" s="120"/>
@@ -7113,7 +7113,7 @@
       <c r="X3" s="431" t="s">
         <v>157</v>
       </c>
-      <c r="Y3" s="658"/>
+      <c r="Y3" s="654"/>
       <c r="Z3" s="408">
         <v>1</v>
       </c>
@@ -7122,7 +7122,7 @@
       <c r="AC3" s="100" t="s">
         <v>480</v>
       </c>
-      <c r="AD3" s="631" t="s">
+      <c r="AD3" s="656" t="s">
         <v>455</v>
       </c>
       <c r="AE3" s="257"/>
@@ -7134,16 +7134,16 @@
       <c r="AK3" s="257"/>
       <c r="AL3" s="16"/>
       <c r="AM3" s="428"/>
-      <c r="AN3" s="641"/>
+      <c r="AN3" s="636"/>
     </row>
     <row r="4" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="238" t="s">
         <v>183</v>
       </c>
-      <c r="B4" s="682" t="s">
+      <c r="B4" s="633" t="s">
         <v>373</v>
       </c>
-      <c r="C4" s="645" t="s">
+      <c r="C4" s="615" t="s">
         <v>154</v>
       </c>
       <c r="D4" s="347" t="s">
@@ -7152,7 +7152,7 @@
       <c r="E4" s="378">
         <v>2</v>
       </c>
-      <c r="F4" s="620"/>
+      <c r="F4" s="641"/>
       <c r="G4" s="381" t="s">
         <v>201</v>
       </c>
@@ -7169,11 +7169,11 @@
         <v>150</v>
       </c>
       <c r="L4" s="204"/>
-      <c r="M4" s="620"/>
+      <c r="M4" s="641"/>
       <c r="N4" s="174" t="s">
         <v>69</v>
       </c>
-      <c r="O4" s="650"/>
+      <c r="O4" s="645"/>
       <c r="P4" s="2" t="s">
         <v>191</v>
       </c>
@@ -7195,12 +7195,12 @@
       <c r="X4" s="431" t="s">
         <v>158</v>
       </c>
-      <c r="Y4" s="658"/>
+      <c r="Y4" s="654"/>
       <c r="Z4" s="409"/>
       <c r="AA4" s="307"/>
       <c r="AB4" s="209"/>
       <c r="AC4" s="16"/>
-      <c r="AD4" s="631"/>
+      <c r="AD4" s="656"/>
       <c r="AE4" s="257"/>
       <c r="AF4" s="257"/>
       <c r="AG4" s="16"/>
@@ -7210,37 +7210,37 @@
       <c r="AK4" s="257"/>
       <c r="AL4" s="16"/>
       <c r="AM4" s="428"/>
-      <c r="AN4" s="641"/>
+      <c r="AN4" s="636"/>
       <c r="AO4" s="338" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="613" t="s">
+      <c r="A5" s="659" t="s">
         <v>418</v>
       </c>
-      <c r="B5" s="683"/>
-      <c r="C5" s="646"/>
+      <c r="B5" s="634"/>
+      <c r="C5" s="616"/>
       <c r="D5" s="61" t="s">
         <v>153</v>
       </c>
       <c r="E5" s="379">
         <v>1</v>
       </c>
-      <c r="F5" s="620"/>
-      <c r="G5" s="674" t="s">
+      <c r="F5" s="641"/>
+      <c r="G5" s="625" t="s">
         <v>192</v>
       </c>
-      <c r="H5" s="674"/>
-      <c r="I5" s="674"/>
-      <c r="J5" s="674"/>
-      <c r="K5" s="674"/>
-      <c r="L5" s="675"/>
-      <c r="M5" s="620"/>
+      <c r="H5" s="625"/>
+      <c r="I5" s="625"/>
+      <c r="J5" s="625"/>
+      <c r="K5" s="625"/>
+      <c r="L5" s="626"/>
+      <c r="M5" s="641"/>
       <c r="N5" s="21">
         <v>8</v>
       </c>
-      <c r="O5" s="650"/>
+      <c r="O5" s="645"/>
       <c r="T5" s="89"/>
       <c r="U5" s="124"/>
       <c r="V5" s="120"/>
@@ -7248,7 +7248,7 @@
       <c r="X5" s="431" t="s">
         <v>159</v>
       </c>
-      <c r="Y5" s="658"/>
+      <c r="Y5" s="654"/>
       <c r="Z5" s="409">
         <v>1</v>
       </c>
@@ -7271,24 +7271,24 @@
       <c r="AK5" s="257"/>
       <c r="AL5" s="80"/>
       <c r="AM5" s="428"/>
-      <c r="AN5" s="641"/>
+      <c r="AN5" s="636"/>
     </row>
     <row r="6" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="614"/>
-      <c r="B6" s="680" t="s">
+      <c r="A6" s="660"/>
+      <c r="B6" s="631" t="s">
         <v>177</v>
       </c>
-      <c r="C6" s="628"/>
-      <c r="D6" s="629"/>
-      <c r="F6" s="620"/>
-      <c r="G6" s="676"/>
-      <c r="H6" s="676"/>
-      <c r="I6" s="676"/>
-      <c r="J6" s="676"/>
-      <c r="K6" s="676"/>
-      <c r="L6" s="677"/>
-      <c r="M6" s="620"/>
-      <c r="O6" s="650"/>
+      <c r="C6" s="661"/>
+      <c r="D6" s="662"/>
+      <c r="F6" s="641"/>
+      <c r="G6" s="627"/>
+      <c r="H6" s="627"/>
+      <c r="I6" s="627"/>
+      <c r="J6" s="627"/>
+      <c r="K6" s="627"/>
+      <c r="L6" s="628"/>
+      <c r="M6" s="641"/>
+      <c r="O6" s="645"/>
       <c r="T6" s="89"/>
       <c r="U6" s="124"/>
       <c r="V6" s="98" t="s">
@@ -7298,7 +7298,7 @@
       <c r="X6" s="431" t="s">
         <v>160</v>
       </c>
-      <c r="Y6" s="658"/>
+      <c r="Y6" s="654"/>
       <c r="Z6" s="407">
         <v>1</v>
       </c>
@@ -7312,16 +7312,16 @@
       <c r="AF6" s="257"/>
       <c r="AG6" s="257"/>
       <c r="AH6" s="257"/>
-      <c r="AI6" s="630"/>
+      <c r="AI6" s="650"/>
       <c r="AJ6" s="441" t="s">
         <v>458</v>
       </c>
-      <c r="AK6" s="630" t="s">
+      <c r="AK6" s="650" t="s">
         <v>251</v>
       </c>
       <c r="AL6" s="257"/>
       <c r="AM6" s="428"/>
-      <c r="AN6" s="641"/>
+      <c r="AN6" s="636"/>
       <c r="AO6" s="338" t="s">
         <v>470</v>
       </c>
@@ -7330,7 +7330,7 @@
       <c r="A7" s="232" t="s">
         <v>572</v>
       </c>
-      <c r="B7" s="681"/>
+      <c r="B7" s="632"/>
       <c r="C7" s="202" t="s">
         <v>374</v>
       </c>
@@ -7340,7 +7340,7 @@
       <c r="E7" s="265">
         <v>3</v>
       </c>
-      <c r="F7" s="620"/>
+      <c r="F7" s="641"/>
       <c r="G7" s="395">
         <v>0</v>
       </c>
@@ -7359,8 +7359,8 @@
       <c r="L7" s="212">
         <v>0</v>
       </c>
-      <c r="M7" s="620"/>
-      <c r="O7" s="650"/>
+      <c r="M7" s="641"/>
+      <c r="O7" s="645"/>
       <c r="R7" s="99" t="s">
         <v>44</v>
       </c>
@@ -7374,7 +7374,7 @@
       <c r="X7" s="431" t="s">
         <v>161</v>
       </c>
-      <c r="Y7" s="658"/>
+      <c r="Y7" s="654"/>
       <c r="Z7" s="407">
         <v>1</v>
       </c>
@@ -7384,18 +7384,18 @@
       <c r="AD7" s="16"/>
       <c r="AE7" s="257"/>
       <c r="AF7" s="257"/>
-      <c r="AG7" s="631" t="s">
+      <c r="AG7" s="656" t="s">
         <v>454</v>
       </c>
       <c r="AH7" s="257"/>
-      <c r="AI7" s="630"/>
+      <c r="AI7" s="650"/>
       <c r="AJ7" s="257"/>
-      <c r="AK7" s="630"/>
+      <c r="AK7" s="650"/>
       <c r="AL7" s="80" t="s">
         <v>496</v>
       </c>
       <c r="AM7" s="428"/>
-      <c r="AN7" s="641"/>
+      <c r="AN7" s="636"/>
       <c r="AP7" s="76" t="s">
         <v>471</v>
       </c>
@@ -7412,27 +7412,27 @@
         <f>SUM(G7:N9)</f>
         <v>15</v>
       </c>
-      <c r="F8" s="620"/>
-      <c r="G8" s="675">
-        <v>0</v>
-      </c>
-      <c r="H8" s="672" t="s">
+      <c r="F8" s="641"/>
+      <c r="G8" s="626">
+        <v>0</v>
+      </c>
+      <c r="H8" s="623" t="s">
         <v>104</v>
       </c>
       <c r="I8" s="598">
         <v>0</v>
       </c>
-      <c r="J8" s="672" t="s">
+      <c r="J8" s="623" t="s">
         <v>104</v>
       </c>
-      <c r="K8" s="678"/>
-      <c r="L8" s="632"/>
-      <c r="M8" s="647"/>
-      <c r="N8" s="637">
+      <c r="K8" s="629"/>
+      <c r="L8" s="663"/>
+      <c r="M8" s="642"/>
+      <c r="N8" s="666">
         <f>N5+N11</f>
         <v>15</v>
       </c>
-      <c r="O8" s="650"/>
+      <c r="O8" s="645"/>
       <c r="T8" s="103" t="s">
         <v>44</v>
       </c>
@@ -7442,7 +7442,7 @@
       <c r="X8" s="431" t="s">
         <v>162</v>
       </c>
-      <c r="Y8" s="658"/>
+      <c r="Y8" s="654"/>
       <c r="Z8" s="409"/>
       <c r="AA8" s="307"/>
       <c r="AB8" s="209"/>
@@ -7450,14 +7450,14 @@
       <c r="AD8" s="16"/>
       <c r="AE8" s="257"/>
       <c r="AF8" s="257"/>
-      <c r="AG8" s="631"/>
+      <c r="AG8" s="656"/>
       <c r="AH8" s="257"/>
-      <c r="AI8" s="630"/>
+      <c r="AI8" s="650"/>
       <c r="AJ8" s="257"/>
       <c r="AK8" s="257"/>
       <c r="AL8" s="257"/>
       <c r="AM8" s="428"/>
-      <c r="AN8" s="641"/>
+      <c r="AN8" s="636"/>
     </row>
     <row r="9" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="232" t="s">
@@ -7472,17 +7472,17 @@
       <c r="D9" s="348" t="s">
         <v>281</v>
       </c>
-      <c r="F9" s="620"/>
-      <c r="G9" s="677"/>
-      <c r="H9" s="673"/>
+      <c r="F9" s="641"/>
+      <c r="G9" s="628"/>
+      <c r="H9" s="624"/>
       <c r="I9" s="600"/>
-      <c r="J9" s="673"/>
-      <c r="K9" s="679"/>
-      <c r="L9" s="633"/>
-      <c r="M9" s="648"/>
-      <c r="N9" s="638"/>
-      <c r="O9" s="651"/>
-      <c r="S9" s="634" t="s">
+      <c r="J9" s="624"/>
+      <c r="K9" s="630"/>
+      <c r="L9" s="664"/>
+      <c r="M9" s="643"/>
+      <c r="N9" s="667"/>
+      <c r="O9" s="646"/>
+      <c r="S9" s="657" t="s">
         <v>61</v>
       </c>
       <c r="T9" s="89"/>
@@ -7494,7 +7494,7 @@
       <c r="X9" s="431" t="s">
         <v>163</v>
       </c>
-      <c r="Y9" s="658"/>
+      <c r="Y9" s="654"/>
       <c r="Z9" s="410"/>
       <c r="AA9" s="307"/>
       <c r="AB9" s="209"/>
@@ -7504,16 +7504,16 @@
       </c>
       <c r="AE9" s="257"/>
       <c r="AF9" s="257"/>
-      <c r="AG9" s="631"/>
+      <c r="AG9" s="656"/>
       <c r="AH9" s="257"/>
-      <c r="AI9" s="630"/>
+      <c r="AI9" s="650"/>
       <c r="AJ9" s="80"/>
-      <c r="AK9" s="630" t="s">
+      <c r="AK9" s="650" t="s">
         <v>251</v>
       </c>
       <c r="AL9" s="257"/>
       <c r="AM9" s="428"/>
-      <c r="AN9" s="641"/>
+      <c r="AN9" s="636"/>
       <c r="AP9" s="2" t="s">
         <v>508</v>
       </c>
@@ -7530,20 +7530,20 @@
         <f>Boat!W8</f>
         <v>39</v>
       </c>
-      <c r="F10" s="620"/>
+      <c r="F10" s="641"/>
       <c r="N10" s="418" t="s">
         <v>396</v>
       </c>
-      <c r="O10" s="622" t="s">
+      <c r="O10" s="678" t="s">
         <v>102</v>
       </c>
-      <c r="P10" s="652" t="s">
+      <c r="P10" s="647" t="s">
         <v>400</v>
       </c>
       <c r="R10" s="74" t="s">
         <v>44</v>
       </c>
-      <c r="S10" s="635"/>
+      <c r="S10" s="665"/>
       <c r="T10" s="89"/>
       <c r="U10" s="123" t="s">
         <v>176</v>
@@ -7555,7 +7555,7 @@
       <c r="X10" s="431" t="s">
         <v>164</v>
       </c>
-      <c r="Y10" s="658"/>
+      <c r="Y10" s="654"/>
       <c r="Z10" s="409">
         <v>0</v>
       </c>
@@ -7573,16 +7573,16 @@
       <c r="AF10" s="238" t="s">
         <v>311</v>
       </c>
-      <c r="AG10" s="631"/>
+      <c r="AG10" s="656"/>
       <c r="AH10" s="80"/>
-      <c r="AI10" s="630"/>
+      <c r="AI10" s="650"/>
       <c r="AJ10" s="257"/>
-      <c r="AK10" s="630"/>
+      <c r="AK10" s="650"/>
       <c r="AL10" s="257"/>
       <c r="AM10" s="442" t="s">
         <v>318</v>
       </c>
-      <c r="AN10" s="641"/>
+      <c r="AN10" s="636"/>
       <c r="AO10" s="204" t="s">
         <v>94</v>
       </c>
@@ -7600,18 +7600,18 @@
       <c r="D11" s="170" t="s">
         <v>355</v>
       </c>
-      <c r="F11" s="620"/>
+      <c r="F11" s="641"/>
       <c r="M11" s="6"/>
       <c r="N11" s="117">
         <v>7</v>
       </c>
-      <c r="O11" s="623"/>
-      <c r="P11" s="653"/>
+      <c r="O11" s="679"/>
+      <c r="P11" s="648"/>
       <c r="Q11" s="65"/>
       <c r="R11" s="120" t="s">
         <v>220</v>
       </c>
-      <c r="S11" s="635"/>
+      <c r="S11" s="665"/>
       <c r="T11" s="102" t="s">
         <v>44</v>
       </c>
@@ -7621,7 +7621,7 @@
       <c r="X11" s="431" t="s">
         <v>165</v>
       </c>
-      <c r="Y11" s="658"/>
+      <c r="Y11" s="654"/>
       <c r="Z11" s="409"/>
       <c r="AA11" s="307">
         <v>1</v>
@@ -7635,14 +7635,14 @@
       <c r="AF11" s="257" t="s">
         <v>476</v>
       </c>
-      <c r="AG11" s="631"/>
+      <c r="AG11" s="656"/>
       <c r="AH11" s="257"/>
       <c r="AI11" s="70"/>
       <c r="AJ11" s="257"/>
       <c r="AK11" s="257"/>
       <c r="AL11" s="257"/>
       <c r="AM11" s="428"/>
-      <c r="AN11" s="641"/>
+      <c r="AN11" s="636"/>
       <c r="AP11" s="76" t="s">
         <v>484</v>
       </c>
@@ -7661,7 +7661,7 @@
       <c r="E12" s="224">
         <v>3</v>
       </c>
-      <c r="F12" s="620"/>
+      <c r="F12" s="641"/>
       <c r="G12" s="337" t="s">
         <v>400</v>
       </c>
@@ -7670,16 +7670,16 @@
       </c>
       <c r="I12" s="605"/>
       <c r="J12" s="605"/>
-      <c r="K12" s="627"/>
+      <c r="K12" s="683"/>
       <c r="L12" s="203"/>
       <c r="M12" s="203"/>
       <c r="N12" s="203"/>
-      <c r="O12" s="623"/>
-      <c r="P12" s="653"/>
+      <c r="O12" s="679"/>
+      <c r="P12" s="648"/>
       <c r="R12" s="122" t="s">
         <v>180</v>
       </c>
-      <c r="S12" s="636"/>
+      <c r="S12" s="658"/>
       <c r="T12" s="101" t="s">
         <v>44</v>
       </c>
@@ -7689,7 +7689,7 @@
       <c r="X12" s="431" t="s">
         <v>166</v>
       </c>
-      <c r="Y12" s="658"/>
+      <c r="Y12" s="654"/>
       <c r="Z12" s="407">
         <v>1</v>
       </c>
@@ -7700,16 +7700,16 @@
       <c r="AC12" s="100" t="s">
         <v>481</v>
       </c>
-      <c r="AD12" s="639" t="s">
+      <c r="AD12" s="668" t="s">
         <v>240</v>
       </c>
       <c r="AE12" s="441" t="s">
         <v>239</v>
       </c>
-      <c r="AF12" s="631" t="s">
+      <c r="AF12" s="656" t="s">
         <v>228</v>
       </c>
-      <c r="AG12" s="631"/>
+      <c r="AG12" s="656"/>
       <c r="AH12" s="238" t="s">
         <v>259</v>
       </c>
@@ -7719,10 +7719,10 @@
       <c r="AJ12" s="257"/>
       <c r="AK12" s="257"/>
       <c r="AL12" s="257"/>
-      <c r="AM12" s="655" t="s">
+      <c r="AM12" s="651" t="s">
         <v>249</v>
       </c>
-      <c r="AN12" s="641"/>
+      <c r="AN12" s="636"/>
       <c r="AO12" s="338" t="s">
         <v>96</v>
       </c>
@@ -7734,17 +7734,17 @@
       <c r="E13" s="448">
         <v>-3</v>
       </c>
-      <c r="F13" s="620"/>
+      <c r="F13" s="641"/>
       <c r="G13" s="605" t="s">
         <v>430</v>
       </c>
       <c r="H13" s="605"/>
       <c r="I13" s="605"/>
-      <c r="J13" s="627"/>
+      <c r="J13" s="683"/>
       <c r="M13" s="6"/>
       <c r="N13" s="6"/>
-      <c r="O13" s="623"/>
-      <c r="P13" s="654"/>
+      <c r="O13" s="679"/>
+      <c r="P13" s="649"/>
       <c r="T13" s="105" t="s">
         <v>44</v>
       </c>
@@ -7754,7 +7754,7 @@
       <c r="X13" s="431" t="s">
         <v>167</v>
       </c>
-      <c r="Y13" s="658"/>
+      <c r="Y13" s="654"/>
       <c r="Z13" s="407">
         <v>1</v>
       </c>
@@ -7765,8 +7765,8 @@
         <v>500</v>
       </c>
       <c r="AC13" s="16"/>
-      <c r="AD13" s="639"/>
-      <c r="AF13" s="631"/>
+      <c r="AD13" s="668"/>
+      <c r="AF13" s="656"/>
       <c r="AG13" s="80"/>
       <c r="AH13" s="238" t="s">
         <v>308</v>
@@ -7777,8 +7777,8 @@
       <c r="AJ13" s="80"/>
       <c r="AK13" s="257"/>
       <c r="AL13" s="257"/>
-      <c r="AM13" s="655"/>
-      <c r="AN13" s="641"/>
+      <c r="AM13" s="651"/>
+      <c r="AN13" s="636"/>
     </row>
     <row r="14" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="450"/>
@@ -7786,18 +7786,18 @@
       <c r="C14" s="459"/>
       <c r="D14" s="452"/>
       <c r="E14" s="453"/>
-      <c r="F14" s="620"/>
+      <c r="F14" s="641"/>
       <c r="G14" s="605" t="s">
         <v>429</v>
       </c>
       <c r="H14" s="605"/>
       <c r="I14" s="605"/>
-      <c r="J14" s="627"/>
+      <c r="J14" s="683"/>
       <c r="K14" s="2">
         <v>12</v>
       </c>
       <c r="N14" s="6"/>
-      <c r="O14" s="623"/>
+      <c r="O14" s="679"/>
       <c r="Q14" s="61" t="s">
         <v>533</v>
       </c>
@@ -7811,24 +7811,24 @@
       <c r="X14" s="431" t="s">
         <v>168</v>
       </c>
-      <c r="Y14" s="658"/>
+      <c r="Y14" s="654"/>
       <c r="Z14" s="407">
         <v>1</v>
       </c>
       <c r="AA14" s="307"/>
       <c r="AB14" s="209"/>
       <c r="AC14" s="16"/>
-      <c r="AD14" s="639"/>
+      <c r="AD14" s="668"/>
       <c r="AE14" s="257"/>
-      <c r="AF14" s="631"/>
+      <c r="AF14" s="656"/>
       <c r="AG14" s="257"/>
       <c r="AH14" s="257"/>
       <c r="AI14" s="70"/>
       <c r="AJ14" s="257"/>
       <c r="AK14" s="257"/>
       <c r="AL14" s="257"/>
-      <c r="AM14" s="655"/>
-      <c r="AN14" s="641"/>
+      <c r="AM14" s="651"/>
+      <c r="AN14" s="636"/>
     </row>
     <row r="15" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="449" t="s">
@@ -7837,8 +7837,8 @@
       <c r="C15" s="598" t="s">
         <v>373</v>
       </c>
-      <c r="F15" s="620"/>
-      <c r="O15" s="623"/>
+      <c r="F15" s="641"/>
+      <c r="O15" s="679"/>
       <c r="R15" s="99" t="s">
         <v>44</v>
       </c>
@@ -7851,7 +7851,7 @@
       <c r="X15" s="431" t="s">
         <v>169</v>
       </c>
-      <c r="Y15" s="658"/>
+      <c r="Y15" s="654"/>
       <c r="Z15" s="409">
         <v>1</v>
       </c>
@@ -7860,8 +7860,8 @@
       <c r="AC15" s="76" t="s">
         <v>479</v>
       </c>
-      <c r="AD15" s="639"/>
-      <c r="AF15" s="631"/>
+      <c r="AD15" s="668"/>
+      <c r="AF15" s="656"/>
       <c r="AG15" s="80"/>
       <c r="AH15" s="238" t="s">
         <v>448</v>
@@ -7874,8 +7874,8 @@
       </c>
       <c r="AK15" s="257"/>
       <c r="AL15" s="257"/>
-      <c r="AM15" s="655"/>
-      <c r="AN15" s="641"/>
+      <c r="AM15" s="651"/>
+      <c r="AN15" s="636"/>
       <c r="AP15" s="76" t="s">
         <v>73</v>
       </c>
@@ -7897,13 +7897,13 @@
       <c r="E16" s="224">
         <v>1</v>
       </c>
-      <c r="F16" s="620"/>
+      <c r="F16" s="641"/>
       <c r="G16" s="337" t="s">
         <v>488</v>
       </c>
       <c r="I16" s="469"/>
       <c r="J16" s="20"/>
-      <c r="O16" s="623"/>
+      <c r="O16" s="679"/>
       <c r="R16" s="435" t="s">
         <v>184</v>
       </c>
@@ -7914,7 +7914,7 @@
       <c r="X16" s="431" t="s">
         <v>170</v>
       </c>
-      <c r="Y16" s="658"/>
+      <c r="Y16" s="654"/>
       <c r="Z16" s="407">
         <v>1</v>
       </c>
@@ -7935,18 +7935,18 @@
       <c r="AM16" s="428" t="s">
         <v>317</v>
       </c>
-      <c r="AN16" s="641"/>
+      <c r="AN16" s="636"/>
       <c r="AP16" s="76" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="17" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="80"/>
-      <c r="F17" s="620"/>
+      <c r="F17" s="641"/>
       <c r="I17" s="470"/>
       <c r="J17" s="20"/>
       <c r="N17" s="6"/>
-      <c r="O17" s="623"/>
+      <c r="O17" s="679"/>
       <c r="Q17" s="21" t="s">
         <v>531</v>
       </c>
@@ -7966,7 +7966,7 @@
       <c r="X17" s="431" t="s">
         <v>171</v>
       </c>
-      <c r="Y17" s="658"/>
+      <c r="Y17" s="654"/>
       <c r="Z17" s="409"/>
       <c r="AA17" s="307"/>
       <c r="AB17" s="209"/>
@@ -7991,7 +7991,7 @@
       <c r="AK17" s="257"/>
       <c r="AL17" s="80"/>
       <c r="AM17" s="428"/>
-      <c r="AN17" s="641"/>
+      <c r="AN17" s="636"/>
       <c r="AO17" s="204" t="s">
         <v>497</v>
       </c>
@@ -8015,21 +8015,21 @@
       <c r="E18" s="99" t="s">
         <v>44</v>
       </c>
-      <c r="F18" s="620"/>
+      <c r="F18" s="641"/>
       <c r="G18" s="337" t="s">
         <v>528</v>
       </c>
       <c r="I18" s="24"/>
       <c r="J18" s="20"/>
-      <c r="O18" s="623"/>
+      <c r="O18" s="679"/>
       <c r="Q18" s="112"/>
-      <c r="R18" s="615" t="s">
+      <c r="R18" s="673" t="s">
         <v>536</v>
       </c>
       <c r="T18" s="100" t="s">
         <v>44</v>
       </c>
-      <c r="U18" s="663" t="s">
+      <c r="U18" s="612" t="s">
         <v>44</v>
       </c>
       <c r="V18" s="120"/>
@@ -8039,7 +8039,7 @@
       <c r="X18" s="431" t="s">
         <v>172</v>
       </c>
-      <c r="Y18" s="658"/>
+      <c r="Y18" s="654"/>
       <c r="Z18" s="409">
         <v>1</v>
       </c>
@@ -8050,38 +8050,38 @@
       <c r="AC18" s="16"/>
       <c r="AD18" s="16"/>
       <c r="AE18" s="257"/>
-      <c r="AF18" s="630" t="s">
+      <c r="AF18" s="650" t="s">
         <v>475</v>
       </c>
       <c r="AG18" s="257"/>
       <c r="AH18" s="70"/>
       <c r="AI18" s="70"/>
-      <c r="AJ18" s="656" t="s">
+      <c r="AJ18" s="652" t="s">
         <v>315</v>
       </c>
       <c r="AK18" s="257"/>
       <c r="AL18" s="80"/>
       <c r="AM18" s="428"/>
-      <c r="AN18" s="641"/>
+      <c r="AN18" s="636"/>
       <c r="AP18" s="76" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="19" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F19" s="620"/>
+      <c r="F19" s="641"/>
       <c r="I19" s="219"/>
-      <c r="O19" s="623"/>
-      <c r="R19" s="616"/>
+      <c r="O19" s="679"/>
+      <c r="R19" s="674"/>
       <c r="S19" s="30" t="s">
         <v>534</v>
       </c>
-      <c r="U19" s="664"/>
+      <c r="U19" s="613"/>
       <c r="V19" s="146"/>
       <c r="W19" s="146"/>
       <c r="X19" s="431" t="s">
         <v>173</v>
       </c>
-      <c r="Y19" s="658"/>
+      <c r="Y19" s="654"/>
       <c r="Z19" s="407">
         <v>1</v>
       </c>
@@ -8090,17 +8090,17 @@
       <c r="AC19" s="16"/>
       <c r="AD19" s="16"/>
       <c r="AE19" s="257"/>
-      <c r="AF19" s="630"/>
+      <c r="AF19" s="650"/>
       <c r="AG19" s="257"/>
       <c r="AH19" s="257"/>
       <c r="AI19" s="70"/>
-      <c r="AJ19" s="656"/>
+      <c r="AJ19" s="652"/>
       <c r="AK19" s="460" t="s">
         <v>251</v>
       </c>
       <c r="AL19" s="80"/>
       <c r="AM19" s="428"/>
-      <c r="AN19" s="641"/>
+      <c r="AN19" s="636"/>
       <c r="AP19" s="76" t="s">
         <v>468</v>
       </c>
@@ -8121,24 +8121,24 @@
       <c r="E20" s="437">
         <v>-1</v>
       </c>
-      <c r="F20" s="620"/>
+      <c r="F20" s="641"/>
       <c r="G20" s="337" t="s">
         <v>491</v>
       </c>
       <c r="I20" s="219"/>
-      <c r="O20" s="623"/>
-      <c r="Q20" s="625" t="s">
+      <c r="O20" s="679"/>
+      <c r="Q20" s="681" t="s">
         <v>48</v>
       </c>
       <c r="T20" s="404" t="s">
         <v>44</v>
       </c>
-      <c r="U20" s="665"/>
+      <c r="U20" s="614"/>
       <c r="W20" s="405"/>
       <c r="X20" s="432" t="s">
         <v>174</v>
       </c>
-      <c r="Y20" s="658"/>
+      <c r="Y20" s="654"/>
       <c r="Z20" s="411">
         <v>1</v>
       </c>
@@ -8163,7 +8163,7 @@
       <c r="AM20" s="381" t="s">
         <v>249</v>
       </c>
-      <c r="AN20" s="641"/>
+      <c r="AN20" s="636"/>
       <c r="AO20" s="338" t="s">
         <v>460</v>
       </c>
@@ -8184,20 +8184,20 @@
       <c r="E21" s="265">
         <v>0</v>
       </c>
-      <c r="F21" s="620"/>
+      <c r="F21" s="641"/>
       <c r="I21" s="219"/>
-      <c r="O21" s="623"/>
-      <c r="Q21" s="626"/>
+      <c r="O21" s="679"/>
+      <c r="Q21" s="682"/>
       <c r="T21" s="422"/>
       <c r="U21" s="14"/>
-      <c r="V21" s="660"/>
+      <c r="V21" s="609"/>
       <c r="W21" s="426" t="s">
         <v>175</v>
       </c>
       <c r="X21" s="429" t="s">
         <v>186</v>
       </c>
-      <c r="Y21" s="658"/>
+      <c r="Y21" s="654"/>
       <c r="Z21" s="445">
         <v>3</v>
       </c>
@@ -8228,15 +8228,15 @@
       <c r="AM21" s="428" t="s">
         <v>545</v>
       </c>
-      <c r="AN21" s="641"/>
+      <c r="AN21" s="636"/>
     </row>
     <row r="22" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F22" s="620"/>
+      <c r="F22" s="641"/>
       <c r="G22" s="337" t="s">
         <v>489</v>
       </c>
       <c r="I22" s="219"/>
-      <c r="O22" s="623"/>
+      <c r="O22" s="679"/>
       <c r="R22" s="434" t="s">
         <v>44</v>
       </c>
@@ -8244,14 +8244,14 @@
         <v>44</v>
       </c>
       <c r="U22" s="15"/>
-      <c r="V22" s="661"/>
+      <c r="V22" s="610"/>
       <c r="W22" s="426" t="s">
         <v>175</v>
       </c>
       <c r="X22" s="429" t="s">
         <v>187</v>
       </c>
-      <c r="Y22" s="658"/>
+      <c r="Y22" s="654"/>
       <c r="Z22" s="415"/>
       <c r="AA22" s="10"/>
       <c r="AB22" s="415"/>
@@ -8262,7 +8262,7 @@
       <c r="AG22" s="6"/>
       <c r="AH22" s="6"/>
       <c r="AI22" s="6"/>
-      <c r="AJ22" s="630" t="s">
+      <c r="AJ22" s="650" t="s">
         <v>472</v>
       </c>
       <c r="AK22" s="257"/>
@@ -8270,7 +8270,7 @@
         <v>478</v>
       </c>
       <c r="AM22" s="300"/>
-      <c r="AN22" s="641"/>
+      <c r="AN22" s="636"/>
     </row>
     <row r="23" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="231" t="s">
@@ -8288,22 +8288,22 @@
       <c r="E23" s="225">
         <v>1</v>
       </c>
-      <c r="F23" s="620"/>
+      <c r="F23" s="641"/>
       <c r="I23" s="219"/>
-      <c r="O23" s="623"/>
-      <c r="Q23" s="625" t="s">
+      <c r="O23" s="679"/>
+      <c r="Q23" s="681" t="s">
         <v>144</v>
       </c>
       <c r="T23" s="17"/>
       <c r="U23" s="420" t="s">
         <v>44</v>
       </c>
-      <c r="V23" s="661"/>
+      <c r="V23" s="610"/>
       <c r="W23" s="148"/>
       <c r="X23" s="429" t="s">
         <v>188</v>
       </c>
-      <c r="Y23" s="658"/>
+      <c r="Y23" s="654"/>
       <c r="Z23" s="17"/>
       <c r="AA23" s="10"/>
       <c r="AB23" s="415"/>
@@ -8314,13 +8314,13 @@
       <c r="AG23" s="6"/>
       <c r="AH23" s="6"/>
       <c r="AI23" s="6"/>
-      <c r="AJ23" s="630"/>
+      <c r="AJ23" s="650"/>
       <c r="AK23" s="257"/>
       <c r="AL23" s="80" t="s">
         <v>507</v>
       </c>
       <c r="AM23" s="300"/>
-      <c r="AN23" s="641"/>
+      <c r="AN23" s="636"/>
     </row>
     <row r="24" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="440" t="s">
@@ -8338,23 +8338,23 @@
       <c r="E24" s="436">
         <v>1</v>
       </c>
-      <c r="F24" s="620"/>
+      <c r="F24" s="641"/>
       <c r="G24" s="61" t="s">
         <v>490</v>
       </c>
       <c r="I24" s="219"/>
-      <c r="O24" s="623"/>
-      <c r="Q24" s="626"/>
+      <c r="O24" s="679"/>
+      <c r="Q24" s="682"/>
       <c r="T24" s="17"/>
       <c r="U24" s="227" t="s">
         <v>44</v>
       </c>
-      <c r="V24" s="661"/>
+      <c r="V24" s="610"/>
       <c r="W24" s="148"/>
       <c r="X24" s="429" t="s">
         <v>185</v>
       </c>
-      <c r="Y24" s="658"/>
+      <c r="Y24" s="654"/>
       <c r="Z24" s="17"/>
       <c r="AA24" s="10"/>
       <c r="AB24" s="415"/>
@@ -8373,12 +8373,12 @@
         <v>463</v>
       </c>
       <c r="AM24" s="300"/>
-      <c r="AN24" s="641"/>
+      <c r="AN24" s="636"/>
     </row>
     <row r="25" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F25" s="620"/>
+      <c r="F25" s="641"/>
       <c r="I25" s="219"/>
-      <c r="O25" s="623"/>
+      <c r="O25" s="679"/>
       <c r="P25" s="204" t="s">
         <v>280</v>
       </c>
@@ -8391,12 +8391,12 @@
       <c r="U25" s="400" t="s">
         <v>44</v>
       </c>
-      <c r="V25" s="662"/>
+      <c r="V25" s="611"/>
       <c r="W25" s="148"/>
       <c r="X25" s="429" t="s">
         <v>189</v>
       </c>
-      <c r="Y25" s="658"/>
+      <c r="Y25" s="654"/>
       <c r="Z25" s="17"/>
       <c r="AA25" s="10"/>
       <c r="AB25" s="415"/>
@@ -8413,7 +8413,7 @@
       <c r="AK25" s="142"/>
       <c r="AL25" s="6"/>
       <c r="AM25" s="300"/>
-      <c r="AN25" s="641"/>
+      <c r="AN25" s="636"/>
     </row>
     <row r="26" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="231" t="s">
@@ -8431,17 +8431,17 @@
       <c r="E26" s="380">
         <v>1</v>
       </c>
-      <c r="F26" s="620"/>
+      <c r="F26" s="641"/>
       <c r="G26" s="337" t="s">
         <v>487</v>
       </c>
       <c r="I26" s="219"/>
-      <c r="O26" s="623"/>
-      <c r="P26" s="643" t="s">
+      <c r="O26" s="679"/>
+      <c r="P26" s="638" t="s">
         <v>526</v>
       </c>
-      <c r="Q26" s="644"/>
-      <c r="R26" s="617" t="s">
+      <c r="Q26" s="639"/>
+      <c r="R26" s="675" t="s">
         <v>535</v>
       </c>
       <c r="T26" s="178"/>
@@ -8453,7 +8453,7 @@
       <c r="X26" s="429" t="s">
         <v>181</v>
       </c>
-      <c r="Y26" s="658"/>
+      <c r="Y26" s="654"/>
       <c r="Z26" s="17"/>
       <c r="AA26" s="10"/>
       <c r="AB26" s="415"/>
@@ -8480,7 +8480,7 @@
       <c r="AM26" s="442" t="s">
         <v>456</v>
       </c>
-      <c r="AN26" s="641"/>
+      <c r="AN26" s="636"/>
     </row>
     <row r="27" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="21" t="s">
@@ -8492,13 +8492,13 @@
       <c r="E27" s="265" t="s">
         <v>44</v>
       </c>
-      <c r="F27" s="621"/>
+      <c r="F27" s="677"/>
       <c r="G27" s="61" t="s">
         <v>544</v>
       </c>
       <c r="I27" s="220"/>
-      <c r="O27" s="624"/>
-      <c r="R27" s="618"/>
+      <c r="O27" s="680"/>
+      <c r="R27" s="676"/>
       <c r="S27" s="421" t="s">
         <v>54</v>
       </c>
@@ -8511,7 +8511,7 @@
       <c r="X27" s="429" t="s">
         <v>530</v>
       </c>
-      <c r="Y27" s="659"/>
+      <c r="Y27" s="655"/>
       <c r="Z27" s="161"/>
       <c r="AA27" s="13"/>
       <c r="AB27" s="416"/>
@@ -8528,10 +8528,48 @@
       <c r="AM27" s="381" t="s">
         <v>319</v>
       </c>
-      <c r="AN27" s="642"/>
+      <c r="AN27" s="637"/>
     </row>
   </sheetData>
   <mergeCells count="54">
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="R18:R19"/>
+    <mergeCell ref="R26:R27"/>
+    <mergeCell ref="F2:F27"/>
+    <mergeCell ref="O10:O27"/>
+    <mergeCell ref="Q20:Q21"/>
+    <mergeCell ref="Q23:Q24"/>
+    <mergeCell ref="G14:J14"/>
+    <mergeCell ref="G13:J13"/>
+    <mergeCell ref="H12:K12"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="AI6:AI10"/>
+    <mergeCell ref="AF12:AF15"/>
+    <mergeCell ref="AG7:AG12"/>
+    <mergeCell ref="L8:L9"/>
+    <mergeCell ref="S9:S12"/>
+    <mergeCell ref="N8:N9"/>
+    <mergeCell ref="AD12:AD15"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="AN1:AN27"/>
+    <mergeCell ref="P26:Q26"/>
+    <mergeCell ref="Q2:Q3"/>
+    <mergeCell ref="M2:M9"/>
+    <mergeCell ref="O2:O9"/>
+    <mergeCell ref="P10:P13"/>
+    <mergeCell ref="AK6:AK7"/>
+    <mergeCell ref="AM12:AM15"/>
+    <mergeCell ref="AF18:AF19"/>
+    <mergeCell ref="AJ18:AJ19"/>
+    <mergeCell ref="Y1:Y27"/>
+    <mergeCell ref="AJ22:AJ23"/>
+    <mergeCell ref="AK9:AK10"/>
+    <mergeCell ref="AD3:AD4"/>
+    <mergeCell ref="S2:S3"/>
+    <mergeCell ref="R2:R3"/>
     <mergeCell ref="V21:V25"/>
     <mergeCell ref="U18:U20"/>
     <mergeCell ref="C2:C3"/>
@@ -8548,44 +8586,6 @@
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="B4:B5"/>
-    <mergeCell ref="AN1:AN27"/>
-    <mergeCell ref="P26:Q26"/>
-    <mergeCell ref="Q2:Q3"/>
-    <mergeCell ref="M2:M9"/>
-    <mergeCell ref="O2:O9"/>
-    <mergeCell ref="P10:P13"/>
-    <mergeCell ref="AK6:AK7"/>
-    <mergeCell ref="AM12:AM15"/>
-    <mergeCell ref="AF18:AF19"/>
-    <mergeCell ref="AJ18:AJ19"/>
-    <mergeCell ref="Y1:Y27"/>
-    <mergeCell ref="AJ22:AJ23"/>
-    <mergeCell ref="AK9:AK10"/>
-    <mergeCell ref="AD3:AD4"/>
-    <mergeCell ref="S2:S3"/>
-    <mergeCell ref="R2:R3"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="AI6:AI10"/>
-    <mergeCell ref="AF12:AF15"/>
-    <mergeCell ref="AG7:AG12"/>
-    <mergeCell ref="L8:L9"/>
-    <mergeCell ref="S9:S12"/>
-    <mergeCell ref="N8:N9"/>
-    <mergeCell ref="AD12:AD15"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="R18:R19"/>
-    <mergeCell ref="R26:R27"/>
-    <mergeCell ref="F2:F27"/>
-    <mergeCell ref="O10:O27"/>
-    <mergeCell ref="Q20:Q21"/>
-    <mergeCell ref="Q23:Q24"/>
-    <mergeCell ref="G14:J14"/>
-    <mergeCell ref="G13:J13"/>
-    <mergeCell ref="H12:K12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8622,12 +8622,12 @@
       <c r="B1" s="603" t="s">
         <v>310</v>
       </c>
-      <c r="C1" s="627"/>
+      <c r="C1" s="683"/>
       <c r="D1" s="204"/>
       <c r="J1" s="603" t="s">
         <v>69</v>
       </c>
-      <c r="K1" s="627"/>
+      <c r="K1" s="683"/>
       <c r="L1" s="195" t="s">
         <v>330</v>
       </c>
@@ -8961,7 +8961,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB54FD83-008D-4F8B-87AC-83E7F70047CB}">
   <dimension ref="A1:AL31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+    <sheetView topLeftCell="N1" workbookViewId="0">
       <selection activeCell="AH21" sqref="AH21"/>
     </sheetView>
   </sheetViews>
@@ -9030,7 +9030,7 @@
       <c r="P1" s="398" t="s">
         <v>397</v>
       </c>
-      <c r="Q1" s="701" t="s">
+      <c r="Q1" s="714" t="s">
         <v>180</v>
       </c>
       <c r="R1" s="100" t="s">
@@ -9054,7 +9054,7 @@
       <c r="AA1" s="517" t="s">
         <v>437</v>
       </c>
-      <c r="AB1" s="695" t="s">
+      <c r="AB1" s="708" t="s">
         <v>594</v>
       </c>
       <c r="AC1" s="99" t="s">
@@ -9076,32 +9076,32 @@
       </c>
     </row>
     <row r="2" spans="1:38" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="706">
+      <c r="A2" s="693">
         <f ca="1">TODAY()</f>
         <v>45285</v>
       </c>
-      <c r="B2" s="708" t="s">
+      <c r="B2" s="695" t="s">
         <v>379</v>
       </c>
-      <c r="C2" s="645" t="s">
+      <c r="C2" s="615" t="s">
         <v>357</v>
       </c>
-      <c r="D2" s="710" t="s">
+      <c r="D2" s="697" t="s">
         <v>102</v>
       </c>
-      <c r="E2" s="712" t="s">
+      <c r="E2" s="699" t="s">
         <v>64</v>
       </c>
       <c r="F2" s="191" t="s">
         <v>218</v>
       </c>
-      <c r="G2" s="613" t="s">
+      <c r="G2" s="659" t="s">
         <v>372</v>
       </c>
       <c r="H2" s="206" t="s">
         <v>218</v>
       </c>
-      <c r="I2" s="692" t="s">
+      <c r="I2" s="705" t="s">
         <v>102</v>
       </c>
       <c r="J2" s="396" t="s">
@@ -9125,7 +9125,7 @@
       <c r="P2" s="399">
         <v>40</v>
       </c>
-      <c r="Q2" s="702"/>
+      <c r="Q2" s="715"/>
       <c r="R2" s="21">
         <f>R7+R20</f>
         <v>4</v>
@@ -9150,7 +9150,7 @@
         <f>IF((Z2+T2)&gt;0,0,-1)</f>
         <v>0</v>
       </c>
-      <c r="AB2" s="696"/>
+      <c r="AB2" s="709"/>
       <c r="AC2" s="35"/>
       <c r="AH2" s="6" t="s">
         <v>344</v>
@@ -9167,14 +9167,14 @@
       </c>
     </row>
     <row r="3" spans="1:38" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="707"/>
-      <c r="B3" s="709"/>
-      <c r="C3" s="646"/>
-      <c r="D3" s="711"/>
-      <c r="E3" s="713"/>
-      <c r="G3" s="614"/>
+      <c r="A3" s="694"/>
+      <c r="B3" s="696"/>
+      <c r="C3" s="616"/>
+      <c r="D3" s="698"/>
+      <c r="E3" s="700"/>
+      <c r="G3" s="660"/>
       <c r="H3" s="6"/>
-      <c r="I3" s="693"/>
+      <c r="I3" s="706"/>
       <c r="K3" s="24">
         <v>2</v>
       </c>
@@ -9189,7 +9189,7 @@
       <c r="V3" s="470"/>
       <c r="W3" s="6"/>
       <c r="X3" s="470"/>
-      <c r="AB3" s="696"/>
+      <c r="AB3" s="709"/>
       <c r="AC3" s="35"/>
       <c r="AE3" s="100" t="s">
         <v>589</v>
@@ -9214,10 +9214,10 @@
         <v>380</v>
       </c>
       <c r="B4" s="243"/>
-      <c r="C4" s="714" t="s">
+      <c r="C4" s="701" t="s">
         <v>177</v>
       </c>
-      <c r="I4" s="693"/>
+      <c r="I4" s="706"/>
       <c r="R4" s="471" t="s">
         <v>589</v>
       </c>
@@ -9229,7 +9229,7 @@
       <c r="V4" s="470"/>
       <c r="W4" s="6"/>
       <c r="X4" s="470"/>
-      <c r="AB4" s="696"/>
+      <c r="AB4" s="709"/>
       <c r="AC4" s="35"/>
       <c r="AE4" s="20"/>
       <c r="AF4" s="100" t="s">
@@ -9256,7 +9256,7 @@
       <c r="B5" s="100" t="s">
         <v>357</v>
       </c>
-      <c r="C5" s="715"/>
+      <c r="C5" s="702"/>
       <c r="D5" s="222" t="s">
         <v>102</v>
       </c>
@@ -9272,7 +9272,7 @@
       <c r="H5" s="206" t="s">
         <v>218</v>
       </c>
-      <c r="I5" s="693"/>
+      <c r="I5" s="706"/>
       <c r="J5" s="397" t="s">
         <v>268</v>
       </c>
@@ -9299,7 +9299,7 @@
       <c r="V5" s="468"/>
       <c r="W5" s="6"/>
       <c r="X5" s="468"/>
-      <c r="AB5" s="696"/>
+      <c r="AB5" s="709"/>
       <c r="AC5" s="2" t="s">
         <v>592</v>
       </c>
@@ -9321,19 +9321,19 @@
       </c>
     </row>
     <row r="6" spans="1:38" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="703" t="s">
+      <c r="A6" s="690" t="s">
         <v>285</v>
       </c>
       <c r="B6" s="105" t="s">
         <v>198</v>
       </c>
-      <c r="C6" s="628"/>
-      <c r="D6" s="629"/>
+      <c r="C6" s="661"/>
+      <c r="D6" s="662"/>
       <c r="E6" s="96">
         <v>1</v>
       </c>
       <c r="G6" s="599"/>
-      <c r="I6" s="693"/>
+      <c r="I6" s="706"/>
       <c r="P6" s="61" t="s">
         <v>592</v>
       </c>
@@ -9345,7 +9345,7 @@
         <f>S7+S11-SUM(V2:V10)</f>
         <v>3</v>
       </c>
-      <c r="AB6" s="696"/>
+      <c r="AB6" s="709"/>
       <c r="AC6" s="35"/>
       <c r="AE6" s="64">
         <f>AE7-SUM(AL2:AL10)+AE11</f>
@@ -9361,7 +9361,7 @@
       <c r="AL6" s="112"/>
     </row>
     <row r="7" spans="1:38" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="704"/>
+      <c r="A7" s="691"/>
       <c r="B7" s="100" t="s">
         <v>154</v>
       </c>
@@ -9372,7 +9372,7 @@
         <v>135</v>
       </c>
       <c r="G7" s="599"/>
-      <c r="I7" s="693"/>
+      <c r="I7" s="706"/>
       <c r="M7" s="16" t="s">
         <v>347</v>
       </c>
@@ -9404,7 +9404,7 @@
       <c r="X7" s="469">
         <v>1</v>
       </c>
-      <c r="AB7" s="696"/>
+      <c r="AB7" s="709"/>
       <c r="AC7" s="99" t="s">
         <v>593</v>
       </c>
@@ -9430,7 +9430,7 @@
       </c>
     </row>
     <row r="8" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="705"/>
+      <c r="A8" s="692"/>
       <c r="B8" s="212" t="s">
         <v>28</v>
       </c>
@@ -9439,7 +9439,7 @@
         <v>3</v>
       </c>
       <c r="G8" s="599"/>
-      <c r="I8" s="693"/>
+      <c r="I8" s="706"/>
       <c r="N8" s="80"/>
       <c r="U8" s="6"/>
       <c r="V8" s="24"/>
@@ -9449,7 +9449,7 @@
       <c r="X8" s="470">
         <v>1</v>
       </c>
-      <c r="AB8" s="696"/>
+      <c r="AB8" s="709"/>
       <c r="AC8" s="515"/>
       <c r="AH8" s="6" t="s">
         <v>612</v>
@@ -9480,7 +9480,7 @@
       </c>
       <c r="G9" s="599"/>
       <c r="H9" s="6"/>
-      <c r="I9" s="693"/>
+      <c r="I9" s="706"/>
       <c r="M9" s="19" t="s">
         <v>525</v>
       </c>
@@ -9493,7 +9493,7 @@
       <c r="X9" s="470">
         <v>1</v>
       </c>
-      <c r="AB9" s="696"/>
+      <c r="AB9" s="709"/>
       <c r="AC9" s="515"/>
       <c r="AE9" s="20"/>
       <c r="AF9" s="20"/>
@@ -9517,7 +9517,7 @@
         <v>39</v>
       </c>
       <c r="G10" s="599"/>
-      <c r="I10" s="693"/>
+      <c r="I10" s="706"/>
       <c r="J10" s="24" t="s">
         <v>372</v>
       </c>
@@ -9532,7 +9532,7 @@
       <c r="V10" s="470"/>
       <c r="W10" s="6"/>
       <c r="X10" s="470"/>
-      <c r="AB10" s="696"/>
+      <c r="AB10" s="709"/>
       <c r="AC10" s="515"/>
       <c r="AE10" s="20"/>
       <c r="AF10" s="20"/>
@@ -9564,7 +9564,7 @@
         <v>265</v>
       </c>
       <c r="G11" s="599"/>
-      <c r="I11" s="693"/>
+      <c r="I11" s="706"/>
       <c r="J11" s="24" t="s">
         <v>194</v>
       </c>
@@ -9590,13 +9590,13 @@
       <c r="S11" s="24">
         <v>3</v>
       </c>
-      <c r="U11" s="698" t="s">
+      <c r="U11" s="711" t="s">
         <v>558</v>
       </c>
-      <c r="V11" s="699"/>
-      <c r="W11" s="699"/>
-      <c r="X11" s="700"/>
-      <c r="AB11" s="697"/>
+      <c r="V11" s="712"/>
+      <c r="W11" s="712"/>
+      <c r="X11" s="713"/>
+      <c r="AB11" s="710"/>
       <c r="AC11" s="99" t="s">
         <v>595</v>
       </c>
@@ -9610,13 +9610,13 @@
         <v>4</v>
       </c>
       <c r="AG11" s="414"/>
-      <c r="AH11" s="698" t="s">
+      <c r="AH11" s="711" t="s">
         <v>603</v>
       </c>
-      <c r="AI11" s="699"/>
-      <c r="AJ11" s="699"/>
-      <c r="AK11" s="699"/>
-      <c r="AL11" s="700"/>
+      <c r="AI11" s="712"/>
+      <c r="AJ11" s="712"/>
+      <c r="AK11" s="712"/>
+      <c r="AL11" s="713"/>
     </row>
     <row r="12" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="227" t="s">
@@ -9627,7 +9627,7 @@
         <v>3</v>
       </c>
       <c r="G12" s="599"/>
-      <c r="I12" s="693"/>
+      <c r="I12" s="706"/>
       <c r="J12" s="24" t="s">
         <v>516</v>
       </c>
@@ -9660,7 +9660,7 @@
       </c>
       <c r="D13" s="20"/>
       <c r="G13" s="599"/>
-      <c r="I13" s="693"/>
+      <c r="I13" s="706"/>
       <c r="J13" s="108" t="s">
         <v>548</v>
       </c>
@@ -9704,7 +9704,7 @@
       <c r="H14" s="206" t="s">
         <v>218</v>
       </c>
-      <c r="I14" s="693"/>
+      <c r="I14" s="706"/>
       <c r="U14" s="67" t="s">
         <v>80</v>
       </c>
@@ -9731,7 +9731,7 @@
       <c r="H15" s="271">
         <v>0</v>
       </c>
-      <c r="I15" s="693"/>
+      <c r="I15" s="706"/>
       <c r="J15" s="108" t="s">
         <v>153</v>
       </c>
@@ -9762,7 +9762,7 @@
       <c r="D16" s="2" t="s">
         <v>492</v>
       </c>
-      <c r="I16" s="693"/>
+      <c r="I16" s="706"/>
       <c r="K16" s="100" t="s">
         <v>44</v>
       </c>
@@ -9798,7 +9798,7 @@
       <c r="G17" s="2" t="s">
         <v>423</v>
       </c>
-      <c r="I17" s="693"/>
+      <c r="I17" s="706"/>
       <c r="L17" s="2" t="s">
         <v>426</v>
       </c>
@@ -9812,13 +9812,13 @@
     </row>
     <row r="18" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G18" s="16"/>
-      <c r="I18" s="693"/>
+      <c r="I18" s="706"/>
       <c r="L18" s="16"/>
       <c r="M18" s="21"/>
-      <c r="O18" s="690" t="s">
+      <c r="O18" s="703" t="s">
         <v>517</v>
       </c>
-      <c r="P18" s="691"/>
+      <c r="P18" s="704"/>
       <c r="Q18" s="127" t="s">
         <v>44</v>
       </c>
@@ -9840,7 +9840,7 @@
       </c>
     </row>
     <row r="19" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I19" s="693"/>
+      <c r="I19" s="706"/>
       <c r="M19" s="21" t="s">
         <v>425</v>
       </c>
@@ -9872,7 +9872,7 @@
       <c r="G20" s="2" t="s">
         <v>423</v>
       </c>
-      <c r="I20" s="693"/>
+      <c r="I20" s="706"/>
       <c r="K20" s="19" t="s">
         <v>422</v>
       </c>
@@ -9903,7 +9903,7 @@
       <c r="X20" s="468"/>
     </row>
     <row r="21" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I21" s="693"/>
+      <c r="I21" s="706"/>
       <c r="M21" s="216" t="s">
         <v>411</v>
       </c>
@@ -9937,7 +9937,7 @@
       <c r="G22" s="2" t="s">
         <v>423</v>
       </c>
-      <c r="I22" s="693"/>
+      <c r="I22" s="706"/>
       <c r="P22" s="99" t="s">
         <v>591</v>
       </c>
@@ -9952,7 +9952,7 @@
       <c r="E23" s="283" t="s">
         <v>44</v>
       </c>
-      <c r="I23" s="693"/>
+      <c r="I23" s="706"/>
       <c r="Q23" s="24">
         <f>SUM(V23:V31)</f>
         <v>6</v>
@@ -9969,7 +9969,7 @@
       </c>
     </row>
     <row r="24" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I24" s="693"/>
+      <c r="I24" s="706"/>
       <c r="U24" s="35"/>
       <c r="V24" s="509">
         <v>0</v>
@@ -9997,7 +9997,7 @@
       <c r="H25" s="191" t="s">
         <v>266</v>
       </c>
-      <c r="I25" s="693"/>
+      <c r="I25" s="706"/>
       <c r="J25" s="397" t="s">
         <v>269</v>
       </c>
@@ -10042,7 +10042,7 @@
       <c r="H26" s="19" t="s">
         <v>218</v>
       </c>
-      <c r="I26" s="693"/>
+      <c r="I26" s="706"/>
       <c r="K26" s="24">
         <v>15</v>
       </c>
@@ -10077,7 +10077,7 @@
       </c>
     </row>
     <row r="27" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I27" s="693"/>
+      <c r="I27" s="706"/>
       <c r="O27" s="2" t="s">
         <v>98</v>
       </c>
@@ -10104,7 +10104,7 @@
       <c r="E28" s="215">
         <v>2</v>
       </c>
-      <c r="I28" s="693"/>
+      <c r="I28" s="706"/>
       <c r="Q28" s="6"/>
       <c r="R28" s="112"/>
       <c r="T28" s="142"/>
@@ -10126,7 +10126,7 @@
       <c r="H29" s="191" t="s">
         <v>267</v>
       </c>
-      <c r="I29" s="694"/>
+      <c r="I29" s="707"/>
       <c r="J29" s="324"/>
       <c r="L29" s="96" t="s">
         <v>273</v>
@@ -10184,6 +10184,13 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="I2:I29"/>
+    <mergeCell ref="AB1:AB11"/>
+    <mergeCell ref="AH11:AL11"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="Q1:Q2"/>
+    <mergeCell ref="U11:X11"/>
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="G5:G14"/>
     <mergeCell ref="A2:A3"/>
@@ -10195,13 +10202,6 @@
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="G2:G3"/>
     <mergeCell ref="C2:C3"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="I2:I29"/>
-    <mergeCell ref="AB1:AB11"/>
-    <mergeCell ref="AH11:AL11"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="Q1:Q2"/>
-    <mergeCell ref="U11:X11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -10212,7 +10212,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2029A93E-B53C-4201-9F17-439C144F3CF1}">
   <dimension ref="A1:AT37"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
       <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
@@ -10313,14 +10313,14 @@
         <f ca="1">TODAY()</f>
         <v>45285</v>
       </c>
-      <c r="T1" s="735"/>
+      <c r="T1" s="742"/>
       <c r="U1" s="142"/>
       <c r="V1" s="6"/>
       <c r="W1" s="6"/>
-      <c r="X1" s="719" t="s">
+      <c r="X1" s="726" t="s">
         <v>441</v>
       </c>
-      <c r="Y1" s="720"/>
+      <c r="Y1" s="727"/>
       <c r="Z1" s="306">
         <f>68-(W8+Y3+X3+U3)</f>
         <v>0</v>
@@ -10336,27 +10336,27 @@
       <c r="AD1" s="302" t="s">
         <v>44</v>
       </c>
-      <c r="AE1" s="721" t="s">
+      <c r="AE1" s="728" t="s">
         <v>190</v>
       </c>
-      <c r="AF1" s="722"/>
-      <c r="AG1" s="723"/>
-      <c r="AH1" s="724" t="s">
+      <c r="AF1" s="729"/>
+      <c r="AG1" s="730"/>
+      <c r="AH1" s="731" t="s">
         <v>293</v>
       </c>
-      <c r="AI1" s="725"/>
-      <c r="AJ1" s="726"/>
-      <c r="AK1" s="613" t="s">
+      <c r="AI1" s="732"/>
+      <c r="AJ1" s="733"/>
+      <c r="AK1" s="659" t="s">
         <v>616</v>
       </c>
       <c r="AL1" s="551" t="s">
         <v>617</v>
       </c>
-      <c r="AM1" s="716" t="s">
+      <c r="AM1" s="723" t="s">
         <v>444</v>
       </c>
-      <c r="AN1" s="717"/>
-      <c r="AO1" s="718"/>
+      <c r="AN1" s="724"/>
+      <c r="AO1" s="725"/>
       <c r="AR1" s="142"/>
     </row>
     <row r="2" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -10371,27 +10371,27 @@
         <f>K2+L2</f>
         <v>25</v>
       </c>
-      <c r="K2" s="743">
+      <c r="K2" s="721">
         <f>SUM(K4:K37)</f>
         <v>6</v>
       </c>
-      <c r="L2" s="741">
+      <c r="L2" s="719">
         <f>SUM(L4:L37)</f>
         <v>19</v>
       </c>
-      <c r="M2" s="727">
+      <c r="M2" s="734">
         <f>SUM(M5:M30)</f>
         <v>0</v>
       </c>
-      <c r="N2" s="729">
+      <c r="N2" s="736">
         <f>SUM(N4:N29)</f>
         <v>9</v>
       </c>
-      <c r="O2" s="731">
+      <c r="O2" s="738">
         <f>SUM(O4:O29)</f>
         <v>9</v>
       </c>
-      <c r="P2" s="637">
+      <c r="P2" s="666">
         <f>SUM(N30:N37)* (-1)</f>
         <v>-1</v>
       </c>
@@ -10404,14 +10404,14 @@
       <c r="S2" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="T2" s="736"/>
+      <c r="T2" s="743"/>
       <c r="U2" s="537" t="s">
         <v>262</v>
       </c>
       <c r="V2" s="482" t="s">
         <v>219</v>
       </c>
-      <c r="W2" s="733" t="s">
+      <c r="W2" s="740" t="s">
         <v>234</v>
       </c>
       <c r="X2" s="483" t="s">
@@ -10453,7 +10453,7 @@
       <c r="AJ2" s="150" t="s">
         <v>288</v>
       </c>
-      <c r="AK2" s="614"/>
+      <c r="AK2" s="660"/>
       <c r="AL2" s="592" t="s">
         <v>288</v>
       </c>
@@ -10481,12 +10481,12 @@
         <f>V3+X3+Y3+U3</f>
         <v>68</v>
       </c>
-      <c r="K3" s="744"/>
-      <c r="L3" s="742"/>
-      <c r="M3" s="728"/>
-      <c r="N3" s="730"/>
-      <c r="O3" s="732"/>
-      <c r="P3" s="638"/>
+      <c r="K3" s="722"/>
+      <c r="L3" s="720"/>
+      <c r="M3" s="735"/>
+      <c r="N3" s="737"/>
+      <c r="O3" s="739"/>
+      <c r="P3" s="667"/>
       <c r="Q3" s="172">
         <f>(M2+N2)-Y3</f>
         <v>0</v>
@@ -10494,7 +10494,7 @@
       <c r="S3" s="159" t="s">
         <v>244</v>
       </c>
-      <c r="T3" s="737"/>
+      <c r="T3" s="744"/>
       <c r="U3" s="538">
         <f>SUM(U4:U29)</f>
         <v>12</v>
@@ -10503,7 +10503,7 @@
         <f>SUM(V4:V29)</f>
         <v>39</v>
       </c>
-      <c r="W3" s="734"/>
+      <c r="W3" s="741"/>
       <c r="X3" s="485">
         <f t="shared" ref="X3:AC3" si="0">SUM(X4:X29)</f>
         <v>8</v>
@@ -10609,7 +10609,7 @@
         <f>AC4</f>
         <v>0</v>
       </c>
-      <c r="P4" s="738">
+      <c r="P4" s="716">
         <v>1</v>
       </c>
       <c r="Q4" s="20"/>
@@ -10695,7 +10695,7 @@
         <f>AC5</f>
         <v>0</v>
       </c>
-      <c r="P5" s="739"/>
+      <c r="P5" s="717"/>
       <c r="Q5" s="20"/>
       <c r="R5" s="2" t="s">
         <v>340</v>
@@ -10789,7 +10789,7 @@
         <f>AC6</f>
         <v>0</v>
       </c>
-      <c r="P6" s="739"/>
+      <c r="P6" s="717"/>
       <c r="Q6" s="19" t="s">
         <v>335</v>
       </c>
@@ -10892,7 +10892,7 @@
         <f>AC7</f>
         <v>1</v>
       </c>
-      <c r="P7" s="739"/>
+      <c r="P7" s="717"/>
       <c r="Q7" s="20"/>
       <c r="R7" s="2" t="s">
         <v>335</v>
@@ -11008,7 +11008,7 @@
         <f t="shared" ref="O8:O37" si="10">AC8</f>
         <v>0</v>
       </c>
-      <c r="P8" s="739"/>
+      <c r="P8" s="717"/>
       <c r="Q8" s="21" t="s">
         <v>233</v>
       </c>
@@ -11099,7 +11099,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="P9" s="739"/>
+      <c r="P9" s="717"/>
       <c r="Q9" s="21" t="s">
         <v>335</v>
       </c>
@@ -11204,7 +11204,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="P10" s="739"/>
+      <c r="P10" s="717"/>
       <c r="Q10" s="20"/>
       <c r="R10" s="2" t="s">
         <v>340</v>
@@ -11294,7 +11294,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="P11" s="739"/>
+      <c r="P11" s="717"/>
       <c r="Q11" s="21" t="s">
         <v>335</v>
       </c>
@@ -11359,14 +11359,14 @@
       <c r="AR11" s="508"/>
     </row>
     <row r="12" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="675" t="s">
+      <c r="A12" s="626" t="s">
         <v>55</v>
       </c>
       <c r="B12" s="30">
         <v>13</v>
       </c>
       <c r="C12" s="2"/>
-      <c r="E12" s="625" t="s">
+      <c r="E12" s="681" t="s">
         <v>56</v>
       </c>
       <c r="G12" s="262"/>
@@ -11391,7 +11391,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="P12" s="739"/>
+      <c r="P12" s="717"/>
       <c r="Q12" s="21" t="s">
         <v>335</v>
       </c>
@@ -11468,14 +11468,14 @@
       </c>
     </row>
     <row r="13" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="677"/>
+      <c r="A13" s="628"/>
       <c r="B13" s="584">
         <v>12</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E13" s="626"/>
+      <c r="E13" s="682"/>
       <c r="F13" s="172">
         <v>0</v>
       </c>
@@ -11499,7 +11499,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="P13" s="739"/>
+      <c r="P13" s="717"/>
       <c r="Q13" s="21" t="s">
         <v>335</v>
       </c>
@@ -11581,7 +11581,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="P14" s="739"/>
+      <c r="P14" s="717"/>
       <c r="Q14" s="20"/>
       <c r="R14" s="200" t="s">
         <v>339</v>
@@ -11682,7 +11682,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="P15" s="739"/>
+      <c r="P15" s="717"/>
       <c r="Q15" s="20"/>
       <c r="R15" s="200" t="s">
         <v>339</v>
@@ -11774,7 +11774,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="P16" s="739"/>
+      <c r="P16" s="717"/>
       <c r="Q16" s="21" t="s">
         <v>335</v>
       </c>
@@ -11875,7 +11875,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="P17" s="739"/>
+      <c r="P17" s="717"/>
       <c r="Q17" s="20"/>
       <c r="R17" s="2" t="s">
         <v>341</v>
@@ -11975,7 +11975,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="P18" s="739"/>
+      <c r="P18" s="717"/>
       <c r="Q18" s="21" t="s">
         <v>335</v>
       </c>
@@ -12065,7 +12065,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="P19" s="739"/>
+      <c r="P19" s="717"/>
       <c r="Q19" s="20"/>
       <c r="R19" s="2" t="s">
         <v>334</v>
@@ -12173,11 +12173,11 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="P20" s="740"/>
+      <c r="P20" s="718"/>
       <c r="Q20" s="603" t="s">
         <v>335</v>
       </c>
-      <c r="R20" s="627"/>
+      <c r="R20" s="683"/>
       <c r="S20" s="534" t="s">
         <v>85</v>
       </c>
@@ -12437,7 +12437,7 @@
     </row>
     <row r="23" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="24"/>
-      <c r="E23" s="682" t="s">
+      <c r="E23" s="633" t="s">
         <v>289</v>
       </c>
       <c r="F23" s="180"/>
@@ -12540,7 +12540,7 @@
       <c r="C24" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="E24" s="683"/>
+      <c r="E24" s="634"/>
       <c r="F24" s="172"/>
       <c r="H24" s="42"/>
       <c r="J24" s="571" t="s">
@@ -12565,7 +12565,7 @@
       <c r="Q24" s="603" t="s">
         <v>335</v>
       </c>
-      <c r="R24" s="627"/>
+      <c r="R24" s="683"/>
       <c r="S24" s="534" t="s">
         <v>249</v>
       </c>
@@ -13216,8 +13216,8 @@
       <c r="AR31" s="508"/>
     </row>
     <row r="32" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="630"/>
-      <c r="B32" s="630"/>
+      <c r="A32" s="650"/>
+      <c r="B32" s="650"/>
       <c r="J32" s="572"/>
       <c r="K32" s="587"/>
       <c r="L32" s="581"/>
@@ -13792,15 +13792,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="Q24:R24"/>
-    <mergeCell ref="P4:P20"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="L2:L3"/>
-    <mergeCell ref="K2:K3"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="Q20:R20"/>
     <mergeCell ref="AM1:AO1"/>
     <mergeCell ref="X1:Y1"/>
     <mergeCell ref="AE1:AG1"/>
@@ -13812,6 +13803,15 @@
     <mergeCell ref="W2:W3"/>
     <mergeCell ref="T1:T3"/>
     <mergeCell ref="AK1:AK2"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="Q24:R24"/>
+    <mergeCell ref="P4:P20"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="L2:L3"/>
+    <mergeCell ref="K2:K3"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="Q20:R20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -13879,7 +13879,7 @@
       <c r="V1" s="603" t="s">
         <v>70</v>
       </c>
-      <c r="W1" s="627"/>
+      <c r="W1" s="683"/>
       <c r="X1" s="62" t="s">
         <v>101</v>
       </c>
@@ -13898,7 +13898,7 @@
       <c r="AC1" s="116" t="s">
         <v>190</v>
       </c>
-      <c r="AD1" s="752" t="s">
+      <c r="AD1" s="759" t="s">
         <v>211</v>
       </c>
       <c r="AE1" s="116" t="s">
@@ -13915,10 +13915,10 @@
       <c r="E2" s="39" t="s">
         <v>73</v>
       </c>
-      <c r="F2" s="751" t="s">
+      <c r="F2" s="790" t="s">
         <v>74</v>
       </c>
-      <c r="G2" s="779" t="s">
+      <c r="G2" s="747" t="s">
         <v>44</v>
       </c>
       <c r="H2" s="40" t="s">
@@ -13946,10 +13946,10 @@
       <c r="U2" s="60" t="s">
         <v>105</v>
       </c>
-      <c r="V2" s="719" t="s">
+      <c r="V2" s="726" t="s">
         <v>120</v>
       </c>
-      <c r="W2" s="720"/>
+      <c r="W2" s="727"/>
       <c r="X2" s="64" t="s">
         <v>109</v>
       </c>
@@ -13968,7 +13968,7 @@
       <c r="AC2" s="117" t="s">
         <v>98</v>
       </c>
-      <c r="AD2" s="753"/>
+      <c r="AD2" s="760"/>
       <c r="AE2" s="64" t="s">
         <v>98</v>
       </c>
@@ -13987,8 +13987,8 @@
       <c r="E3" s="39" t="s">
         <v>79</v>
       </c>
-      <c r="F3" s="679"/>
-      <c r="G3" s="780"/>
+      <c r="F3" s="630"/>
+      <c r="G3" s="748"/>
       <c r="H3" s="40" t="s">
         <v>80</v>
       </c>
@@ -13999,13 +13999,13 @@
         <v>81</v>
       </c>
       <c r="N3" s="44"/>
-      <c r="O3" s="789" t="s">
+      <c r="O3" s="757" t="s">
         <v>44</v>
       </c>
-      <c r="P3" s="771" t="s">
+      <c r="P3" s="778" t="s">
         <v>217</v>
       </c>
-      <c r="Q3" s="772"/>
+      <c r="Q3" s="779"/>
       <c r="S3" s="57" t="s">
         <v>218</v>
       </c>
@@ -14015,15 +14015,15 @@
       <c r="W3" s="59" t="s">
         <v>104</v>
       </c>
-      <c r="AD3" s="753"/>
+      <c r="AD3" s="760"/>
     </row>
     <row r="4" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G4" s="780"/>
+      <c r="G4" s="748"/>
       <c r="H4" s="6"/>
       <c r="L4" s="687" t="s">
         <v>82</v>
       </c>
-      <c r="O4" s="790"/>
+      <c r="O4" s="758"/>
       <c r="T4" s="55" t="s">
         <v>97</v>
       </c>
@@ -14037,8 +14037,8 @@
         <v>194</v>
       </c>
       <c r="Z4" s="605"/>
-      <c r="AA4" s="627"/>
-      <c r="AD4" s="753"/>
+      <c r="AA4" s="683"/>
+      <c r="AD4" s="760"/>
     </row>
     <row r="5" spans="1:31" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" s="52" t="s">
@@ -14053,21 +14053,21 @@
       <c r="F5" s="66" t="s">
         <v>84</v>
       </c>
-      <c r="G5" s="780"/>
+      <c r="G5" s="748"/>
       <c r="H5" s="46" t="s">
         <v>75</v>
       </c>
-      <c r="K5" s="758" t="s">
+      <c r="K5" s="765" t="s">
         <v>215</v>
       </c>
-      <c r="L5" s="773"/>
+      <c r="L5" s="780"/>
       <c r="M5" s="2" t="s">
         <v>213</v>
       </c>
       <c r="N5" s="61" t="s">
         <v>212</v>
       </c>
-      <c r="O5" s="790"/>
+      <c r="O5" s="758"/>
       <c r="P5" s="108" t="s">
         <v>214</v>
       </c>
@@ -14083,11 +14083,11 @@
       <c r="U5" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="Y5" s="761" t="s">
+      <c r="Y5" s="768" t="s">
         <v>282</v>
       </c>
-      <c r="Z5" s="762"/>
-      <c r="AD5" s="753"/>
+      <c r="Z5" s="769"/>
+      <c r="AD5" s="760"/>
     </row>
     <row r="6" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C6" s="109"/>
@@ -14097,16 +14097,16 @@
       <c r="E6" s="45" t="s">
         <v>85</v>
       </c>
-      <c r="G6" s="780"/>
+      <c r="G6" s="748"/>
       <c r="H6" s="46" t="s">
         <v>80</v>
       </c>
       <c r="I6" s="23">
         <v>15</v>
       </c>
-      <c r="K6" s="759"/>
-      <c r="L6" s="773"/>
-      <c r="O6" s="790"/>
+      <c r="K6" s="766"/>
+      <c r="L6" s="780"/>
+      <c r="O6" s="758"/>
       <c r="T6" s="2" t="s">
         <v>100</v>
       </c>
@@ -14116,23 +14116,23 @@
       <c r="V6" s="21">
         <v>-1</v>
       </c>
-      <c r="AD6" s="753"/>
+      <c r="AD6" s="760"/>
     </row>
     <row r="7" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C7" s="110"/>
-      <c r="G7" s="780"/>
+      <c r="G7" s="748"/>
       <c r="H7" s="6"/>
-      <c r="K7" s="759"/>
-      <c r="L7" s="773"/>
+      <c r="K7" s="766"/>
+      <c r="L7" s="780"/>
       <c r="N7" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="O7" s="790"/>
+      <c r="O7" s="758"/>
       <c r="P7" s="73"/>
       <c r="U7" s="104" t="s">
         <v>20</v>
       </c>
-      <c r="AD7" s="753"/>
+      <c r="AD7" s="760"/>
     </row>
     <row r="8" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C8" s="130"/>
@@ -14145,7 +14145,7 @@
       <c r="F8" s="66" t="s">
         <v>86</v>
       </c>
-      <c r="G8" s="780"/>
+      <c r="G8" s="748"/>
       <c r="H8" s="50" t="s">
         <v>75</v>
       </c>
@@ -14155,41 +14155,41 @@
       <c r="J8" s="111">
         <v>115</v>
       </c>
-      <c r="K8" s="759"/>
-      <c r="L8" s="773"/>
-      <c r="O8" s="790"/>
+      <c r="K8" s="766"/>
+      <c r="L8" s="780"/>
+      <c r="O8" s="758"/>
       <c r="P8" s="49"/>
-      <c r="S8" s="755" t="s">
+      <c r="S8" s="762" t="s">
         <v>210</v>
       </c>
-      <c r="T8" s="756"/>
-      <c r="U8" s="756"/>
-      <c r="V8" s="756"/>
-      <c r="W8" s="756"/>
-      <c r="X8" s="756"/>
-      <c r="Y8" s="756"/>
-      <c r="Z8" s="756"/>
-      <c r="AA8" s="756"/>
-      <c r="AB8" s="756"/>
-      <c r="AC8" s="757"/>
-      <c r="AD8" s="753"/>
+      <c r="T8" s="763"/>
+      <c r="U8" s="763"/>
+      <c r="V8" s="763"/>
+      <c r="W8" s="763"/>
+      <c r="X8" s="763"/>
+      <c r="Y8" s="763"/>
+      <c r="Z8" s="763"/>
+      <c r="AA8" s="763"/>
+      <c r="AB8" s="763"/>
+      <c r="AC8" s="764"/>
+      <c r="AD8" s="760"/>
     </row>
     <row r="9" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="745"/>
-      <c r="G9" s="780"/>
+      <c r="C9" s="784"/>
+      <c r="G9" s="748"/>
       <c r="H9" s="6"/>
-      <c r="K9" s="759"/>
-      <c r="L9" s="783" t="s">
+      <c r="K9" s="766"/>
+      <c r="L9" s="751" t="s">
         <v>216</v>
       </c>
-      <c r="M9" s="784"/>
-      <c r="N9" s="785"/>
-      <c r="O9" s="790"/>
+      <c r="M9" s="752"/>
+      <c r="N9" s="753"/>
+      <c r="O9" s="758"/>
       <c r="P9" s="75"/>
-      <c r="AD9" s="753"/>
+      <c r="AD9" s="760"/>
     </row>
     <row r="10" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="746"/>
+      <c r="C10" s="785"/>
       <c r="D10" s="23"/>
       <c r="E10" s="45" t="s">
         <v>87</v>
@@ -14197,7 +14197,7 @@
       <c r="F10" s="66" t="s">
         <v>88</v>
       </c>
-      <c r="G10" s="780"/>
+      <c r="G10" s="748"/>
       <c r="H10" s="51"/>
       <c r="I10" s="21" t="s">
         <v>80</v>
@@ -14205,33 +14205,33 @@
       <c r="J10" s="3">
         <v>15</v>
       </c>
-      <c r="K10" s="759"/>
-      <c r="M10" s="748" t="s">
+      <c r="K10" s="766"/>
+      <c r="M10" s="787" t="s">
         <v>89</v>
       </c>
-      <c r="N10" s="749"/>
-      <c r="O10" s="749"/>
-      <c r="P10" s="749"/>
-      <c r="Q10" s="749"/>
-      <c r="R10" s="749"/>
-      <c r="S10" s="749"/>
-      <c r="T10" s="749"/>
-      <c r="U10" s="749"/>
-      <c r="V10" s="749"/>
-      <c r="W10" s="749"/>
-      <c r="X10" s="749"/>
-      <c r="Y10" s="749"/>
-      <c r="Z10" s="749"/>
-      <c r="AA10" s="749"/>
-      <c r="AB10" s="749"/>
-      <c r="AC10" s="750"/>
-      <c r="AD10" s="753"/>
+      <c r="N10" s="788"/>
+      <c r="O10" s="788"/>
+      <c r="P10" s="788"/>
+      <c r="Q10" s="788"/>
+      <c r="R10" s="788"/>
+      <c r="S10" s="788"/>
+      <c r="T10" s="788"/>
+      <c r="U10" s="788"/>
+      <c r="V10" s="788"/>
+      <c r="W10" s="788"/>
+      <c r="X10" s="788"/>
+      <c r="Y10" s="788"/>
+      <c r="Z10" s="788"/>
+      <c r="AA10" s="788"/>
+      <c r="AB10" s="788"/>
+      <c r="AC10" s="789"/>
+      <c r="AD10" s="760"/>
     </row>
     <row r="11" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="747"/>
-      <c r="G11" s="780"/>
+      <c r="C11" s="786"/>
+      <c r="G11" s="748"/>
       <c r="H11" s="6"/>
-      <c r="K11" s="759"/>
+      <c r="K11" s="766"/>
       <c r="R11" s="52" t="s">
         <v>44</v>
       </c>
@@ -14239,17 +14239,17 @@
       <c r="Y11" s="68" t="s">
         <v>120</v>
       </c>
-      <c r="Z11" s="769" t="s">
+      <c r="Z11" s="776" t="s">
         <v>120</v>
       </c>
-      <c r="AA11" s="770"/>
+      <c r="AA11" s="777"/>
       <c r="AB11" s="52" t="s">
         <v>44</v>
       </c>
       <c r="AC11" s="118" t="s">
         <v>120</v>
       </c>
-      <c r="AD11" s="753"/>
+      <c r="AD11" s="760"/>
     </row>
     <row r="12" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C12" s="129"/>
@@ -14262,7 +14262,7 @@
       <c r="F12" s="66" t="s">
         <v>91</v>
       </c>
-      <c r="G12" s="780"/>
+      <c r="G12" s="748"/>
       <c r="H12" s="128"/>
       <c r="I12" s="19" t="s">
         <v>80</v>
@@ -14270,8 +14270,8 @@
       <c r="J12" s="3">
         <v>15</v>
       </c>
-      <c r="K12" s="759"/>
-      <c r="L12" s="774" t="s">
+      <c r="K12" s="766"/>
+      <c r="L12" s="781" t="s">
         <v>92</v>
       </c>
       <c r="M12" s="21" t="s">
@@ -14302,25 +14302,25 @@
         <v>115</v>
       </c>
       <c r="Y12" s="6"/>
-      <c r="AA12" s="763" t="s">
+      <c r="AA12" s="770" t="s">
         <v>125</v>
       </c>
-      <c r="AB12" s="764"/>
+      <c r="AB12" s="771"/>
       <c r="AC12" s="21" t="s">
         <v>230</v>
       </c>
-      <c r="AD12" s="753"/>
+      <c r="AD12" s="760"/>
     </row>
     <row r="13" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="745"/>
-      <c r="G13" s="780"/>
-      <c r="K13" s="759"/>
-      <c r="L13" s="775"/>
+      <c r="C13" s="784"/>
+      <c r="G13" s="748"/>
+      <c r="K13" s="766"/>
+      <c r="L13" s="782"/>
       <c r="M13" s="47"/>
-      <c r="Q13" s="782" t="s">
+      <c r="Q13" s="750" t="s">
         <v>208</v>
       </c>
-      <c r="R13" s="644"/>
+      <c r="R13" s="639"/>
       <c r="S13" s="599"/>
       <c r="T13" s="6"/>
       <c r="U13" s="96" t="s">
@@ -14329,17 +14329,17 @@
       <c r="X13" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="AA13" s="765"/>
-      <c r="AB13" s="766"/>
-      <c r="AD13" s="753"/>
+      <c r="AA13" s="772"/>
+      <c r="AB13" s="773"/>
+      <c r="AD13" s="760"/>
     </row>
     <row r="14" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
         <v>332</v>
       </c>
-      <c r="C14" s="747"/>
+      <c r="C14" s="786"/>
       <c r="D14" s="23"/>
-      <c r="G14" s="780"/>
+      <c r="G14" s="748"/>
       <c r="H14" s="125"/>
       <c r="I14" s="99" t="s">
         <v>44</v>
@@ -14347,8 +14347,8 @@
       <c r="J14" s="111">
         <v>115</v>
       </c>
-      <c r="K14" s="759"/>
-      <c r="L14" s="775"/>
+      <c r="K14" s="766"/>
+      <c r="L14" s="782"/>
       <c r="M14" s="21" t="s">
         <v>110</v>
       </c>
@@ -14369,9 +14369,9 @@
       <c r="Y14" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="AA14" s="765"/>
-      <c r="AB14" s="766"/>
-      <c r="AD14" s="753"/>
+      <c r="AA14" s="772"/>
+      <c r="AB14" s="773"/>
+      <c r="AD14" s="760"/>
     </row>
     <row r="15" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C15" s="130" t="s">
@@ -14386,19 +14386,19 @@
       <c r="F15" s="66" t="s">
         <v>93</v>
       </c>
-      <c r="G15" s="780"/>
+      <c r="G15" s="748"/>
       <c r="H15" s="2" t="s">
         <v>80</v>
       </c>
       <c r="I15" s="53" t="s">
         <v>80</v>
       </c>
-      <c r="K15" s="759"/>
-      <c r="L15" s="776"/>
-      <c r="Q15" s="782" t="s">
+      <c r="K15" s="766"/>
+      <c r="L15" s="783"/>
+      <c r="Q15" s="750" t="s">
         <v>209</v>
       </c>
-      <c r="R15" s="644"/>
+      <c r="R15" s="639"/>
       <c r="S15" s="599"/>
       <c r="T15" s="6"/>
       <c r="V15" s="68" t="s">
@@ -14407,14 +14407,14 @@
       <c r="X15" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="AA15" s="765"/>
-      <c r="AB15" s="766"/>
-      <c r="AD15" s="753"/>
+      <c r="AA15" s="772"/>
+      <c r="AB15" s="773"/>
+      <c r="AD15" s="760"/>
     </row>
     <row r="16" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C16" s="132"/>
-      <c r="G16" s="780"/>
-      <c r="K16" s="759"/>
+      <c r="G16" s="748"/>
+      <c r="K16" s="766"/>
       <c r="N16" s="47"/>
       <c r="O16" s="61" t="s">
         <v>108</v>
@@ -14433,24 +14433,24 @@
       <c r="Z16" s="76" t="s">
         <v>126</v>
       </c>
-      <c r="AA16" s="765"/>
-      <c r="AB16" s="766"/>
-      <c r="AD16" s="753"/>
+      <c r="AA16" s="772"/>
+      <c r="AB16" s="773"/>
+      <c r="AD16" s="760"/>
     </row>
     <row r="17" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C17" s="109"/>
       <c r="E17" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="F17" s="777" t="s">
+      <c r="F17" s="745" t="s">
         <v>95</v>
       </c>
-      <c r="G17" s="780"/>
+      <c r="G17" s="748"/>
       <c r="H17" s="54"/>
       <c r="I17" s="133" t="s">
         <v>80</v>
       </c>
-      <c r="K17" s="759"/>
+      <c r="K17" s="766"/>
       <c r="S17" s="599"/>
       <c r="V17" s="68" t="s">
         <v>44</v>
@@ -14458,9 +14458,9 @@
       <c r="X17" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="AA17" s="765"/>
-      <c r="AB17" s="766"/>
-      <c r="AD17" s="753"/>
+      <c r="AA17" s="772"/>
+      <c r="AB17" s="773"/>
+      <c r="AD17" s="760"/>
     </row>
     <row r="18" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C18" s="130"/>
@@ -14470,15 +14470,15 @@
       <c r="E18" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="F18" s="778"/>
-      <c r="G18" s="780"/>
+      <c r="F18" s="746"/>
+      <c r="G18" s="748"/>
       <c r="H18" s="108" t="s">
         <v>75</v>
       </c>
       <c r="I18" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="K18" s="759"/>
+      <c r="K18" s="766"/>
       <c r="O18" s="64" t="s">
         <v>114</v>
       </c>
@@ -14489,42 +14489,39 @@
       <c r="X18" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="AA18" s="767"/>
-      <c r="AB18" s="768"/>
-      <c r="AD18" s="753"/>
+      <c r="AA18" s="774"/>
+      <c r="AB18" s="775"/>
+      <c r="AD18" s="760"/>
     </row>
     <row r="19" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F19" s="64" t="s">
         <v>207</v>
       </c>
-      <c r="G19" s="781"/>
-      <c r="K19" s="760"/>
+      <c r="G19" s="749"/>
+      <c r="K19" s="767"/>
       <c r="Q19" s="68" t="s">
         <v>44</v>
       </c>
-      <c r="R19" s="786" t="s">
+      <c r="R19" s="754" t="s">
         <v>123</v>
       </c>
-      <c r="S19" s="787"/>
-      <c r="T19" s="788"/>
+      <c r="S19" s="755"/>
+      <c r="T19" s="756"/>
       <c r="V19" s="77" t="s">
         <v>114</v>
       </c>
       <c r="Y19" s="19" t="s">
         <v>124</v>
       </c>
-      <c r="AD19" s="754"/>
+      <c r="AD19" s="761"/>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="G2:G19"/>
-    <mergeCell ref="Q13:R13"/>
-    <mergeCell ref="Q15:R15"/>
-    <mergeCell ref="L9:N9"/>
-    <mergeCell ref="R19:T19"/>
-    <mergeCell ref="S12:S18"/>
-    <mergeCell ref="O3:O9"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="V2:W2"/>
+    <mergeCell ref="M10:AC10"/>
+    <mergeCell ref="F2:F3"/>
     <mergeCell ref="AD1:AD19"/>
     <mergeCell ref="S8:AC8"/>
     <mergeCell ref="K5:K19"/>
@@ -14536,11 +14533,14 @@
     <mergeCell ref="P3:Q3"/>
     <mergeCell ref="L4:L8"/>
     <mergeCell ref="L12:L15"/>
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="V2:W2"/>
-    <mergeCell ref="M10:AC10"/>
-    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="G2:G19"/>
+    <mergeCell ref="Q13:R13"/>
+    <mergeCell ref="Q15:R15"/>
+    <mergeCell ref="L9:N9"/>
+    <mergeCell ref="R19:T19"/>
+    <mergeCell ref="S12:S18"/>
+    <mergeCell ref="O3:O9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>